<commit_message>
Creating successfully RestFul WS CRUD
</commit_message>
<xml_diff>
--- a/Training_Plan.xlsx
+++ b/Training_Plan.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="45" windowWidth="19155" windowHeight="11760" activeTab="4"/>
@@ -6755,7 +6755,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="26">
     <font>
       <sz val="11"/>
@@ -7199,6 +7199,29 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -7220,31 +7243,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -7433,7 +7433,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -7468,7 +7467,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -7644,7 +7642,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:J30"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
@@ -8110,7 +8108,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:E145"/>
   <sheetViews>
     <sheetView topLeftCell="A130" workbookViewId="0">
@@ -8365,10 +8363,10 @@
     <row r="27" spans="2:5">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
-      <c r="D27" s="44" t="s">
+      <c r="D27" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="E27" s="45"/>
+      <c r="E27" s="54"/>
     </row>
     <row r="28" spans="2:5">
       <c r="B28" s="2"/>
@@ -8431,10 +8429,10 @@
     <row r="34" spans="2:5">
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
-      <c r="D34" s="48" t="s">
+      <c r="D34" s="57" t="s">
         <v>81</v>
       </c>
-      <c r="E34" s="48"/>
+      <c r="E34" s="57"/>
     </row>
     <row r="35" spans="2:5">
       <c r="B35" s="2"/>
@@ -8507,10 +8505,10 @@
     <row r="42" spans="2:5">
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
-      <c r="D42" s="49" t="s">
+      <c r="D42" s="58" t="s">
         <v>94</v>
       </c>
-      <c r="E42" s="50"/>
+      <c r="E42" s="59"/>
     </row>
     <row r="43" spans="2:5">
       <c r="B43" s="2"/>
@@ -8597,10 +8595,10 @@
     <row r="51" spans="2:5">
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
-      <c r="D51" s="46" t="s">
+      <c r="D51" s="55" t="s">
         <v>60</v>
       </c>
-      <c r="E51" s="46"/>
+      <c r="E51" s="55"/>
     </row>
     <row r="52" spans="2:5">
       <c r="B52" s="2"/>
@@ -8658,7 +8656,7 @@
       <c r="D57" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="E57" s="47" t="s">
+      <c r="E57" s="56" t="s">
         <v>73</v>
       </c>
     </row>
@@ -8668,7 +8666,7 @@
       <c r="D58" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="E58" s="47"/>
+      <c r="E58" s="56"/>
     </row>
     <row r="59" spans="2:5">
       <c r="B59" s="2"/>
@@ -9395,11 +9393,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B3:C13"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9491,7 +9489,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B3:C43"/>
   <sheetViews>
     <sheetView topLeftCell="A20" workbookViewId="0">
@@ -9711,11 +9709,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:C48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9749,7 +9747,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="300">
+    <row r="5" spans="2:3" ht="285">
       <c r="B5" s="4" t="s">
         <v>269</v>
       </c>
@@ -9900,154 +9898,154 @@
       </c>
     </row>
     <row r="24" spans="2:3" ht="26.25">
-      <c r="B24" s="51" t="s">
+      <c r="B24" s="44" t="s">
         <v>306</v>
       </c>
       <c r="C24" s="37"/>
     </row>
     <row r="25" spans="2:3" ht="33" customHeight="1">
-      <c r="B25" s="52" t="s">
+      <c r="B25" s="60" t="s">
         <v>307</v>
       </c>
-      <c r="C25" s="52"/>
+      <c r="C25" s="60"/>
     </row>
     <row r="26" spans="2:3">
-      <c r="B26" s="52" t="s">
+      <c r="B26" s="60" t="s">
         <v>308</v>
       </c>
-      <c r="C26" s="52"/>
+      <c r="C26" s="60"/>
     </row>
     <row r="27" spans="2:3" ht="15.75" thickBot="1">
-      <c r="B27" s="56" t="s">
+      <c r="B27" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="57"/>
+      <c r="C27" s="49"/>
     </row>
     <row r="28" spans="2:3" ht="15.75" thickBot="1">
-      <c r="B28" s="55" t="s">
+      <c r="B28" s="47" t="s">
         <v>309</v>
       </c>
       <c r="C28" s="2"/>
     </row>
     <row r="29" spans="2:3" ht="15.75" thickBot="1">
-      <c r="B29" s="54" t="s">
+      <c r="B29" s="46" t="s">
         <v>310</v>
       </c>
       <c r="C29" s="2"/>
     </row>
     <row r="30" spans="2:3" ht="15.75" thickBot="1">
-      <c r="B30" s="55" t="s">
+      <c r="B30" s="47" t="s">
         <v>311</v>
       </c>
       <c r="C30" s="2"/>
     </row>
     <row r="31" spans="2:3" ht="15.75" thickBot="1">
-      <c r="B31" s="53"/>
+      <c r="B31" s="45"/>
       <c r="C31" s="2"/>
     </row>
     <row r="32" spans="2:3" ht="15.75" thickBot="1">
-      <c r="B32" s="55" t="s">
+      <c r="B32" s="47" t="s">
         <v>312</v>
       </c>
       <c r="C32" s="2"/>
     </row>
     <row r="33" spans="2:3" ht="15.75" thickBot="1">
-      <c r="B33" s="54" t="s">
+      <c r="B33" s="46" t="s">
         <v>313</v>
       </c>
       <c r="C33" s="2"/>
     </row>
     <row r="34" spans="2:3" ht="15.75" thickBot="1">
-      <c r="B34" s="54" t="s">
+      <c r="B34" s="46" t="s">
         <v>314</v>
       </c>
       <c r="C34" s="2"/>
     </row>
     <row r="35" spans="2:3">
-      <c r="B35" s="58" t="s">
+      <c r="B35" s="50" t="s">
         <v>315</v>
       </c>
-      <c r="C35" s="59"/>
+      <c r="C35" s="51"/>
     </row>
     <row r="36" spans="2:3" ht="50.25" customHeight="1">
-      <c r="B36" s="52" t="s">
+      <c r="B36" s="60" t="s">
         <v>316</v>
       </c>
-      <c r="C36" s="52"/>
+      <c r="C36" s="60"/>
     </row>
     <row r="37" spans="2:3" ht="32.25" customHeight="1">
-      <c r="B37" s="52" t="s">
+      <c r="B37" s="60" t="s">
         <v>317</v>
       </c>
-      <c r="C37" s="52"/>
+      <c r="C37" s="60"/>
     </row>
     <row r="38" spans="2:3" ht="15.75" thickBot="1">
-      <c r="B38" s="60" t="s">
+      <c r="B38" s="52" t="s">
         <v>318</v>
       </c>
-      <c r="C38" s="57"/>
+      <c r="C38" s="49"/>
     </row>
     <row r="39" spans="2:3" ht="15.75" thickBot="1">
-      <c r="B39" s="54" t="s">
+      <c r="B39" s="46" t="s">
         <v>319</v>
       </c>
       <c r="C39" s="2"/>
     </row>
     <row r="40" spans="2:3" ht="15.75" thickBot="1">
-      <c r="B40" s="54" t="s">
+      <c r="B40" s="46" t="s">
         <v>320</v>
       </c>
     </row>
     <row r="41" spans="2:3" ht="15.75" thickBot="1">
-      <c r="B41" s="54" t="s">
+      <c r="B41" s="46" t="s">
         <v>321</v>
       </c>
     </row>
     <row r="42" spans="2:3" ht="15.75" thickBot="1">
-      <c r="B42" s="54" t="s">
+      <c r="B42" s="46" t="s">
         <v>322</v>
       </c>
     </row>
     <row r="43" spans="2:3" ht="15.75" thickBot="1">
-      <c r="B43" s="54" t="s">
+      <c r="B43" s="46" t="s">
         <v>323</v>
       </c>
     </row>
     <row r="44" spans="2:3" ht="15.75" thickBot="1">
-      <c r="B44" s="54" t="s">
+      <c r="B44" s="46" t="s">
         <v>324</v>
       </c>
     </row>
     <row r="45" spans="2:3" ht="15.75" thickBot="1">
-      <c r="B45" s="54" t="s">
+      <c r="B45" s="46" t="s">
         <v>325</v>
       </c>
     </row>
     <row r="46" spans="2:3">
-      <c r="B46" s="58" t="s">
+      <c r="B46" s="50" t="s">
         <v>326</v>
       </c>
     </row>
     <row r="47" spans="2:3" ht="36" customHeight="1">
-      <c r="B47" s="52" t="s">
+      <c r="B47" s="60" t="s">
         <v>327</v>
       </c>
-      <c r="C47" s="52"/>
+      <c r="C47" s="60"/>
     </row>
     <row r="48" spans="2:3" ht="49.5" customHeight="1">
-      <c r="B48" s="52" t="s">
+      <c r="B48" s="60" t="s">
         <v>328</v>
       </c>
-      <c r="C48" s="52"/>
+      <c r="C48" s="60"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="B48:C48"/>
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="B36:C36"/>
     <mergeCell ref="B37:C37"/>
     <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Adding Wrapper class *DTOList in order for Json to convert a list.
</commit_message>
<xml_diff>
--- a/Training_Plan.xlsx
+++ b/Training_Plan.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="362">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="405">
   <si>
     <t>Java core</t>
   </si>
@@ -6752,18 +6752,6 @@
     <t>Whatever beans are available in the ApplicationContext can be referred to from each WebApplicationContext. It is a best practice to keep a clear separation between middle-tier services such as business logic components and data access classes  (that are typically defined in the ApplicationContext) and web- related components such as controllers and view resolvers  (that are defined in the WebApplicationContext per Dispatcher Servlet).</t>
   </si>
   <si>
-    <t>@RequestMapping annotation is used to map the request URI to the handler method. We can also specify the HTTP method that should be used by client application to invoke the rest method.</t>
-  </si>
-  <si>
-    <t>@ResponseBody annotation is used to map the response object in the response body. Once the response object is returned by the handler method, MappingJackson2HttpMessageConverter kicks in and convert it to JSON response.</t>
-  </si>
-  <si>
-    <t>@PathVariable annotation is the easy way to extract the data from the rest URI and map it to the method argument.</t>
-  </si>
-  <si>
-    <t>@RequestBody annotation is used to map the request body JSON data into the Employee object, again this is done by the MappingJackson2HttpMessageConverter mapping.</t>
-  </si>
-  <si>
     <t>What are differences between GET and POST method?</t>
   </si>
   <si>
@@ -6849,13 +6837,682 @@
   </si>
   <si>
     <t>Data is not displayed in the URL</t>
+  </si>
+  <si>
+    <t>Content Negotiation using Spring MVC</t>
+  </si>
+  <si>
+    <t>There are two ways to generate output using Spring MVC:</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">You can use the RESTful </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>@ResponseBody</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> approach and HTTP message converters, typically to return data-formats like JSON or XML. Programmatic clients, mobile apps and AJAX enabled browsers are the usual clients.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Alternatively you may use </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>view resolution</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Although views are perfectly capable of generating JSON and XML if you wish (more on that in my next post), views are normally used to generate presentation formats like HTML for a traditional web-application.</t>
+    </r>
+  </si>
+  <si>
+    <t>Actually there is a third possibility - some applications require both, and Spring MVC supports such combinations easily. We will come back to that right at the end.</t>
+  </si>
+  <si>
+    <t>There are three situations where we need to know what type of data-format to send in the HTTP response:</t>
+  </si>
+  <si>
+    <r>
+      <t>HttpMessageConverters:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Determine the right converter to use.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Request Mappings:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Map an incoming HTTP request to different methods that return different formats.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>View Resolution:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Pick the right view to use.</t>
+    </r>
+  </si>
+  <si>
+    <t>Enabling Content Negotiation in Spring MVC??</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Spring supports a couple of conventions for selecting the format required: URL suffixes and/or a URL parameter. These work alongside the use of Accept headers. As a result, the content-type can be requested in any of three ways. By default they are checked in this </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>order:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+    + Add a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>path extension (suffix) in the URL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. So, if the incoming URL is something like http://myserver/myapp/accounts/list</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.html</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> then HTML is required. For a spreadsheet the URL should be http://myserver/myapp/accounts/list.xls. The suffix to media-type mapping is automatically defined via the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>JavaBeans Activation Framework</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> or JAF (so activation.jar must be on the class path).
+    + </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">A URL parameter </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>like this: http://myserver/myapp/accounts/list?</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>format=xls</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. The name of the parameter is format by default, but this may be changed. Using a parameter is disabled by default, but when enabled, it is checked second.
+    + Finally the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Accept HTTP header property is checked</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. This is how HTTP is actually defined to work, but, as previously mentioned, it can be problematic to use.
+</t>
+    </r>
+  </si>
+  <si>
+    <t>@Controller</t>
+  </si>
+  <si>
+    <t>Use the @Controller annotation to annotate the class that will be the controller in MVC and handle the HTTP request.</t>
+  </si>
+  <si>
+    <t>@RequestMapping</t>
+  </si>
+  <si>
+    <t>@PathVariable</t>
+  </si>
+  <si>
+    <t>A path variable in the URI could be injected as a parameter using the @PathVariable annotation.
+For example:
+@RequestMapping(method=RequestMethod.GET, value="/emp/{id}")
+public ModelAndView getEmployee(@PathVariable String id) { … }</t>
+  </si>
+  <si>
+    <t>is used to map the response object in the response body. Once the response object is returned by the handler method, MappingJackson2HttpMessageConverter kicks in and convert it to JSON response.</t>
+  </si>
+  <si>
+    <t>@ResponseBody</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@RequestBody </t>
+  </si>
+  <si>
+    <t>Is used to map the request body JSON data into the Employee object, again this is done by the MappingJackson2HttpMessageConverter mapping.</t>
+  </si>
+  <si>
+    <r>
+      <t>Use the @RequestMapping annotation to annotate the function that should handle certain HTTP methods, URIs, or HTTP headers. This annotation is the key to the Spring REST support. You change the method parameter to handle other HTTP methods.
+For example:
+@RequestMapping(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>method</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>=RequestMethod.GET,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> value</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">="/emps", 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>headers</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">="Accept=application/xml, application/json",  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>produces</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = MediaType.APPLICATION_XML_VALUE,  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>consumes</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = MediaType.APPLICATION_XML_VALUE)</t>
+    </r>
+  </si>
+  <si>
+    <t>Multiple representation support</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Representing the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">same resource </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">with </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>different MIME types</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is an important aspect of RESTful web services. Generally, you would use the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>same URI</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> with a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">different "accept" HTTP header </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">to fetch the resource with different representation. You can also use a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">different URI, or a URI with different request parameters.
+ + </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">ContentNegotiatingViewResolver </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>can pick a different view resolver to handle the same URI (with the difference of the accept header)
+ + There's also another way to produce multiple representations—by combining the HttpMessageConverter and c@ResponseBody annotation. With this method you don't need to use the View technologies.</t>
+    </r>
+  </si>
+  <si>
+    <t>HttpMessageConverter</t>
+  </si>
+  <si>
+    <t>How can Spring serialize/de-serialize the objects to raw texts? This is handled by HttpMessageConverter</t>
+  </si>
+  <si>
+    <t>With...</t>
+  </si>
+  <si>
+    <t>You can...</t>
+  </si>
+  <si>
+    <t>StringHttpMessageConverter</t>
+  </si>
+  <si>
+    <t>Read/write a string from request and response. By default, it supports the media type text/* and writes with a Content-Type of text/plain.</t>
+  </si>
+  <si>
+    <t>FormHttpMessageConverter</t>
+  </si>
+  <si>
+    <t>Read/write form data from request and response. By default, it reads the media type application/x-www-form-urlencoded and writes data into MultiValueMap&lt;String,String&gt;.</t>
+  </si>
+  <si>
+    <t>MarshallingHttpMessageConverter</t>
+  </si>
+  <si>
+    <t>Read/write XML data using Spring's marshaller/un-marshaller. It converts data of media type application/xml.</t>
+  </si>
+  <si>
+    <t>MappingJacksonHttpMessageConverter</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Read/write JSON data using Jackson's </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>ObjectMapper</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. It converts data of media type application/json.</t>
+    </r>
+  </si>
+  <si>
+    <t>AtomFeedHttpMessageConverter</t>
+  </si>
+  <si>
+    <t>Read/write ATOM feed using ROME's Feed API. It converts data of media type application/atom+xml.</t>
+  </si>
+  <si>
+    <t>RssChannelHttpMessageConverter</t>
+  </si>
+  <si>
+    <t>Read/write RSS feed using ROME's feed API. It converts data of media type application/rss+xml.</t>
+  </si>
+  <si>
+    <t>First, you must configure the HttpMessageConverter. To produce multiple representations, customize several HttpMessageConverter instances to convert the object to different media types.</t>
+  </si>
+  <si>
+    <t>Listing 1. Configure HttpMessageConverter in rest-servlet.xml
+&lt;bean class="org.springframework.web.servlet.mvc.annotation
+.AnnotationMethodHandlerAdapter"&gt;
+   &lt;property name="messageConverters"&gt;
+       &lt;list&gt;
+           &lt;ref bean="jsonConverter" /&gt;
+   &lt;ref bean="marshallingConverter" /&gt;
+   &lt;ref bean="atomConverter" /&gt;
+       &lt;/list&gt;
+   &lt;/property&gt;
+&lt;/bean&gt;
+&lt;bean id="jsonConverter" 
+            class="org.springframework.http.converter.json
+.MappingJacksonHttpMessageConverter"&gt;
+   &lt;property name="supportedMediaTypes" value="application/json" /&gt;
+&lt;/bean&gt;</t>
+  </si>
+  <si>
+    <t>The next step is to write a method to handle the request that asks for JSON representation. Listing 2 shows the details.</t>
+  </si>
+  <si>
+    <t>Listing 2. Handle JSON requests defined in EmployeeController
+@RequestMapping(method=RequestMethod.GET, value="/emp/{id}", 
+  headers="Accept=application/json")
+public @ResponseBody Employee getEmp(@PathVariable String id) {
+Employee e = employeeDS.get(Long.parseLong(id));
+return e;
+}
+@RequestMapping(method=RequestMethod.GET, value="/emps", 
+  headers="Accept=application/json")
+public @ResponseBody EmployeeListinggetAllEmp() {
+List&lt;Employee&gt; employees = employeeDS.getAll();
+EmployeeListinglist = new EmployeeList(employees);
+return list;
+}</t>
+  </si>
+  <si>
+    <t>Implement POST, PUT, and DELETE</t>
+  </si>
+  <si>
+    <t>@RequestMapping(method=RequestMethod.POST, value="/emp")
+public @ResponseBody Employee addEmp(@RequestBody Employee e) {
+employeeDS.add(e);
+return e;
+}
+@RequestMapping(method=RequestMethod.PUT, value="/emp/{id}")
+public @ResponseBody Employee updateEmp(
+ @RequestBody Employee e, @PathVariable String id) {
+employeeDS.update(e);
+return e;
+}
+@RequestMapping(method=RequestMethod.DELETE, value="/emp/{id}")
+public @ResponseBody void removeEmp(@PathVariable String id) {
+employeeDS.remove(Long.parseLong(id));
+}</t>
+  </si>
+  <si>
+    <t>STEPS</t>
+  </si>
+  <si>
+    <t>Details</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="26">
+  <fonts count="29">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -7045,6 +7702,25 @@
       <color rgb="FF333333"/>
       <name val="Open Sans"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -7207,7 +7883,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -7324,6 +8000,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -7348,14 +8030,44 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -7757,7 +8469,7 @@
   <dimension ref="B2:J30"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8474,10 +9186,10 @@
     <row r="27" spans="2:5">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
-      <c r="D27" s="54" t="s">
+      <c r="D27" s="56" t="s">
         <v>47</v>
       </c>
-      <c r="E27" s="55"/>
+      <c r="E27" s="57"/>
     </row>
     <row r="28" spans="2:5">
       <c r="B28" s="2"/>
@@ -8540,10 +9252,10 @@
     <row r="34" spans="2:5">
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
-      <c r="D34" s="58" t="s">
+      <c r="D34" s="60" t="s">
         <v>81</v>
       </c>
-      <c r="E34" s="58"/>
+      <c r="E34" s="60"/>
     </row>
     <row r="35" spans="2:5">
       <c r="B35" s="2"/>
@@ -8616,10 +9328,10 @@
     <row r="42" spans="2:5">
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
-      <c r="D42" s="59" t="s">
+      <c r="D42" s="61" t="s">
         <v>94</v>
       </c>
-      <c r="E42" s="60"/>
+      <c r="E42" s="62"/>
     </row>
     <row r="43" spans="2:5">
       <c r="B43" s="2"/>
@@ -8706,10 +9418,10 @@
     <row r="51" spans="2:5">
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
-      <c r="D51" s="56" t="s">
+      <c r="D51" s="58" t="s">
         <v>60</v>
       </c>
-      <c r="E51" s="56"/>
+      <c r="E51" s="58"/>
     </row>
     <row r="52" spans="2:5">
       <c r="B52" s="2"/>
@@ -8767,7 +9479,7 @@
       <c r="D57" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="E57" s="57" t="s">
+      <c r="E57" s="59" t="s">
         <v>73</v>
       </c>
     </row>
@@ -8777,7 +9489,7 @@
       <c r="D58" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="E58" s="57"/>
+      <c r="E58" s="59"/>
     </row>
     <row r="59" spans="2:5">
       <c r="B59" s="2"/>
@@ -9601,10 +10313,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A3:C59"/>
+  <dimension ref="A3:C86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="B86" sqref="B86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9792,182 +10504,379 @@
       </c>
       <c r="C38" s="37"/>
     </row>
-    <row r="39" spans="1:3" ht="30">
-      <c r="B39" s="37" t="s">
+    <row r="40" spans="1:3">
+      <c r="B40" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="C40" s="2"/>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="55"/>
+      <c r="B41" s="15" t="s">
+        <v>281</v>
+      </c>
+      <c r="C41" s="15" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="30">
+      <c r="A42" s="53" t="s">
+        <v>330</v>
+      </c>
+      <c r="B42" s="53" t="s">
+        <v>331</v>
+      </c>
+      <c r="C42" s="53" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="53" t="s">
+        <v>333</v>
+      </c>
+      <c r="B43" s="53" t="s">
+        <v>334</v>
+      </c>
+      <c r="C43" s="53" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="53" t="s">
+        <v>336</v>
+      </c>
+      <c r="B44" s="53" t="s">
+        <v>337</v>
+      </c>
+      <c r="C44" s="53" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="30">
+      <c r="A45" s="53" t="s">
+        <v>339</v>
+      </c>
+      <c r="B45" s="53" t="s">
+        <v>340</v>
+      </c>
+      <c r="C45" s="53" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="53" t="s">
+        <v>342</v>
+      </c>
+      <c r="B46" s="53" t="s">
+        <v>343</v>
+      </c>
+      <c r="C46" s="53" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="30">
+      <c r="A47" s="53" t="s">
+        <v>345</v>
+      </c>
+      <c r="B47" s="53" t="s">
+        <v>346</v>
+      </c>
+      <c r="C47" s="53" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="30">
+      <c r="A48" s="53" t="s">
+        <v>348</v>
+      </c>
+      <c r="B48" s="53" t="s">
+        <v>349</v>
+      </c>
+      <c r="C48" s="53" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="59" t="s">
+        <v>351</v>
+      </c>
+      <c r="B49" s="53" t="s">
+        <v>352</v>
+      </c>
+      <c r="C49" s="59" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="59"/>
+      <c r="B50" s="53"/>
+      <c r="C50" s="59"/>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="59"/>
+      <c r="B51" s="53" t="s">
+        <v>353</v>
+      </c>
+      <c r="C51" s="59"/>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="53" t="s">
+        <v>355</v>
+      </c>
+      <c r="B52" s="53" t="s">
+        <v>356</v>
+      </c>
+      <c r="C52" s="53" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="B53" s="64"/>
+    </row>
+    <row r="54" spans="1:3" ht="31.5">
+      <c r="B54" s="22" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="B55" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="B56" s="65"/>
+    </row>
+    <row r="57" spans="1:3" ht="32.25" customHeight="1">
+      <c r="B57" s="66" t="s">
+        <v>360</v>
+      </c>
+      <c r="C57" s="66"/>
+    </row>
+    <row r="58" spans="1:3" ht="33" customHeight="1">
+      <c r="B58" s="66" t="s">
+        <v>361</v>
+      </c>
+      <c r="C58" s="66"/>
+    </row>
+    <row r="59" spans="1:3" ht="19.5" customHeight="1">
+      <c r="B59" s="66" t="s">
+        <v>362</v>
+      </c>
+      <c r="C59" s="66"/>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="B60" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="C60" s="2"/>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="B61" s="67"/>
+      <c r="C61" s="2"/>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="B62" s="68" t="s">
+        <v>364</v>
+      </c>
+      <c r="C62" s="2"/>
+    </row>
+    <row r="63" spans="1:3" ht="30">
+      <c r="B63" s="69" t="s">
+        <v>365</v>
+      </c>
+      <c r="C63" s="2"/>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="B64" s="68" t="s">
+        <v>366</v>
+      </c>
+      <c r="C64" s="2"/>
+    </row>
+    <row r="65" spans="2:3" ht="225">
+      <c r="B65" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="C65" s="54" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3" ht="30">
+      <c r="B66" s="37" t="s">
         <v>261</v>
       </c>
-      <c r="C39" s="37"/>
-    </row>
-    <row r="40" spans="1:3" ht="36.75" customHeight="1">
-      <c r="B40" s="62" t="s">
-        <v>329</v>
-      </c>
-      <c r="C40" s="63"/>
-    </row>
-    <row r="41" spans="1:3">
-      <c r="B41" s="2"/>
-      <c r="C41" s="53"/>
-    </row>
-    <row r="42" spans="1:3" ht="35.25" customHeight="1">
-      <c r="B42" s="62" t="s">
-        <v>330</v>
-      </c>
-      <c r="C42" s="63"/>
-    </row>
-    <row r="43" spans="1:3">
-      <c r="B43" s="2"/>
-      <c r="C43" s="53"/>
-    </row>
-    <row r="44" spans="1:3" ht="19.5" customHeight="1">
-      <c r="B44" s="62" t="s">
-        <v>331</v>
-      </c>
-      <c r="C44" s="63"/>
-    </row>
-    <row r="45" spans="1:3">
-      <c r="B45" s="2"/>
-      <c r="C45" s="2"/>
-    </row>
-    <row r="46" spans="1:3" ht="20.25" customHeight="1">
-      <c r="B46" s="62" t="s">
-        <v>332</v>
-      </c>
-      <c r="C46" s="63"/>
-    </row>
-    <row r="47" spans="1:3">
-      <c r="B47" s="2" t="s">
-        <v>333</v>
-      </c>
-      <c r="C47" s="2"/>
-    </row>
-    <row r="48" spans="1:3">
-      <c r="A48" s="64"/>
-      <c r="B48" s="15" t="s">
-        <v>281</v>
-      </c>
-      <c r="C48" s="15" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" ht="45">
-      <c r="A49" s="53" t="s">
-        <v>334</v>
-      </c>
-      <c r="B49" s="53" t="s">
-        <v>335</v>
-      </c>
-      <c r="C49" s="53" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" ht="30">
-      <c r="A50" s="53" t="s">
-        <v>337</v>
-      </c>
-      <c r="B50" s="53" t="s">
-        <v>338</v>
-      </c>
-      <c r="C50" s="53" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3">
-      <c r="A51" s="53" t="s">
-        <v>340</v>
-      </c>
-      <c r="B51" s="53" t="s">
-        <v>341</v>
-      </c>
-      <c r="C51" s="53" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" ht="30">
-      <c r="A52" s="53" t="s">
-        <v>343</v>
-      </c>
-      <c r="B52" s="53" t="s">
-        <v>344</v>
-      </c>
-      <c r="C52" s="53" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3">
-      <c r="A53" s="53" t="s">
-        <v>346</v>
-      </c>
-      <c r="B53" s="53" t="s">
-        <v>347</v>
-      </c>
-      <c r="C53" s="53" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" ht="60">
-      <c r="A54" s="53" t="s">
-        <v>349</v>
-      </c>
-      <c r="B54" s="53" t="s">
-        <v>350</v>
-      </c>
-      <c r="C54" s="53" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" ht="60">
-      <c r="A55" s="53" t="s">
-        <v>352</v>
-      </c>
-      <c r="B55" s="53" t="s">
-        <v>353</v>
-      </c>
-      <c r="C55" s="53" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3">
-      <c r="A56" s="57" t="s">
-        <v>355</v>
-      </c>
-      <c r="B56" s="53" t="s">
-        <v>356</v>
-      </c>
-      <c r="C56" s="57" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3">
-      <c r="A57" s="57"/>
-      <c r="B57" s="53"/>
-      <c r="C57" s="57"/>
-    </row>
-    <row r="58" spans="1:3">
-      <c r="A58" s="57"/>
-      <c r="B58" s="53" t="s">
-        <v>357</v>
-      </c>
-      <c r="C58" s="57"/>
-    </row>
-    <row r="59" spans="1:3">
-      <c r="A59" s="53" t="s">
-        <v>359</v>
-      </c>
-      <c r="B59" s="53" t="s">
-        <v>360</v>
-      </c>
-      <c r="C59" s="53" t="s">
-        <v>361</v>
+      <c r="C66" s="37"/>
+    </row>
+    <row r="67" spans="2:3" ht="30.75">
+      <c r="B67" s="71" t="s">
+        <v>369</v>
+      </c>
+      <c r="C67" s="54" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="68" spans="2:3" ht="137.25" customHeight="1">
+      <c r="B68" s="72" t="s">
+        <v>371</v>
+      </c>
+      <c r="C68" s="16" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="69" spans="2:3" ht="105.75">
+      <c r="B69" s="71" t="s">
+        <v>372</v>
+      </c>
+      <c r="C69" s="54" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="70" spans="2:3" ht="53.25" customHeight="1">
+      <c r="B70" s="73" t="s">
+        <v>375</v>
+      </c>
+      <c r="C70" s="70" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="71" spans="2:3" ht="32.25" customHeight="1">
+      <c r="B71" s="71" t="s">
+        <v>376</v>
+      </c>
+      <c r="C71" s="70" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="72" spans="2:3" ht="135">
+      <c r="B72" s="71" t="s">
+        <v>379</v>
+      </c>
+      <c r="C72" s="74" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="73" spans="2:3" ht="30.75">
+      <c r="B73" s="71" t="s">
+        <v>381</v>
+      </c>
+      <c r="C73" s="54" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="74" spans="2:3">
+      <c r="B74" s="75" t="s">
+        <v>383</v>
+      </c>
+      <c r="C74" s="75" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="75" spans="2:3" ht="30">
+      <c r="B75" s="75" t="s">
+        <v>385</v>
+      </c>
+      <c r="C75" s="54" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="76" spans="2:3" ht="33.75" customHeight="1">
+      <c r="B76" s="75" t="s">
+        <v>387</v>
+      </c>
+      <c r="C76" s="54" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="77" spans="2:3" ht="30">
+      <c r="B77" s="75" t="s">
+        <v>389</v>
+      </c>
+      <c r="C77" s="54" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="78" spans="2:3" ht="30.75">
+      <c r="B78" s="75" t="s">
+        <v>391</v>
+      </c>
+      <c r="C78" s="54" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="79" spans="2:3" ht="30">
+      <c r="B79" s="75" t="s">
+        <v>393</v>
+      </c>
+      <c r="C79" s="54" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="80" spans="2:3">
+      <c r="B80" s="75" t="s">
+        <v>395</v>
+      </c>
+      <c r="C80" s="54" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" s="76" t="s">
+        <v>403</v>
+      </c>
+      <c r="B82" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="C82" s="77" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" ht="270">
+      <c r="A83">
+        <v>1</v>
+      </c>
+      <c r="B83" s="78" t="s">
+        <v>397</v>
+      </c>
+      <c r="C83" s="54" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" ht="240">
+      <c r="A84">
+        <v>2</v>
+      </c>
+      <c r="B84" s="54" t="s">
+        <v>399</v>
+      </c>
+      <c r="C84" s="54" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="255">
+      <c r="A85">
+        <v>3</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="C85" s="13" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" ht="195">
+      <c r="B86" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="C86" s="42" t="s">
+        <v>295</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A56:A58"/>
-    <mergeCell ref="C56:C58"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B46:C46"/>
+  <mergeCells count="5">
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="C49:C51"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -9979,8 +10888,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:C48"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18:C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10006,7 +10915,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="105">
+    <row r="4" spans="2:3" ht="111" customHeight="1">
       <c r="B4" s="2" t="s">
         <v>267</v>
       </c>
@@ -10171,16 +11080,16 @@
       <c r="C24" s="37"/>
     </row>
     <row r="25" spans="2:3" ht="33" customHeight="1">
-      <c r="B25" s="61" t="s">
+      <c r="B25" s="63" t="s">
         <v>307</v>
       </c>
-      <c r="C25" s="61"/>
+      <c r="C25" s="63"/>
     </row>
     <row r="26" spans="2:3">
-      <c r="B26" s="61" t="s">
+      <c r="B26" s="63" t="s">
         <v>308</v>
       </c>
-      <c r="C26" s="61"/>
+      <c r="C26" s="63"/>
     </row>
     <row r="27" spans="2:3" ht="15.75" thickBot="1">
       <c r="B27" s="48" t="s">
@@ -10235,16 +11144,16 @@
       <c r="C35" s="51"/>
     </row>
     <row r="36" spans="2:3" ht="50.25" customHeight="1">
-      <c r="B36" s="61" t="s">
+      <c r="B36" s="63" t="s">
         <v>316</v>
       </c>
-      <c r="C36" s="61"/>
+      <c r="C36" s="63"/>
     </row>
     <row r="37" spans="2:3" ht="32.25" customHeight="1">
-      <c r="B37" s="61" t="s">
+      <c r="B37" s="63" t="s">
         <v>317</v>
       </c>
-      <c r="C37" s="61"/>
+      <c r="C37" s="63"/>
     </row>
     <row r="38" spans="2:3" ht="15.75" thickBot="1">
       <c r="B38" s="52" t="s">
@@ -10294,16 +11203,16 @@
       </c>
     </row>
     <row r="47" spans="2:3" ht="36" customHeight="1">
-      <c r="B47" s="61" t="s">
+      <c r="B47" s="63" t="s">
         <v>327</v>
       </c>
-      <c r="C47" s="61"/>
+      <c r="C47" s="63"/>
     </row>
     <row r="48" spans="2:3" ht="49.5" customHeight="1">
-      <c r="B48" s="61" t="s">
+      <c r="B48" s="63" t="s">
         <v>328</v>
       </c>
-      <c r="C48" s="61"/>
+      <c r="C48" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Add ApplicationContextProvider to obtain the ApplicationContext.
</commit_message>
<xml_diff>
--- a/Training_Plan.xlsx
+++ b/Training_Plan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="19155" windowHeight="11760" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="19155" windowHeight="11760" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Plan" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="407">
   <si>
     <t>Java core</t>
   </si>
@@ -4687,53 +4687,6 @@
     <t>Inversion of control in Spring?</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - Inversion of Control (IoC)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> is a general concept, and it can be expressed in many different ways and </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Dependency Injection </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>is merely one concrete example of Inversion of Control.
- - This concept says that you do not create your objects but describe how they should be created. 
- - You don't directly connect your components and services together in code but describe which services are needed by which components in a configuration file. 
- - A container (the IOC container) is then responsible for hooking it all up.</t>
-    </r>
-  </si>
-  <si>
     <t>What do you use Spring for?</t>
   </si>
   <si>
@@ -4893,123 +4846,6 @@
   </si>
   <si>
     <t>Annotation in Spring? What is the meaning of annotation @Controller?</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve"> - Starting from Spring 2.5 it became possible to configure the dependency injection using annotations. 
- - So instead of using XML to describe a bean wiring, you can move the bean configuration into the component class itself by using annotations on the relevant class, method, or field declaration.
-+  </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>@Required:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> The @Required annotation applies to bean property setter methods.
-+  </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">@Autowired </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">annotation can apply to bean property setter methods, non-setter methods, constructor and properties.
-+ </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>@Qualifier</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> annotation along with @Autowired can be used to remove the confusion by specifiying which exact bean will be wired.
- + </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>JSR-250 Annotations</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Spring supports JSR-250 based annotations which include @Resource, @PostConstruct and @PreDestroy annotations.
-+ </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>@Controller</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> annotation indicates that a particular class serves the role of a controller. DispatcherServlet delegates the request to the controllers to execute the functionality specific to it. </t>
-    </r>
   </si>
   <si>
     <t>What is Spring Template, REST template?</t>
@@ -7506,6 +7342,306 @@
   </si>
   <si>
     <t>Details</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> - Starting from Spring 2.5 it became possible to configure the dependency injection using annotations. 
+ - So instead of using XML to describe a bean wiring, you can move the bean configuration into the component class itself by using annotations on the relevant class, method, or field declaration.
++  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>@Required:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> The @Required annotation applies to bean property setter methods.
++  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">@Autowired </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">annotation can apply to bean property setter methods, constructor and properties.
++ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>@Qualifier</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> annotation along with @Autowired can be used to remove the confusion by specifiying which exact bean will be wired.
+ + </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>JSR-250 Annotations</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Spring supports JSR-250 based annotations which include @Resource, @PostConstruct and @PreDestroy annotations.
++ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>@Controller</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> annotation indicates that a particular class serves the role of a controller. DispatcherServlet delegates the request to the controllers to execute the functionality specific to it. </t>
+    </r>
+  </si>
+  <si>
+    <t>Components and Services</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A component is a small unit of reusable code. It should </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>implement</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and expose </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>just one service, and do it well</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. In practical terms, a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>component is a class that implements a service (interface)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. The interface is the contract of the service, which creates an abstraction layer so you can replace the service implementation without effort."</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Inversion of Control (IoC)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is a general concept, and it can be expressed in many different ways and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Dependency Injection </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">is merely one concrete example of Inversion of Control.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Inversion of Control (IoC)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> means that objects do not create other objects on which they rely to do their work. Instead, they get the objects that they need from an outside source (for example, an xml configuration file).
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Dependency Injection (DI)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> means that this is done without the object intervention, usually by a framework component that passes constructor parameters and set properties.
+ - This concept says that you do not create your objects but describe how they should be created. 
+ - You don't directly connect your components and services together in code but describe which services are needed by which components in a configuration file. 
+ - A </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>container</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (the IOC container) is then responsible for hooking it all up.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -7883,7 +8019,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -8006,36 +8142,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -8067,6 +8179,33 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -9186,10 +9325,10 @@
     <row r="27" spans="2:5">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
-      <c r="D27" s="56" t="s">
+      <c r="D27" s="71" t="s">
         <v>47</v>
       </c>
-      <c r="E27" s="57"/>
+      <c r="E27" s="72"/>
     </row>
     <row r="28" spans="2:5">
       <c r="B28" s="2"/>
@@ -9252,10 +9391,10 @@
     <row r="34" spans="2:5">
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
-      <c r="D34" s="60" t="s">
+      <c r="D34" s="75" t="s">
         <v>81</v>
       </c>
-      <c r="E34" s="60"/>
+      <c r="E34" s="75"/>
     </row>
     <row r="35" spans="2:5">
       <c r="B35" s="2"/>
@@ -9328,10 +9467,10 @@
     <row r="42" spans="2:5">
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
-      <c r="D42" s="61" t="s">
+      <c r="D42" s="76" t="s">
         <v>94</v>
       </c>
-      <c r="E42" s="62"/>
+      <c r="E42" s="77"/>
     </row>
     <row r="43" spans="2:5">
       <c r="B43" s="2"/>
@@ -9418,10 +9557,10 @@
     <row r="51" spans="2:5">
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
-      <c r="D51" s="58" t="s">
+      <c r="D51" s="73" t="s">
         <v>60</v>
       </c>
-      <c r="E51" s="58"/>
+      <c r="E51" s="73"/>
     </row>
     <row r="52" spans="2:5">
       <c r="B52" s="2"/>
@@ -9479,7 +9618,7 @@
       <c r="D57" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="E57" s="59" t="s">
+      <c r="E57" s="74" t="s">
         <v>73</v>
       </c>
     </row>
@@ -9489,7 +9628,7 @@
       <c r="D58" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="E58" s="59"/>
+      <c r="E58" s="74"/>
     </row>
     <row r="59" spans="2:5">
       <c r="B59" s="2"/>
@@ -10315,8 +10454,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A3:C86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="B86" sqref="B86"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10506,198 +10645,198 @@
     </row>
     <row r="40" spans="1:3">
       <c r="B40" s="2" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C40" s="2"/>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="55"/>
       <c r="B41" s="15" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C41" s="15" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="30">
       <c r="A42" s="53" t="s">
+        <v>328</v>
+      </c>
+      <c r="B42" s="53" t="s">
+        <v>329</v>
+      </c>
+      <c r="C42" s="53" t="s">
         <v>330</v>
-      </c>
-      <c r="B42" s="53" t="s">
-        <v>331</v>
-      </c>
-      <c r="C42" s="53" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="53" t="s">
+        <v>331</v>
+      </c>
+      <c r="B43" s="53" t="s">
+        <v>332</v>
+      </c>
+      <c r="C43" s="53" t="s">
         <v>333</v>
-      </c>
-      <c r="B43" s="53" t="s">
-        <v>334</v>
-      </c>
-      <c r="C43" s="53" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="53" t="s">
+        <v>334</v>
+      </c>
+      <c r="B44" s="53" t="s">
+        <v>335</v>
+      </c>
+      <c r="C44" s="53" t="s">
         <v>336</v>
-      </c>
-      <c r="B44" s="53" t="s">
-        <v>337</v>
-      </c>
-      <c r="C44" s="53" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="30">
       <c r="A45" s="53" t="s">
+        <v>337</v>
+      </c>
+      <c r="B45" s="53" t="s">
+        <v>338</v>
+      </c>
+      <c r="C45" s="53" t="s">
         <v>339</v>
-      </c>
-      <c r="B45" s="53" t="s">
-        <v>340</v>
-      </c>
-      <c r="C45" s="53" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="53" t="s">
+        <v>340</v>
+      </c>
+      <c r="B46" s="53" t="s">
+        <v>341</v>
+      </c>
+      <c r="C46" s="53" t="s">
         <v>342</v>
-      </c>
-      <c r="B46" s="53" t="s">
-        <v>343</v>
-      </c>
-      <c r="C46" s="53" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="30">
       <c r="A47" s="53" t="s">
+        <v>343</v>
+      </c>
+      <c r="B47" s="53" t="s">
+        <v>344</v>
+      </c>
+      <c r="C47" s="53" t="s">
         <v>345</v>
-      </c>
-      <c r="B47" s="53" t="s">
-        <v>346</v>
-      </c>
-      <c r="C47" s="53" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="30">
       <c r="A48" s="53" t="s">
+        <v>346</v>
+      </c>
+      <c r="B48" s="53" t="s">
+        <v>347</v>
+      </c>
+      <c r="C48" s="53" t="s">
         <v>348</v>
       </c>
-      <c r="B48" s="53" t="s">
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="74" t="s">
         <v>349</v>
       </c>
-      <c r="C48" s="53" t="s">
+      <c r="B49" s="53" t="s">
         <v>350</v>
       </c>
-    </row>
-    <row r="49" spans="1:3">
-      <c r="A49" s="59" t="s">
+      <c r="C49" s="74" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="74"/>
+      <c r="B50" s="53"/>
+      <c r="C50" s="74"/>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="74"/>
+      <c r="B51" s="53" t="s">
         <v>351</v>
       </c>
-      <c r="B49" s="53" t="s">
-        <v>352</v>
-      </c>
-      <c r="C49" s="59" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3">
-      <c r="A50" s="59"/>
-      <c r="B50" s="53"/>
-      <c r="C50" s="59"/>
-    </row>
-    <row r="51" spans="1:3">
-      <c r="A51" s="59"/>
-      <c r="B51" s="53" t="s">
-        <v>353</v>
-      </c>
-      <c r="C51" s="59"/>
+      <c r="C51" s="74"/>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="53" t="s">
+        <v>353</v>
+      </c>
+      <c r="B52" s="53" t="s">
+        <v>354</v>
+      </c>
+      <c r="C52" s="53" t="s">
         <v>355</v>
       </c>
-      <c r="B52" s="53" t="s">
-        <v>356</v>
-      </c>
-      <c r="C52" s="53" t="s">
-        <v>357</v>
-      </c>
     </row>
     <row r="53" spans="1:3">
-      <c r="B53" s="64"/>
+      <c r="B53" s="57"/>
     </row>
     <row r="54" spans="1:3" ht="31.5">
       <c r="B54" s="22" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="B55" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="B56" s="58"/>
+    </row>
+    <row r="57" spans="1:3" ht="32.25" customHeight="1">
+      <c r="B57" s="78" t="s">
+        <v>358</v>
+      </c>
+      <c r="C57" s="78"/>
+    </row>
+    <row r="58" spans="1:3" ht="33" customHeight="1">
+      <c r="B58" s="78" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="56" spans="1:3">
-      <c r="B56" s="65"/>
-    </row>
-    <row r="57" spans="1:3" ht="32.25" customHeight="1">
-      <c r="B57" s="66" t="s">
+      <c r="C58" s="78"/>
+    </row>
+    <row r="59" spans="1:3" ht="19.5" customHeight="1">
+      <c r="B59" s="78" t="s">
         <v>360</v>
       </c>
-      <c r="C57" s="66"/>
-    </row>
-    <row r="58" spans="1:3" ht="33" customHeight="1">
-      <c r="B58" s="66" t="s">
-        <v>361</v>
-      </c>
-      <c r="C58" s="66"/>
-    </row>
-    <row r="59" spans="1:3" ht="19.5" customHeight="1">
-      <c r="B59" s="66" t="s">
-        <v>362</v>
-      </c>
-      <c r="C59" s="66"/>
+      <c r="C59" s="78"/>
     </row>
     <row r="60" spans="1:3">
       <c r="B60" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="C60" s="2"/>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="B61" s="59"/>
+      <c r="C61" s="2"/>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="B62" s="60" t="s">
+        <v>362</v>
+      </c>
+      <c r="C62" s="2"/>
+    </row>
+    <row r="63" spans="1:3" ht="30">
+      <c r="B63" s="61" t="s">
         <v>363</v>
       </c>
-      <c r="C60" s="2"/>
-    </row>
-    <row r="61" spans="1:3">
-      <c r="B61" s="67"/>
-      <c r="C61" s="2"/>
-    </row>
-    <row r="62" spans="1:3">
-      <c r="B62" s="68" t="s">
+      <c r="C63" s="2"/>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="B64" s="60" t="s">
         <v>364</v>
-      </c>
-      <c r="C62" s="2"/>
-    </row>
-    <row r="63" spans="1:3" ht="30">
-      <c r="B63" s="69" t="s">
-        <v>365</v>
-      </c>
-      <c r="C63" s="2"/>
-    </row>
-    <row r="64" spans="1:3">
-      <c r="B64" s="68" t="s">
-        <v>366</v>
       </c>
       <c r="C64" s="2"/>
     </row>
     <row r="65" spans="2:3" ht="225">
       <c r="B65" s="2" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C65" s="54" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="66" spans="2:3" ht="30">
@@ -10707,137 +10846,137 @@
       <c r="C66" s="37"/>
     </row>
     <row r="67" spans="2:3" ht="30.75">
-      <c r="B67" s="71" t="s">
+      <c r="B67" s="63" t="s">
+        <v>367</v>
+      </c>
+      <c r="C67" s="54" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="68" spans="2:3" ht="137.25" customHeight="1">
+      <c r="B68" s="64" t="s">
         <v>369</v>
       </c>
-      <c r="C67" s="54" t="s">
+      <c r="C68" s="16" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="69" spans="2:3" ht="105.75">
+      <c r="B69" s="63" t="s">
         <v>370</v>
       </c>
-    </row>
-    <row r="68" spans="2:3" ht="137.25" customHeight="1">
-      <c r="B68" s="72" t="s">
+      <c r="C69" s="54" t="s">
         <v>371</v>
       </c>
-      <c r="C68" s="16" t="s">
+    </row>
+    <row r="70" spans="2:3" ht="53.25" customHeight="1">
+      <c r="B70" s="65" t="s">
+        <v>373</v>
+      </c>
+      <c r="C70" s="62" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="71" spans="2:3" ht="32.25" customHeight="1">
+      <c r="B71" s="63" t="s">
+        <v>374</v>
+      </c>
+      <c r="C71" s="62" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="72" spans="2:3" ht="135">
+      <c r="B72" s="63" t="s">
+        <v>377</v>
+      </c>
+      <c r="C72" s="66" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="69" spans="2:3" ht="105.75">
-      <c r="B69" s="71" t="s">
-        <v>372</v>
-      </c>
-      <c r="C69" s="54" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="70" spans="2:3" ht="53.25" customHeight="1">
-      <c r="B70" s="73" t="s">
-        <v>375</v>
-      </c>
-      <c r="C70" s="70" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="71" spans="2:3" ht="32.25" customHeight="1">
-      <c r="B71" s="71" t="s">
-        <v>376</v>
-      </c>
-      <c r="C71" s="70" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="72" spans="2:3" ht="135">
-      <c r="B72" s="71" t="s">
+    <row r="73" spans="2:3" ht="30.75">
+      <c r="B73" s="63" t="s">
         <v>379</v>
       </c>
-      <c r="C72" s="74" t="s">
+      <c r="C73" s="54" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="73" spans="2:3" ht="30.75">
-      <c r="B73" s="71" t="s">
+    <row r="74" spans="2:3">
+      <c r="B74" s="67" t="s">
         <v>381</v>
       </c>
-      <c r="C73" s="54" t="s">
+      <c r="C74" s="67" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="74" spans="2:3">
-      <c r="B74" s="75" t="s">
+    <row r="75" spans="2:3" ht="30">
+      <c r="B75" s="67" t="s">
         <v>383</v>
       </c>
-      <c r="C74" s="75" t="s">
+      <c r="C75" s="54" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="75" spans="2:3" ht="30">
-      <c r="B75" s="75" t="s">
+    <row r="76" spans="2:3" ht="33.75" customHeight="1">
+      <c r="B76" s="67" t="s">
         <v>385</v>
       </c>
-      <c r="C75" s="54" t="s">
+      <c r="C76" s="54" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="76" spans="2:3" ht="33.75" customHeight="1">
-      <c r="B76" s="75" t="s">
+    <row r="77" spans="2:3" ht="30">
+      <c r="B77" s="67" t="s">
         <v>387</v>
       </c>
-      <c r="C76" s="54" t="s">
+      <c r="C77" s="54" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="77" spans="2:3" ht="30">
-      <c r="B77" s="75" t="s">
+    <row r="78" spans="2:3" ht="30.75">
+      <c r="B78" s="67" t="s">
         <v>389</v>
       </c>
-      <c r="C77" s="54" t="s">
+      <c r="C78" s="54" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="78" spans="2:3" ht="30.75">
-      <c r="B78" s="75" t="s">
+    <row r="79" spans="2:3" ht="30">
+      <c r="B79" s="67" t="s">
         <v>391</v>
       </c>
-      <c r="C78" s="54" t="s">
+      <c r="C79" s="54" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="79" spans="2:3" ht="30">
-      <c r="B79" s="75" t="s">
+    <row r="80" spans="2:3">
+      <c r="B80" s="67" t="s">
         <v>393</v>
       </c>
-      <c r="C79" s="54" t="s">
+      <c r="C80" s="54" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="80" spans="2:3">
-      <c r="B80" s="75" t="s">
-        <v>395</v>
-      </c>
-      <c r="C80" s="54" t="s">
-        <v>396</v>
-      </c>
-    </row>
     <row r="82" spans="1:3">
-      <c r="A82" s="76" t="s">
-        <v>403</v>
+      <c r="A82" s="68" t="s">
+        <v>401</v>
       </c>
       <c r="B82" s="15" t="s">
         <v>217</v>
       </c>
-      <c r="C82" s="77" t="s">
-        <v>404</v>
+      <c r="C82" s="69" t="s">
+        <v>402</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="270">
       <c r="A83">
         <v>1</v>
       </c>
-      <c r="B83" s="78" t="s">
-        <v>397</v>
+      <c r="B83" s="70" t="s">
+        <v>395</v>
       </c>
       <c r="C83" s="54" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="240">
@@ -10845,10 +10984,10 @@
         <v>2</v>
       </c>
       <c r="B84" s="54" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C84" s="54" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="255">
@@ -10856,18 +10995,18 @@
         <v>3</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C85" s="13" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="195">
       <c r="B86" s="4" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C86" s="42" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
   </sheetData>
@@ -10886,10 +11025,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:C48"/>
+  <dimension ref="B2:C49"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18:C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10915,313 +11054,321 @@
         <v>266</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="111" customHeight="1">
+    <row r="4" spans="2:3" ht="205.5" customHeight="1">
       <c r="B4" s="2" t="s">
         <v>267</v>
       </c>
       <c r="C4" s="40" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" ht="62.25" customHeight="1">
+      <c r="B5" s="35" t="s">
+        <v>404</v>
+      </c>
+      <c r="C5" s="40" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" ht="307.5" customHeight="1">
+      <c r="B6" s="4" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="5" spans="2:3" ht="285">
-      <c r="B5" s="4" t="s">
+      <c r="C6" s="40" t="s">
         <v>269</v>
       </c>
-      <c r="C5" s="40" t="s">
+    </row>
+    <row r="7" spans="2:3" ht="180">
+      <c r="B7" s="37" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="6" spans="2:3" ht="195">
-      <c r="B6" s="37" t="s">
+      <c r="C7" s="56" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" ht="105">
+      <c r="B8" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="C6" s="37" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" ht="105">
-      <c r="B7" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="C7" s="37" t="s">
+      <c r="C8" s="37" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3">
+      <c r="B9" s="15" t="s">
+        <v>275</v>
+      </c>
+      <c r="C9" s="15" t="s">
         <v>276</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3">
-      <c r="B8" s="15" t="s">
-        <v>277</v>
-      </c>
-      <c r="C8" s="15" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3">
-      <c r="B9" s="37" t="s">
-        <v>279</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="10" spans="2:3">
       <c r="B10" s="37" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
     </row>
     <row r="11" spans="2:3">
       <c r="B11" s="37" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
     </row>
     <row r="12" spans="2:3">
       <c r="B12" s="37" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
     </row>
     <row r="13" spans="2:3">
       <c r="B13" s="37" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
     </row>
     <row r="14" spans="2:3">
       <c r="B14" s="37" t="s">
+        <v>285</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3">
+      <c r="B15" s="37" t="s">
+        <v>287</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3">
+      <c r="B16" s="37"/>
+      <c r="C16" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="C14" s="2" t="s">
+    </row>
+    <row r="17" spans="2:3" ht="60">
+      <c r="B17" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="C17" s="37" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" ht="165">
+      <c r="B18" s="2" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="15" spans="2:3">
-      <c r="B15" s="37"/>
-      <c r="C15" s="2" t="s">
+      <c r="C18" s="41" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="16" spans="2:3" ht="60">
-      <c r="B16" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="C16" s="37" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" ht="165">
-      <c r="B17" s="2" t="s">
+    <row r="19" spans="2:3" ht="195">
+      <c r="B19" s="4" t="s">
         <v>292</v>
       </c>
-      <c r="C17" s="41" t="s">
+      <c r="C19" s="42" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="18" spans="2:3" ht="195">
-      <c r="B18" s="4" t="s">
+    <row r="20" spans="2:3" ht="165">
+      <c r="B20" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="C18" s="42" t="s">
+      <c r="C20" s="37" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="19" spans="2:3" ht="165">
-      <c r="B19" s="2" t="s">
+    <row r="21" spans="2:3" ht="409.5" customHeight="1">
+      <c r="B21" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="C19" s="37" t="s">
+      <c r="C21" s="40" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="20" spans="2:3" ht="409.5" customHeight="1">
-      <c r="B20" s="2" t="s">
+    <row r="22" spans="2:3" ht="45">
+      <c r="B22" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="C20" s="40" t="s">
+      <c r="C22" s="37" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="21" spans="2:3" ht="45">
-      <c r="B21" s="2" t="s">
+    <row r="23" spans="2:3" ht="30">
+      <c r="B23" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="C21" s="37" t="s">
+      <c r="C23" s="37" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="22" spans="2:3" ht="30">
-      <c r="B22" s="2" t="s">
+    <row r="24" spans="2:3" ht="225">
+      <c r="B24" s="43" t="s">
         <v>302</v>
       </c>
-      <c r="C22" s="37" t="s">
+      <c r="C24" s="40" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="23" spans="2:3" ht="225">
-      <c r="B23" s="43" t="s">
+    <row r="25" spans="2:3" ht="26.25">
+      <c r="B25" s="44" t="s">
         <v>304</v>
       </c>
-      <c r="C23" s="40" t="s">
+      <c r="C25" s="37"/>
+    </row>
+    <row r="26" spans="2:3" ht="33" customHeight="1">
+      <c r="B26" s="79" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="24" spans="2:3" ht="26.25">
-      <c r="B24" s="44" t="s">
+      <c r="C26" s="79"/>
+    </row>
+    <row r="27" spans="2:3">
+      <c r="B27" s="79" t="s">
         <v>306</v>
       </c>
-      <c r="C24" s="37"/>
-    </row>
-    <row r="25" spans="2:3" ht="33" customHeight="1">
-      <c r="B25" s="63" t="s">
+      <c r="C27" s="79"/>
+    </row>
+    <row r="28" spans="2:3" ht="15.75" thickBot="1">
+      <c r="B28" s="48" t="s">
+        <v>33</v>
+      </c>
+      <c r="C28" s="49"/>
+    </row>
+    <row r="29" spans="2:3" ht="15.75" thickBot="1">
+      <c r="B29" s="47" t="s">
         <v>307</v>
       </c>
-      <c r="C25" s="63"/>
-    </row>
-    <row r="26" spans="2:3">
-      <c r="B26" s="63" t="s">
+      <c r="C29" s="2"/>
+    </row>
+    <row r="30" spans="2:3" ht="15.75" thickBot="1">
+      <c r="B30" s="46" t="s">
         <v>308</v>
       </c>
-      <c r="C26" s="63"/>
-    </row>
-    <row r="27" spans="2:3" ht="15.75" thickBot="1">
-      <c r="B27" s="48" t="s">
-        <v>33</v>
-      </c>
-      <c r="C27" s="49"/>
-    </row>
-    <row r="28" spans="2:3" ht="15.75" thickBot="1">
-      <c r="B28" s="47" t="s">
+      <c r="C30" s="2"/>
+    </row>
+    <row r="31" spans="2:3" ht="15.75" thickBot="1">
+      <c r="B31" s="47" t="s">
         <v>309</v>
       </c>
-      <c r="C28" s="2"/>
-    </row>
-    <row r="29" spans="2:3" ht="15.75" thickBot="1">
-      <c r="B29" s="46" t="s">
+      <c r="C31" s="2"/>
+    </row>
+    <row r="32" spans="2:3" ht="15.75" thickBot="1">
+      <c r="B32" s="45"/>
+      <c r="C32" s="2"/>
+    </row>
+    <row r="33" spans="2:3" ht="15.75" thickBot="1">
+      <c r="B33" s="47" t="s">
         <v>310</v>
-      </c>
-      <c r="C29" s="2"/>
-    </row>
-    <row r="30" spans="2:3" ht="15.75" thickBot="1">
-      <c r="B30" s="47" t="s">
-        <v>311</v>
-      </c>
-      <c r="C30" s="2"/>
-    </row>
-    <row r="31" spans="2:3" ht="15.75" thickBot="1">
-      <c r="B31" s="45"/>
-      <c r="C31" s="2"/>
-    </row>
-    <row r="32" spans="2:3" ht="15.75" thickBot="1">
-      <c r="B32" s="47" t="s">
-        <v>312</v>
-      </c>
-      <c r="C32" s="2"/>
-    </row>
-    <row r="33" spans="2:3" ht="15.75" thickBot="1">
-      <c r="B33" s="46" t="s">
-        <v>313</v>
       </c>
       <c r="C33" s="2"/>
     </row>
     <row r="34" spans="2:3" ht="15.75" thickBot="1">
       <c r="B34" s="46" t="s">
+        <v>311</v>
+      </c>
+      <c r="C34" s="2"/>
+    </row>
+    <row r="35" spans="2:3" ht="15.75" thickBot="1">
+      <c r="B35" s="46" t="s">
+        <v>312</v>
+      </c>
+      <c r="C35" s="2"/>
+    </row>
+    <row r="36" spans="2:3">
+      <c r="B36" s="50" t="s">
+        <v>313</v>
+      </c>
+      <c r="C36" s="51"/>
+    </row>
+    <row r="37" spans="2:3" ht="50.25" customHeight="1">
+      <c r="B37" s="79" t="s">
         <v>314</v>
       </c>
-      <c r="C34" s="2"/>
-    </row>
-    <row r="35" spans="2:3">
-      <c r="B35" s="50" t="s">
+      <c r="C37" s="79"/>
+    </row>
+    <row r="38" spans="2:3" ht="32.25" customHeight="1">
+      <c r="B38" s="79" t="s">
         <v>315</v>
       </c>
-      <c r="C35" s="51"/>
-    </row>
-    <row r="36" spans="2:3" ht="50.25" customHeight="1">
-      <c r="B36" s="63" t="s">
+      <c r="C38" s="79"/>
+    </row>
+    <row r="39" spans="2:3" ht="15.75" thickBot="1">
+      <c r="B39" s="52" t="s">
         <v>316</v>
       </c>
-      <c r="C36" s="63"/>
-    </row>
-    <row r="37" spans="2:3" ht="32.25" customHeight="1">
-      <c r="B37" s="63" t="s">
-        <v>317</v>
-      </c>
-      <c r="C37" s="63"/>
-    </row>
-    <row r="38" spans="2:3" ht="15.75" thickBot="1">
-      <c r="B38" s="52" t="s">
-        <v>318</v>
-      </c>
-      <c r="C38" s="49"/>
-    </row>
-    <row r="39" spans="2:3" ht="15.75" thickBot="1">
-      <c r="B39" s="46" t="s">
-        <v>319</v>
-      </c>
-      <c r="C39" s="2"/>
+      <c r="C39" s="49"/>
     </row>
     <row r="40" spans="2:3" ht="15.75" thickBot="1">
       <c r="B40" s="46" t="s">
-        <v>320</v>
-      </c>
+        <v>317</v>
+      </c>
+      <c r="C40" s="2"/>
     </row>
     <row r="41" spans="2:3" ht="15.75" thickBot="1">
       <c r="B41" s="46" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="42" spans="2:3" ht="15.75" thickBot="1">
       <c r="B42" s="46" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="43" spans="2:3" ht="15.75" thickBot="1">
       <c r="B43" s="46" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
     </row>
     <row r="44" spans="2:3" ht="15.75" thickBot="1">
       <c r="B44" s="46" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
     </row>
     <row r="45" spans="2:3" ht="15.75" thickBot="1">
       <c r="B45" s="46" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" ht="15.75" thickBot="1">
+      <c r="B46" s="46" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3">
+      <c r="B47" s="50" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" ht="36" customHeight="1">
+      <c r="B48" s="79" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="46" spans="2:3">
-      <c r="B46" s="50" t="s">
+      <c r="C48" s="79"/>
+    </row>
+    <row r="49" spans="2:3" ht="49.5" customHeight="1">
+      <c r="B49" s="79" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="47" spans="2:3" ht="36" customHeight="1">
-      <c r="B47" s="63" t="s">
-        <v>327</v>
-      </c>
-      <c r="C47" s="63"/>
-    </row>
-    <row r="48" spans="2:3" ht="49.5" customHeight="1">
-      <c r="B48" s="63" t="s">
-        <v>328</v>
-      </c>
-      <c r="C48" s="63"/>
+      <c r="C49" s="79"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
     <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B47:C47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Centralize the database configuration bean to Hibernate.xml
</commit_message>
<xml_diff>
--- a/Training_Plan.xlsx
+++ b/Training_Plan.xlsx
@@ -5558,11 +5558,6 @@
     <t>How many spring modules have you worked with?</t>
   </si>
   <si>
-    <t xml:space="preserve"> - The core container, Spring context(ApplicationContext)
- - Spring DAO to integrate with Hibernate
- - Spring Web module, Spring MVC framework for developping RESTFul web services</t>
-  </si>
-  <si>
     <t>How does Spring MVC  find the right controller?</t>
   </si>
   <si>
@@ -7642,6 +7637,11 @@
       </rPr>
       <t xml:space="preserve"> (the IOC container) is then responsible for hooking it all up.</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> - The core container, Spring context(ApplicationContext)
+ - Spring DAO, ORM to integrate with Hibernate
+ - Spring Web module, Spring MVC framework for developping RESTFul web services</t>
   </si>
 </sst>
 </file>
@@ -8019,7 +8019,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -8180,6 +8180,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -9325,10 +9328,10 @@
     <row r="27" spans="2:5">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
-      <c r="D27" s="71" t="s">
+      <c r="D27" s="72" t="s">
         <v>47</v>
       </c>
-      <c r="E27" s="72"/>
+      <c r="E27" s="73"/>
     </row>
     <row r="28" spans="2:5">
       <c r="B28" s="2"/>
@@ -9391,10 +9394,10 @@
     <row r="34" spans="2:5">
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
-      <c r="D34" s="75" t="s">
+      <c r="D34" s="76" t="s">
         <v>81</v>
       </c>
-      <c r="E34" s="75"/>
+      <c r="E34" s="76"/>
     </row>
     <row r="35" spans="2:5">
       <c r="B35" s="2"/>
@@ -9467,10 +9470,10 @@
     <row r="42" spans="2:5">
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
-      <c r="D42" s="76" t="s">
+      <c r="D42" s="77" t="s">
         <v>94</v>
       </c>
-      <c r="E42" s="77"/>
+      <c r="E42" s="78"/>
     </row>
     <row r="43" spans="2:5">
       <c r="B43" s="2"/>
@@ -9557,10 +9560,10 @@
     <row r="51" spans="2:5">
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
-      <c r="D51" s="73" t="s">
+      <c r="D51" s="74" t="s">
         <v>60</v>
       </c>
-      <c r="E51" s="73"/>
+      <c r="E51" s="74"/>
     </row>
     <row r="52" spans="2:5">
       <c r="B52" s="2"/>
@@ -9618,7 +9621,7 @@
       <c r="D57" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="E57" s="74" t="s">
+      <c r="E57" s="75" t="s">
         <v>73</v>
       </c>
     </row>
@@ -9628,7 +9631,7 @@
       <c r="D58" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="E58" s="74"/>
+      <c r="E58" s="75"/>
     </row>
     <row r="59" spans="2:5">
       <c r="B59" s="2"/>
@@ -10645,7 +10648,7 @@
     </row>
     <row r="40" spans="1:3">
       <c r="B40" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C40" s="2"/>
     </row>
@@ -10660,113 +10663,113 @@
     </row>
     <row r="42" spans="1:3" ht="30">
       <c r="A42" s="53" t="s">
+        <v>327</v>
+      </c>
+      <c r="B42" s="53" t="s">
         <v>328</v>
       </c>
-      <c r="B42" s="53" t="s">
+      <c r="C42" s="53" t="s">
         <v>329</v>
-      </c>
-      <c r="C42" s="53" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="53" t="s">
+        <v>330</v>
+      </c>
+      <c r="B43" s="53" t="s">
         <v>331</v>
       </c>
-      <c r="B43" s="53" t="s">
+      <c r="C43" s="53" t="s">
         <v>332</v>
-      </c>
-      <c r="C43" s="53" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="53" t="s">
+        <v>333</v>
+      </c>
+      <c r="B44" s="53" t="s">
         <v>334</v>
       </c>
-      <c r="B44" s="53" t="s">
+      <c r="C44" s="53" t="s">
         <v>335</v>
-      </c>
-      <c r="C44" s="53" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="30">
       <c r="A45" s="53" t="s">
+        <v>336</v>
+      </c>
+      <c r="B45" s="53" t="s">
         <v>337</v>
       </c>
-      <c r="B45" s="53" t="s">
+      <c r="C45" s="53" t="s">
         <v>338</v>
-      </c>
-      <c r="C45" s="53" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="53" t="s">
+        <v>339</v>
+      </c>
+      <c r="B46" s="53" t="s">
         <v>340</v>
       </c>
-      <c r="B46" s="53" t="s">
+      <c r="C46" s="53" t="s">
         <v>341</v>
-      </c>
-      <c r="C46" s="53" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="30">
       <c r="A47" s="53" t="s">
+        <v>342</v>
+      </c>
+      <c r="B47" s="53" t="s">
         <v>343</v>
       </c>
-      <c r="B47" s="53" t="s">
+      <c r="C47" s="53" t="s">
         <v>344</v>
-      </c>
-      <c r="C47" s="53" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="30">
       <c r="A48" s="53" t="s">
+        <v>345</v>
+      </c>
+      <c r="B48" s="53" t="s">
         <v>346</v>
       </c>
-      <c r="B48" s="53" t="s">
+      <c r="C48" s="53" t="s">
         <v>347</v>
       </c>
-      <c r="C48" s="53" t="s">
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="75" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="49" spans="1:3">
-      <c r="A49" s="74" t="s">
+      <c r="B49" s="53" t="s">
         <v>349</v>
       </c>
-      <c r="B49" s="53" t="s">
+      <c r="C49" s="75" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="75"/>
+      <c r="B50" s="53"/>
+      <c r="C50" s="75"/>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="75"/>
+      <c r="B51" s="53" t="s">
         <v>350</v>
       </c>
-      <c r="C49" s="74" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3">
-      <c r="A50" s="74"/>
-      <c r="B50" s="53"/>
-      <c r="C50" s="74"/>
-    </row>
-    <row r="51" spans="1:3">
-      <c r="A51" s="74"/>
-      <c r="B51" s="53" t="s">
-        <v>351</v>
-      </c>
-      <c r="C51" s="74"/>
+      <c r="C51" s="75"/>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="53" t="s">
+        <v>352</v>
+      </c>
+      <c r="B52" s="53" t="s">
         <v>353</v>
       </c>
-      <c r="B52" s="53" t="s">
+      <c r="C52" s="53" t="s">
         <v>354</v>
-      </c>
-      <c r="C52" s="53" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -10774,38 +10777,38 @@
     </row>
     <row r="54" spans="1:3" ht="31.5">
       <c r="B54" s="22" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="B55" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="B56" s="58"/>
     </row>
     <row r="57" spans="1:3" ht="32.25" customHeight="1">
-      <c r="B57" s="78" t="s">
+      <c r="B57" s="79" t="s">
+        <v>357</v>
+      </c>
+      <c r="C57" s="79"/>
+    </row>
+    <row r="58" spans="1:3" ht="33" customHeight="1">
+      <c r="B58" s="79" t="s">
         <v>358</v>
       </c>
-      <c r="C57" s="78"/>
-    </row>
-    <row r="58" spans="1:3" ht="33" customHeight="1">
-      <c r="B58" s="78" t="s">
+      <c r="C58" s="79"/>
+    </row>
+    <row r="59" spans="1:3" ht="19.5" customHeight="1">
+      <c r="B59" s="79" t="s">
         <v>359</v>
       </c>
-      <c r="C58" s="78"/>
-    </row>
-    <row r="59" spans="1:3" ht="19.5" customHeight="1">
-      <c r="B59" s="78" t="s">
-        <v>360</v>
-      </c>
-      <c r="C59" s="78"/>
+      <c r="C59" s="79"/>
     </row>
     <row r="60" spans="1:3">
       <c r="B60" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C60" s="2"/>
     </row>
@@ -10815,28 +10818,28 @@
     </row>
     <row r="62" spans="1:3">
       <c r="B62" s="60" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C62" s="2"/>
     </row>
     <row r="63" spans="1:3" ht="30">
       <c r="B63" s="61" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C63" s="2"/>
     </row>
     <row r="64" spans="1:3">
       <c r="B64" s="60" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C64" s="2"/>
     </row>
     <row r="65" spans="2:3" ht="225">
       <c r="B65" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="C65" s="54" t="s">
         <v>365</v>
-      </c>
-      <c r="C65" s="54" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="66" spans="2:3" ht="30">
@@ -10847,125 +10850,125 @@
     </row>
     <row r="67" spans="2:3" ht="30.75">
       <c r="B67" s="63" t="s">
+        <v>366</v>
+      </c>
+      <c r="C67" s="54" t="s">
         <v>367</v>
-      </c>
-      <c r="C67" s="54" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="68" spans="2:3" ht="137.25" customHeight="1">
       <c r="B68" s="64" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C68" s="16" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="69" spans="2:3" ht="105.75">
       <c r="B69" s="63" t="s">
+        <v>369</v>
+      </c>
+      <c r="C69" s="54" t="s">
         <v>370</v>
-      </c>
-      <c r="C69" s="54" t="s">
-        <v>371</v>
       </c>
     </row>
     <row r="70" spans="2:3" ht="53.25" customHeight="1">
       <c r="B70" s="65" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C70" s="62" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="71" spans="2:3" ht="32.25" customHeight="1">
       <c r="B71" s="63" t="s">
+        <v>373</v>
+      </c>
+      <c r="C71" s="62" t="s">
         <v>374</v>
-      </c>
-      <c r="C71" s="62" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="72" spans="2:3" ht="135">
       <c r="B72" s="63" t="s">
+        <v>376</v>
+      </c>
+      <c r="C72" s="66" t="s">
         <v>377</v>
-      </c>
-      <c r="C72" s="66" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="73" spans="2:3" ht="30.75">
       <c r="B73" s="63" t="s">
+        <v>378</v>
+      </c>
+      <c r="C73" s="54" t="s">
         <v>379</v>
-      </c>
-      <c r="C73" s="54" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="74" spans="2:3">
       <c r="B74" s="67" t="s">
+        <v>380</v>
+      </c>
+      <c r="C74" s="67" t="s">
         <v>381</v>
-      </c>
-      <c r="C74" s="67" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="75" spans="2:3" ht="30">
       <c r="B75" s="67" t="s">
+        <v>382</v>
+      </c>
+      <c r="C75" s="54" t="s">
         <v>383</v>
-      </c>
-      <c r="C75" s="54" t="s">
-        <v>384</v>
       </c>
     </row>
     <row r="76" spans="2:3" ht="33.75" customHeight="1">
       <c r="B76" s="67" t="s">
+        <v>384</v>
+      </c>
+      <c r="C76" s="54" t="s">
         <v>385</v>
-      </c>
-      <c r="C76" s="54" t="s">
-        <v>386</v>
       </c>
     </row>
     <row r="77" spans="2:3" ht="30">
       <c r="B77" s="67" t="s">
+        <v>386</v>
+      </c>
+      <c r="C77" s="54" t="s">
         <v>387</v>
-      </c>
-      <c r="C77" s="54" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="78" spans="2:3" ht="30.75">
       <c r="B78" s="67" t="s">
+        <v>388</v>
+      </c>
+      <c r="C78" s="54" t="s">
         <v>389</v>
-      </c>
-      <c r="C78" s="54" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="79" spans="2:3" ht="30">
       <c r="B79" s="67" t="s">
+        <v>390</v>
+      </c>
+      <c r="C79" s="54" t="s">
         <v>391</v>
-      </c>
-      <c r="C79" s="54" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="80" spans="2:3">
       <c r="B80" s="67" t="s">
+        <v>392</v>
+      </c>
+      <c r="C80" s="54" t="s">
         <v>393</v>
-      </c>
-      <c r="C80" s="54" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" s="68" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B82" s="15" t="s">
         <v>217</v>
       </c>
       <c r="C82" s="69" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="270">
@@ -10973,10 +10976,10 @@
         <v>1</v>
       </c>
       <c r="B83" s="70" t="s">
+        <v>394</v>
+      </c>
+      <c r="C83" s="54" t="s">
         <v>395</v>
-      </c>
-      <c r="C83" s="54" t="s">
-        <v>396</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="240">
@@ -10984,10 +10987,10 @@
         <v>2</v>
       </c>
       <c r="B84" s="54" t="s">
+        <v>396</v>
+      </c>
+      <c r="C84" s="54" t="s">
         <v>397</v>
-      </c>
-      <c r="C84" s="54" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="255">
@@ -10995,10 +10998,10 @@
         <v>3</v>
       </c>
       <c r="B85" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="C85" s="13" t="s">
         <v>399</v>
-      </c>
-      <c r="C85" s="13" t="s">
-        <v>400</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="195">
@@ -11027,8 +11030,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:C49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11059,15 +11062,15 @@
         <v>267</v>
       </c>
       <c r="C4" s="40" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="62.25" customHeight="1">
       <c r="B5" s="35" t="s">
+        <v>403</v>
+      </c>
+      <c r="C5" s="40" t="s">
         <v>404</v>
-      </c>
-      <c r="C5" s="40" t="s">
-        <v>405</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="307.5" customHeight="1">
@@ -11083,7 +11086,7 @@
         <v>270</v>
       </c>
       <c r="C7" s="56" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="105">
@@ -11200,43 +11203,43 @@
       <c r="B22" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="C22" s="37" t="s">
-        <v>299</v>
+      <c r="C22" s="71" t="s">
+        <v>406</v>
       </c>
     </row>
     <row r="23" spans="2:3" ht="30">
       <c r="B23" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="C23" s="37" t="s">
         <v>300</v>
-      </c>
-      <c r="C23" s="37" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="24" spans="2:3" ht="225">
       <c r="B24" s="43" t="s">
+        <v>301</v>
+      </c>
+      <c r="C24" s="40" t="s">
         <v>302</v>
-      </c>
-      <c r="C24" s="40" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="25" spans="2:3" ht="26.25">
       <c r="B25" s="44" t="s">
+        <v>303</v>
+      </c>
+      <c r="C25" s="37"/>
+    </row>
+    <row r="26" spans="2:3" ht="33" customHeight="1">
+      <c r="B26" s="80" t="s">
         <v>304</v>
       </c>
-      <c r="C25" s="37"/>
-    </row>
-    <row r="26" spans="2:3" ht="33" customHeight="1">
-      <c r="B26" s="79" t="s">
+      <c r="C26" s="80"/>
+    </row>
+    <row r="27" spans="2:3">
+      <c r="B27" s="80" t="s">
         <v>305</v>
       </c>
-      <c r="C26" s="79"/>
-    </row>
-    <row r="27" spans="2:3">
-      <c r="B27" s="79" t="s">
-        <v>306</v>
-      </c>
-      <c r="C27" s="79"/>
+      <c r="C27" s="80"/>
     </row>
     <row r="28" spans="2:3" ht="15.75" thickBot="1">
       <c r="B28" s="48" t="s">
@@ -11246,19 +11249,19 @@
     </row>
     <row r="29" spans="2:3" ht="15.75" thickBot="1">
       <c r="B29" s="47" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C29" s="2"/>
     </row>
     <row r="30" spans="2:3" ht="15.75" thickBot="1">
       <c r="B30" s="46" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C30" s="2"/>
     </row>
     <row r="31" spans="2:3" ht="15.75" thickBot="1">
       <c r="B31" s="47" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C31" s="2"/>
     </row>
@@ -11268,98 +11271,98 @@
     </row>
     <row r="33" spans="2:3" ht="15.75" thickBot="1">
       <c r="B33" s="47" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C33" s="2"/>
     </row>
     <row r="34" spans="2:3" ht="15.75" thickBot="1">
       <c r="B34" s="46" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C34" s="2"/>
     </row>
     <row r="35" spans="2:3" ht="15.75" thickBot="1">
       <c r="B35" s="46" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C35" s="2"/>
     </row>
     <row r="36" spans="2:3">
       <c r="B36" s="50" t="s">
+        <v>312</v>
+      </c>
+      <c r="C36" s="51"/>
+    </row>
+    <row r="37" spans="2:3" ht="50.25" customHeight="1">
+      <c r="B37" s="80" t="s">
         <v>313</v>
       </c>
-      <c r="C36" s="51"/>
-    </row>
-    <row r="37" spans="2:3" ht="50.25" customHeight="1">
-      <c r="B37" s="79" t="s">
+      <c r="C37" s="80"/>
+    </row>
+    <row r="38" spans="2:3" ht="32.25" customHeight="1">
+      <c r="B38" s="80" t="s">
         <v>314</v>
       </c>
-      <c r="C37" s="79"/>
-    </row>
-    <row r="38" spans="2:3" ht="32.25" customHeight="1">
-      <c r="B38" s="79" t="s">
-        <v>315</v>
-      </c>
-      <c r="C38" s="79"/>
+      <c r="C38" s="80"/>
     </row>
     <row r="39" spans="2:3" ht="15.75" thickBot="1">
       <c r="B39" s="52" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C39" s="49"/>
     </row>
     <row r="40" spans="2:3" ht="15.75" thickBot="1">
       <c r="B40" s="46" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C40" s="2"/>
     </row>
     <row r="41" spans="2:3" ht="15.75" thickBot="1">
       <c r="B41" s="46" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="42" spans="2:3" ht="15.75" thickBot="1">
       <c r="B42" s="46" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="43" spans="2:3" ht="15.75" thickBot="1">
       <c r="B43" s="46" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="44" spans="2:3" ht="15.75" thickBot="1">
       <c r="B44" s="46" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="45" spans="2:3" ht="15.75" thickBot="1">
       <c r="B45" s="46" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="46" spans="2:3" ht="15.75" thickBot="1">
       <c r="B46" s="46" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="47" spans="2:3">
       <c r="B47" s="50" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" ht="36" customHeight="1">
+      <c r="B48" s="80" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="48" spans="2:3" ht="36" customHeight="1">
-      <c r="B48" s="79" t="s">
+      <c r="C48" s="80"/>
+    </row>
+    <row r="49" spans="2:3" ht="49.5" customHeight="1">
+      <c r="B49" s="80" t="s">
         <v>325</v>
       </c>
-      <c r="C48" s="79"/>
-    </row>
-    <row r="49" spans="2:3" ht="49.5" customHeight="1">
-      <c r="B49" s="79" t="s">
-        <v>326</v>
-      </c>
-      <c r="C49" s="79"/>
+      <c r="C49" s="80"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Adding some new questions and using qualifier for injecting.
</commit_message>
<xml_diff>
--- a/Training_Plan.xlsx
+++ b/Training_Plan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="19155" windowHeight="11760" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="19155" windowHeight="11760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Plan" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="407">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="429">
   <si>
     <t>Java core</t>
   </si>
@@ -1695,9 +1695,6 @@
   </si>
   <si>
     <t>Java Serialization with array or collection</t>
-  </si>
-  <si>
-    <t>Rule: In case of array or collection, all the objects of array or collection must be serializable. If any object is not serialiizable, serialization will be failed.</t>
   </si>
   <si>
     <t>Externalizable in java</t>
@@ -7642,6 +7639,107 @@
     <t xml:space="preserve"> - The core container, Spring context(ApplicationContext)
  - Spring DAO, ORM to integrate with Hibernate
  - Spring Web module, Spring MVC framework for developping RESTFul web services</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Rule: In case of array or collection, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>all the objects of array or collection must be serializable</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. If any object is not serialiizable, serialization will be failed.</t>
+    </r>
+  </si>
+  <si>
+    <t>Building a RESTFul Service with Spring MVC</t>
+  </si>
+  <si>
+    <t>Create resource representation class</t>
+  </si>
+  <si>
+    <t>SOAP based web service while still serve a purpose are bloated, hard to consume directly from the client side and are bound by a hard contract. REST services on the other hand have been a go to choice for developing services consumed by web applications due to the lightweight JSON responses and soft contract. What I mean by soft contract is, REST services aren’t bound to a WSDL but still have a contract in which you need to abide by or have a versioning strategy in place.</t>
+  </si>
+  <si>
+    <t>While not overly exciting lots of folks are familiar with insurance, agencies sell policies to policyholders. Lets say we want to get all the possible agencies we can purchase a policy from.</t>
+  </si>
+  <si>
+    <t>Expectation</t>
+  </si>
+  <si>
+    <t>Depending on your philosophy of building services, you could return domain object from your business logic layer or create a class that represents the resource a client is requesting. In our case lets create an agency resource object that contains a small subset of an agency object.</t>
+  </si>
+  <si>
+    <t>Defines which service entry points correspond to a given HTTP url, and how parameters are to be read from the HTTP request</t>
+  </si>
+  <si>
+    <t>Presentation layer</t>
+  </si>
+  <si>
+    <t>Service Layer</t>
+  </si>
+  <si>
+    <t>contains any business logic such as validations, defines the scope of business transactions</t>
+  </si>
+  <si>
+    <t>Create resource controller (@Controller)</t>
+  </si>
+  <si>
+    <t>Create the service classes (@Service)</t>
+  </si>
+  <si>
+    <t>The DAO classes map the database to/from in-memory domain objects</t>
+  </si>
+  <si>
+    <t>Persistence Layer</t>
+  </si>
+  <si>
+    <t>Create the persistence class (@Repository). DAO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   '- HashMap has a inner class called Entry which stores key-value pairs.
+    - Above Entry object is stored in Entry[ ](Array) called table
+    - An index of table is logically known as bucket and it stores first element of linkedlist
+    - Key object’s hashcode() is used to find bucket of that Entry object.
+    - If two key object ‘s have same hashcode , they will go in same bucket of table array.
+    - Key object ‘s equals() method is used to ensure uniqueness of key object.
+    - Value object  ‘s equals() and hashcode() method is not used at all</t>
+  </si>
+  <si>
+    <t>hashcode() and equals() method in java</t>
+  </si>
+  <si>
+    <t>equals():</t>
+  </si>
+  <si>
+    <t>hashcode():</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - This method is used to simply check the equality between two objects.
+ - By default, it checks where two reference refer to same object or not(==).</t>
+  </si>
+  <si>
+    <t>How HashMap works in java</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - This method is used to get unique integer for given object. 
+ - This integer is used to find bucket when storing in hashmap or hashset.
+ - By default, This method returns integer represention of memory address where object is stored.</t>
   </si>
 </sst>
 </file>
@@ -7884,7 +7982,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -8015,11 +8113,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -8184,6 +8300,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -8211,6 +8333,16 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -8231,13 +8363,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>47624</xdr:colOff>
-      <xdr:row>86</xdr:row>
+      <xdr:row>92</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>85724</xdr:colOff>
-      <xdr:row>96</xdr:row>
+      <xdr:row>102</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -9074,10 +9206,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:E145"/>
+  <dimension ref="B2:E151"/>
   <sheetViews>
-    <sheetView topLeftCell="A130" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25:E25"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="E71" sqref="E71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9169,7 +9301,7 @@
     </row>
     <row r="10" spans="2:5" ht="31.5">
       <c r="B10" s="22" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C10" s="23"/>
       <c r="D10" s="23"/>
@@ -9191,100 +9323,100 @@
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="E12" s="29" t="s">
         <v>214</v>
-      </c>
-      <c r="E12" s="29" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="13" spans="2:5">
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="31" t="s">
+        <v>215</v>
+      </c>
+      <c r="E13" s="31" t="s">
         <v>216</v>
-      </c>
-      <c r="E13" s="31" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="14" spans="2:5">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="E14" s="29" t="s">
         <v>218</v>
-      </c>
-      <c r="E14" s="29" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="15" spans="2:5" ht="30">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="E15" s="29" t="s">
         <v>220</v>
-      </c>
-      <c r="E15" s="29" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="16" spans="2:5">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="E16" s="29" t="s">
         <v>222</v>
-      </c>
-      <c r="E16" s="29" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="17" spans="2:5">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="E17" s="29" t="s">
         <v>224</v>
-      </c>
-      <c r="E17" s="29" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="18" spans="2:5">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="E18" s="29" t="s">
         <v>226</v>
       </c>
-      <c r="E18" s="29" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" ht="63.75">
+    </row>
+    <row r="19" spans="2:5" ht="74.25" customHeight="1">
       <c r="B19" s="2"/>
       <c r="C19" s="32"/>
       <c r="D19" s="33" t="s">
+        <v>227</v>
+      </c>
+      <c r="E19" s="30" t="s">
         <v>228</v>
-      </c>
-      <c r="E19" s="30" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="20" spans="2:5" ht="78.75">
       <c r="B20" s="2"/>
       <c r="C20" s="32"/>
       <c r="D20" s="33" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E20" s="30" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="21" spans="2:5" ht="93.75">
       <c r="B21" s="2"/>
       <c r="C21" s="32"/>
       <c r="D21" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="E21" s="30" t="s">
         <v>231</v>
-      </c>
-      <c r="E21" s="30" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="22" spans="2:5">
@@ -9328,10 +9460,10 @@
     <row r="27" spans="2:5">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
-      <c r="D27" s="72" t="s">
+      <c r="D27" s="74" t="s">
         <v>47</v>
       </c>
-      <c r="E27" s="73"/>
+      <c r="E27" s="75"/>
     </row>
     <row r="28" spans="2:5">
       <c r="B28" s="2"/>
@@ -9394,10 +9526,10 @@
     <row r="34" spans="2:5">
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
-      <c r="D34" s="76" t="s">
+      <c r="D34" s="78" t="s">
         <v>81</v>
       </c>
-      <c r="E34" s="76"/>
+      <c r="E34" s="78"/>
     </row>
     <row r="35" spans="2:5">
       <c r="B35" s="2"/>
@@ -9470,10 +9602,10 @@
     <row r="42" spans="2:5">
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
-      <c r="D42" s="77" t="s">
+      <c r="D42" s="79" t="s">
         <v>94</v>
       </c>
-      <c r="E42" s="78"/>
+      <c r="E42" s="80"/>
     </row>
     <row r="43" spans="2:5">
       <c r="B43" s="2"/>
@@ -9560,10 +9692,10 @@
     <row r="51" spans="2:5">
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
-      <c r="D51" s="74" t="s">
+      <c r="D51" s="76" t="s">
         <v>60</v>
       </c>
-      <c r="E51" s="74"/>
+      <c r="E51" s="76"/>
     </row>
     <row r="52" spans="2:5">
       <c r="B52" s="2"/>
@@ -9621,7 +9753,7 @@
       <c r="D57" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="E57" s="75" t="s">
+      <c r="E57" s="77" t="s">
         <v>73</v>
       </c>
     </row>
@@ -9631,7 +9763,7 @@
       <c r="D58" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="E58" s="75"/>
+      <c r="E58" s="77"/>
     </row>
     <row r="59" spans="2:5">
       <c r="B59" s="2"/>
@@ -9666,562 +9798,564 @@
     <row r="62" spans="2:5">
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
-      <c r="D62" s="2"/>
-      <c r="E62" s="2"/>
-    </row>
-    <row r="64" spans="2:5" ht="31.5">
-      <c r="B64" s="22" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="65" spans="2:5" ht="60">
+      <c r="D62" s="73"/>
+      <c r="E62" s="73"/>
+    </row>
+    <row r="63" spans="2:5" ht="18.75">
+      <c r="B63" s="2"/>
+      <c r="C63" s="2"/>
+      <c r="D63" s="18" t="s">
+        <v>423</v>
+      </c>
+      <c r="E63" s="73"/>
+    </row>
+    <row r="64" spans="2:5" ht="18" customHeight="1">
+      <c r="B64" s="2"/>
+      <c r="C64" s="2"/>
+      <c r="D64" s="69" t="s">
+        <v>425</v>
+      </c>
+      <c r="E64" s="69" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="65" spans="2:5" ht="62.25" customHeight="1">
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
-      <c r="D65" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="E65" s="25" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="66" spans="2:5" ht="45">
+      <c r="D65" s="13" t="s">
+        <v>428</v>
+      </c>
+      <c r="E65" s="86" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="66" spans="2:5">
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
-      <c r="D66" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="E66" s="17" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="67" spans="2:5" ht="60">
+      <c r="D66" s="13"/>
+      <c r="E66" s="13"/>
+    </row>
+    <row r="67" spans="2:5" ht="31.5">
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
-      <c r="D67" t="s">
-        <v>114</v>
-      </c>
-      <c r="E67" s="13" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="68" spans="2:5" ht="45">
+      <c r="D67" s="22" t="s">
+        <v>427</v>
+      </c>
+      <c r="E67" s="73"/>
+    </row>
+    <row r="68" spans="2:5" ht="150">
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
-      <c r="D68" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="E68" s="17" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="69" spans="2:5" ht="45">
-      <c r="B69" s="2"/>
-      <c r="C69" s="2"/>
-      <c r="D69" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="E69" s="17" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="70" spans="2:5" ht="30">
-      <c r="B70" s="2"/>
-      <c r="C70" s="2"/>
-      <c r="D70" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="E70" s="17" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="71" spans="2:5" ht="30">
+      <c r="D68" s="73" t="s">
+        <v>422</v>
+      </c>
+      <c r="E68" s="2"/>
+    </row>
+    <row r="70" spans="2:5" ht="31.5">
+      <c r="B70" s="22" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="71" spans="2:5" ht="60">
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
       <c r="D71" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="E71" s="17" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="72" spans="2:5" ht="120">
+        <v>111</v>
+      </c>
+      <c r="E71" s="25" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="72" spans="2:5" ht="45">
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
       <c r="D72" s="2" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="E72" s="17" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
     </row>
     <row r="73" spans="2:5" ht="60">
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
-      <c r="D73" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="E73" s="17" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="75" spans="2:5" ht="31.5">
-      <c r="B75" s="22" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="76" spans="2:5" ht="225">
+      <c r="D73" t="s">
+        <v>114</v>
+      </c>
+      <c r="E73" s="13" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="74" spans="2:5" ht="45">
+      <c r="B74" s="2"/>
+      <c r="C74" s="2"/>
+      <c r="D74" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E74" s="17" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="75" spans="2:5" ht="45">
+      <c r="B75" s="2"/>
+      <c r="C75" s="2"/>
+      <c r="D75" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E75" s="17" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="76" spans="2:5" ht="30">
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
       <c r="D76" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="E76" s="21" t="s">
-        <v>150</v>
+        <v>117</v>
+      </c>
+      <c r="E76" s="17" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="77" spans="2:5" ht="30">
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
       <c r="D77" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="E77" s="17" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="78" spans="2:5" ht="90">
+        <v>123</v>
+      </c>
+      <c r="E77" s="72" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="78" spans="2:5" ht="120">
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
       <c r="D78" s="2" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="E78" s="17" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="79" spans="2:5" ht="45">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="79" spans="2:5" ht="60">
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
       <c r="D79" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="E79" s="21" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="80" spans="2:5" ht="60">
-      <c r="B80" s="2"/>
-      <c r="C80" s="2"/>
-      <c r="D80" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="E80" s="21" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="81" spans="2:5" ht="90">
-      <c r="B81" s="2"/>
-      <c r="C81" s="2"/>
-      <c r="D81" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="E81" s="21" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="82" spans="2:5" ht="30">
+        <v>126</v>
+      </c>
+      <c r="E79" s="17" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="81" spans="2:5" ht="31.5">
+      <c r="B81" s="22" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="82" spans="2:5" ht="225">
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
       <c r="D82" s="2" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="E82" s="21" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
     </row>
     <row r="83" spans="2:5" ht="30">
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
       <c r="D83" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="E83" s="21" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="84" spans="2:5" ht="60">
+        <v>130</v>
+      </c>
+      <c r="E83" s="17" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="84" spans="2:5" ht="90">
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
       <c r="D84" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="E84" s="21" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="85" spans="2:5" ht="90">
+        <v>129</v>
+      </c>
+      <c r="E84" s="17" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="85" spans="2:5" ht="45">
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
       <c r="D85" s="2" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
       <c r="E85" s="21" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
     </row>
     <row r="86" spans="2:5" ht="60">
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
       <c r="D86" s="2" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
       <c r="E86" s="21" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="87" spans="2:5">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="87" spans="2:5" ht="90">
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
-      <c r="D87" s="2"/>
-      <c r="E87" s="21"/>
-    </row>
-    <row r="88" spans="2:5">
+      <c r="D87" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="E87" s="21" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="88" spans="2:5" ht="30">
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
-      <c r="D88" s="2"/>
-      <c r="E88" s="21"/>
-    </row>
-    <row r="89" spans="2:5">
+      <c r="D88" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E88" s="21" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="89" spans="2:5" ht="30">
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
-      <c r="D89" s="2"/>
-      <c r="E89" s="21"/>
-    </row>
-    <row r="90" spans="2:5">
+      <c r="D89" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="E89" s="21" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="90" spans="2:5" ht="60">
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
-      <c r="D90" s="2"/>
-      <c r="E90" s="21"/>
-    </row>
-    <row r="91" spans="2:5">
+      <c r="D90" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E90" s="21" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="91" spans="2:5" ht="90">
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
-      <c r="D91" s="2"/>
-      <c r="E91" s="21"/>
-    </row>
-    <row r="92" spans="2:5">
+      <c r="D91" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="E91" s="21" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="92" spans="2:5" ht="60">
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
-      <c r="D92" s="2"/>
-      <c r="E92" s="21"/>
+      <c r="D92" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E92" s="21" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="93" spans="2:5">
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
       <c r="D93" s="2"/>
-      <c r="E93" s="26"/>
+      <c r="E93" s="21"/>
     </row>
     <row r="94" spans="2:5">
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
       <c r="D94" s="2"/>
-      <c r="E94" s="2"/>
+      <c r="E94" s="21"/>
     </row>
     <row r="95" spans="2:5">
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
       <c r="D95" s="2"/>
-      <c r="E95" s="2"/>
+      <c r="E95" s="21"/>
     </row>
     <row r="96" spans="2:5">
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
       <c r="D96" s="2"/>
-      <c r="E96" s="2"/>
+      <c r="E96" s="21"/>
     </row>
     <row r="97" spans="2:5">
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
       <c r="D97" s="2"/>
-      <c r="E97" s="2"/>
-    </row>
-    <row r="98" spans="2:5" ht="60">
+      <c r="E97" s="21"/>
+    </row>
+    <row r="98" spans="2:5">
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
-      <c r="D98" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="E98" s="26" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="99" spans="2:5" ht="75">
+      <c r="D98" s="2"/>
+      <c r="E98" s="21"/>
+    </row>
+    <row r="99" spans="2:5">
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
-      <c r="D99" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="E99" s="26" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="100" spans="2:5" ht="60">
+      <c r="D99" s="2"/>
+      <c r="E99" s="26"/>
+    </row>
+    <row r="100" spans="2:5">
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
-      <c r="D100" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="E100" s="26" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="101" spans="2:5" ht="45">
+      <c r="D100" s="2"/>
+      <c r="E100" s="2"/>
+    </row>
+    <row r="101" spans="2:5">
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
-      <c r="D101" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="E101" s="26" t="s">
-        <v>168</v>
-      </c>
+      <c r="D101" s="2"/>
+      <c r="E101" s="2"/>
     </row>
     <row r="102" spans="2:5">
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
-      <c r="D102" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="E102" s="26" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="103" spans="2:5" ht="75">
+      <c r="D102" s="2"/>
+      <c r="E102" s="2"/>
+    </row>
+    <row r="103" spans="2:5">
       <c r="B103" s="2"/>
       <c r="C103" s="2"/>
-      <c r="D103" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="E103" s="26" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="104" spans="2:5" ht="135">
+      <c r="D103" s="2"/>
+      <c r="E103" s="2"/>
+    </row>
+    <row r="104" spans="2:5" ht="60">
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
       <c r="D104" s="2" t="s">
-        <v>173</v>
+        <v>158</v>
       </c>
       <c r="E104" s="26" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="105" spans="2:5" ht="90">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="105" spans="2:5" ht="75">
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
       <c r="D105" s="2" t="s">
-        <v>175</v>
+        <v>160</v>
       </c>
       <c r="E105" s="26" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="106" spans="2:5" ht="45">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="106" spans="2:5" ht="60">
       <c r="B106" s="2"/>
       <c r="C106" s="2"/>
       <c r="D106" s="2" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="E106" s="26" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="107" spans="2:5">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="107" spans="2:5" ht="45">
       <c r="B107" s="2"/>
       <c r="C107" s="2"/>
       <c r="D107" s="2" t="s">
-        <v>179</v>
+        <v>166</v>
       </c>
       <c r="E107" s="26" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="108" spans="2:5" ht="30">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="108" spans="2:5">
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
-      <c r="D108" s="26" t="s">
-        <v>181</v>
+      <c r="D108" s="2" t="s">
+        <v>168</v>
       </c>
       <c r="E108" s="26" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="109" spans="2:5">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="109" spans="2:5" ht="75">
       <c r="B109" s="2"/>
       <c r="C109" s="2"/>
       <c r="D109" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="E109" s="26"/>
-    </row>
-    <row r="110" spans="2:5">
+        <v>170</v>
+      </c>
+      <c r="E109" s="26" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="110" spans="2:5" ht="135">
       <c r="B110" s="2"/>
       <c r="C110" s="2"/>
-      <c r="D110" s="15" t="s">
-        <v>184</v>
-      </c>
-      <c r="E110" s="15" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="111" spans="2:5">
+      <c r="D110" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E110" s="26" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="111" spans="2:5" ht="90">
       <c r="B111" s="2"/>
       <c r="C111" s="2"/>
-      <c r="D111" s="26" t="s">
-        <v>186</v>
+      <c r="D111" s="2" t="s">
+        <v>174</v>
       </c>
       <c r="E111" s="26" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="112" spans="2:5">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="112" spans="2:5" ht="45">
       <c r="B112" s="2"/>
       <c r="C112" s="2"/>
-      <c r="D112" s="26" t="s">
-        <v>188</v>
+      <c r="D112" s="2" t="s">
+        <v>176</v>
       </c>
       <c r="E112" s="26" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
     </row>
     <row r="113" spans="2:5">
       <c r="B113" s="2"/>
       <c r="C113" s="2"/>
-      <c r="D113" s="26" t="s">
-        <v>190</v>
+      <c r="D113" s="2" t="s">
+        <v>178</v>
       </c>
       <c r="E113" s="26" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="114" spans="2:5">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="114" spans="2:5" ht="30">
       <c r="B114" s="2"/>
       <c r="C114" s="2"/>
       <c r="D114" s="26" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="E114" s="26" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="115" spans="2:5" ht="31.5">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="115" spans="2:5">
       <c r="B115" s="2"/>
-      <c r="C115" s="22" t="s">
-        <v>194</v>
-      </c>
-      <c r="D115" s="2"/>
+      <c r="C115" s="2"/>
+      <c r="D115" s="2" t="s">
+        <v>182</v>
+      </c>
       <c r="E115" s="26"/>
     </row>
-    <row r="116" spans="2:5" ht="105">
+    <row r="116" spans="2:5">
       <c r="B116" s="2"/>
       <c r="C116" s="2"/>
-      <c r="D116" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="E116" s="28" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="117" spans="2:5" ht="120">
+      <c r="D116" s="15" t="s">
+        <v>183</v>
+      </c>
+      <c r="E116" s="15" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="117" spans="2:5">
       <c r="B117" s="2"/>
       <c r="C117" s="2"/>
-      <c r="D117" s="2" t="s">
-        <v>196</v>
+      <c r="D117" s="26" t="s">
+        <v>185</v>
       </c>
       <c r="E117" s="26" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="118" spans="2:5" ht="255">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="118" spans="2:5">
       <c r="B118" s="2"/>
       <c r="C118" s="2"/>
-      <c r="D118" s="2" t="s">
-        <v>197</v>
+      <c r="D118" s="26" t="s">
+        <v>187</v>
       </c>
       <c r="E118" s="26" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="119" spans="2:5" ht="180">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="119" spans="2:5">
       <c r="B119" s="2"/>
       <c r="C119" s="2"/>
-      <c r="D119" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="E119" s="28" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="120" spans="2:5" ht="30">
+      <c r="D119" s="26" t="s">
+        <v>189</v>
+      </c>
+      <c r="E119" s="26" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="120" spans="2:5">
       <c r="B120" s="2"/>
       <c r="C120" s="2"/>
-      <c r="D120" s="28" t="s">
-        <v>205</v>
-      </c>
-      <c r="E120" s="28"/>
-    </row>
-    <row r="121" spans="2:5" ht="30">
+      <c r="D120" s="26" t="s">
+        <v>191</v>
+      </c>
+      <c r="E120" s="26" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="121" spans="2:5" ht="31.5">
       <c r="B121" s="2"/>
-      <c r="C121" s="2"/>
-      <c r="D121" s="28" t="s">
-        <v>206</v>
-      </c>
-      <c r="E121" s="28"/>
-    </row>
-    <row r="122" spans="2:5" ht="30">
+      <c r="C121" s="22" t="s">
+        <v>193</v>
+      </c>
+      <c r="D121" s="2"/>
+      <c r="E121" s="26"/>
+    </row>
+    <row r="122" spans="2:5" ht="105">
       <c r="B122" s="2"/>
       <c r="C122" s="2"/>
-      <c r="D122" s="28" t="s">
-        <v>208</v>
-      </c>
-      <c r="E122" s="28"/>
-    </row>
-    <row r="123" spans="2:5" ht="45">
+      <c r="D122" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="E122" s="28" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="123" spans="2:5" ht="120">
       <c r="B123" s="2"/>
       <c r="C123" s="2"/>
-      <c r="D123" s="28" t="s">
-        <v>202</v>
-      </c>
-      <c r="E123" s="28"/>
-    </row>
-    <row r="124" spans="2:5">
+      <c r="D123" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="E123" s="26" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="124" spans="2:5" ht="255">
       <c r="B124" s="2"/>
       <c r="C124" s="2"/>
-      <c r="D124" s="28" t="s">
-        <v>209</v>
-      </c>
-      <c r="E124" s="28"/>
-    </row>
-    <row r="125" spans="2:5" ht="60">
+      <c r="D124" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="E124" s="26" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="125" spans="2:5" ht="180">
       <c r="B125" s="2"/>
       <c r="C125" s="2"/>
-      <c r="D125" s="28" t="s">
-        <v>210</v>
-      </c>
-      <c r="E125" s="28"/>
+      <c r="D125" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="E125" s="28" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="126" spans="2:5" ht="30">
       <c r="B126" s="2"/>
       <c r="C126" s="2"/>
       <c r="D126" s="28" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="E126" s="28"/>
     </row>
-    <row r="127" spans="2:5">
+    <row r="127" spans="2:5" ht="30">
       <c r="B127" s="2"/>
       <c r="C127" s="2"/>
       <c r="D127" s="28" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="E127" s="28"/>
     </row>
@@ -10229,104 +10363,116 @@
       <c r="B128" s="2"/>
       <c r="C128" s="2"/>
       <c r="D128" s="28" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="E128" s="28"/>
     </row>
-    <row r="129" spans="2:5" ht="30">
+    <row r="129" spans="2:5" ht="45">
       <c r="B129" s="2"/>
       <c r="C129" s="2"/>
       <c r="D129" s="28" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E129" s="28"/>
     </row>
     <row r="130" spans="2:5">
       <c r="B130" s="2"/>
       <c r="C130" s="2"/>
-      <c r="D130" s="28"/>
-      <c r="E130" s="26"/>
-    </row>
-    <row r="132" spans="2:5" ht="31.5">
-      <c r="C132" s="22" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="133" spans="2:5" ht="90">
+      <c r="D130" s="28" t="s">
+        <v>208</v>
+      </c>
+      <c r="E130" s="28"/>
+    </row>
+    <row r="131" spans="2:5" ht="60">
+      <c r="B131" s="2"/>
+      <c r="C131" s="2"/>
+      <c r="D131" s="28" t="s">
+        <v>209</v>
+      </c>
+      <c r="E131" s="28"/>
+    </row>
+    <row r="132" spans="2:5" ht="30">
+      <c r="B132" s="2"/>
+      <c r="C132" s="2"/>
+      <c r="D132" s="28" t="s">
+        <v>210</v>
+      </c>
+      <c r="E132" s="28"/>
+    </row>
+    <row r="133" spans="2:5">
       <c r="B133" s="2"/>
       <c r="C133" s="2"/>
-      <c r="D133" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E133" s="21" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="134" spans="2:5" ht="90">
+      <c r="D133" s="28" t="s">
+        <v>211</v>
+      </c>
+      <c r="E133" s="28"/>
+    </row>
+    <row r="134" spans="2:5" ht="30">
       <c r="B134" s="2"/>
       <c r="C134" s="2"/>
       <c r="D134" s="28" t="s">
-        <v>155</v>
-      </c>
-      <c r="E134" s="21" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="135" spans="2:5" ht="105">
+        <v>202</v>
+      </c>
+      <c r="E134" s="28"/>
+    </row>
+    <row r="135" spans="2:5" ht="30">
       <c r="B135" s="2"/>
       <c r="C135" s="2"/>
-      <c r="D135" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="E135" s="21" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="136" spans="2:5" ht="90">
+      <c r="D135" s="28" t="s">
+        <v>203</v>
+      </c>
+      <c r="E135" s="28"/>
+    </row>
+    <row r="136" spans="2:5">
       <c r="B136" s="2"/>
       <c r="C136" s="2"/>
-      <c r="D136" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="E136" s="21" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="137" spans="2:5">
-      <c r="B137" s="2"/>
-      <c r="C137" s="2"/>
-      <c r="D137" s="2"/>
-      <c r="E137" s="21"/>
-    </row>
-    <row r="138" spans="2:5">
-      <c r="B138" s="2"/>
-      <c r="C138" s="2"/>
-      <c r="D138" s="2"/>
-      <c r="E138" s="21"/>
-    </row>
-    <row r="139" spans="2:5">
+      <c r="D136" s="28"/>
+      <c r="E136" s="26"/>
+    </row>
+    <row r="138" spans="2:5" ht="31.5">
+      <c r="C138" s="22" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="139" spans="2:5" ht="90">
       <c r="B139" s="2"/>
       <c r="C139" s="2"/>
-      <c r="D139" s="2"/>
-      <c r="E139" s="21"/>
-    </row>
-    <row r="140" spans="2:5">
+      <c r="D139" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E139" s="21" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="140" spans="2:5" ht="90">
       <c r="B140" s="2"/>
       <c r="C140" s="2"/>
-      <c r="D140" s="2"/>
-      <c r="E140" s="21"/>
-    </row>
-    <row r="141" spans="2:5">
+      <c r="D140" s="28" t="s">
+        <v>154</v>
+      </c>
+      <c r="E140" s="21" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="141" spans="2:5" ht="105">
       <c r="B141" s="2"/>
       <c r="C141" s="2"/>
-      <c r="D141" s="2"/>
-      <c r="E141" s="21"/>
-    </row>
-    <row r="142" spans="2:5">
+      <c r="D141" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="E141" s="21" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="142" spans="2:5" ht="90">
       <c r="B142" s="2"/>
       <c r="C142" s="2"/>
-      <c r="D142" s="2"/>
-      <c r="E142" s="21"/>
+      <c r="D142" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E142" s="21" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="143" spans="2:5">
       <c r="B143" s="2"/>
@@ -10340,8 +10486,44 @@
       <c r="D144" s="2"/>
       <c r="E144" s="21"/>
     </row>
-    <row r="145" spans="5:5">
-      <c r="E145" s="27"/>
+    <row r="145" spans="2:5">
+      <c r="B145" s="2"/>
+      <c r="C145" s="2"/>
+      <c r="D145" s="2"/>
+      <c r="E145" s="21"/>
+    </row>
+    <row r="146" spans="2:5">
+      <c r="B146" s="2"/>
+      <c r="C146" s="2"/>
+      <c r="D146" s="2"/>
+      <c r="E146" s="21"/>
+    </row>
+    <row r="147" spans="2:5">
+      <c r="B147" s="2"/>
+      <c r="C147" s="2"/>
+      <c r="D147" s="2"/>
+      <c r="E147" s="21"/>
+    </row>
+    <row r="148" spans="2:5">
+      <c r="B148" s="2"/>
+      <c r="C148" s="2"/>
+      <c r="D148" s="2"/>
+      <c r="E148" s="21"/>
+    </row>
+    <row r="149" spans="2:5">
+      <c r="B149" s="2"/>
+      <c r="C149" s="2"/>
+      <c r="D149" s="2"/>
+      <c r="E149" s="21"/>
+    </row>
+    <row r="150" spans="2:5">
+      <c r="B150" s="2"/>
+      <c r="C150" s="2"/>
+      <c r="D150" s="2"/>
+      <c r="E150" s="21"/>
+    </row>
+    <row r="151" spans="2:5">
+      <c r="E151" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -10351,9 +10533,12 @@
     <mergeCell ref="D34:E34"/>
     <mergeCell ref="D42:E42"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="D63" r:id="rId1" display="http://www.java2blog.com/2014/02/hashcode-and-equals-method-in-java.html"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -10362,7 +10547,7 @@
   <dimension ref="B3:C13"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10381,62 +10566,62 @@
     </row>
     <row r="4" spans="2:3" ht="45">
       <c r="B4" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="5" spans="2:3">
       <c r="B5" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C5" s="30" t="s">
         <v>233</v>
-      </c>
-      <c r="C5" s="30" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="30" customHeight="1">
       <c r="B6" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C6" s="2"/>
     </row>
     <row r="7" spans="2:3" ht="315">
       <c r="B7" s="30" t="s">
+        <v>235</v>
+      </c>
+      <c r="C7" s="30" t="s">
         <v>236</v>
-      </c>
-      <c r="C7" s="30" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="105">
       <c r="B8" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="C8" s="30" t="s">
         <v>238</v>
-      </c>
-      <c r="C8" s="30" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="9" spans="2:3" ht="60">
       <c r="B9" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="C9" s="34" t="s">
         <v>240</v>
-      </c>
-      <c r="C9" s="34" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="10" spans="2:3" ht="165">
       <c r="B10" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="C10" s="30" t="s">
         <v>242</v>
-      </c>
-      <c r="C10" s="30" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="11" spans="2:3" ht="105">
       <c r="B11" s="2"/>
       <c r="C11" s="30" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="12" spans="2:3">
@@ -10455,76 +10640,76 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A3:C86"/>
+  <dimension ref="A3:C101"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="B102" sqref="B102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
     <col min="2" max="2" width="67.85546875" customWidth="1"/>
     <col min="3" max="3" width="88" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:3" ht="90.75">
       <c r="B3" s="35" t="s">
+        <v>244</v>
+      </c>
+      <c r="C3" s="30" t="s">
         <v>245</v>
-      </c>
-      <c r="C3" s="30" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="23.25">
       <c r="B4" s="36" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C4" s="2"/>
     </row>
     <row r="5" spans="2:3" ht="45">
       <c r="B5" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="C5" s="30" t="s">
         <v>250</v>
-      </c>
-      <c r="C5" s="30" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="135">
       <c r="B6" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="C6" s="30" t="s">
         <v>252</v>
-      </c>
-      <c r="C6" s="30" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="315">
       <c r="B7" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="C7" s="30" t="s">
         <v>254</v>
-      </c>
-      <c r="C7" s="30" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="60">
       <c r="B8" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="C8" s="30" t="s">
         <v>256</v>
-      </c>
-      <c r="C8" s="30" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="9" spans="2:3" ht="31.5">
       <c r="B9" s="36" t="s">
+        <v>257</v>
+      </c>
+      <c r="C9" s="30" t="s">
         <v>258</v>
-      </c>
-      <c r="C9" s="30" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="10" spans="2:3" ht="31.5">
       <c r="B10" s="32" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C10" s="2"/>
     </row>
@@ -10634,142 +10819,142 @@
     </row>
     <row r="37" spans="1:3" ht="90">
       <c r="B37" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="C37" s="37" t="s">
         <v>262</v>
-      </c>
-      <c r="C37" s="37" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="B38" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C38" s="37"/>
     </row>
     <row r="40" spans="1:3">
       <c r="B40" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C40" s="2"/>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="55"/>
       <c r="B41" s="15" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C41" s="15" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="30">
       <c r="A42" s="53" t="s">
+        <v>326</v>
+      </c>
+      <c r="B42" s="53" t="s">
         <v>327</v>
       </c>
-      <c r="B42" s="53" t="s">
+      <c r="C42" s="53" t="s">
         <v>328</v>
-      </c>
-      <c r="C42" s="53" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="53" t="s">
+        <v>329</v>
+      </c>
+      <c r="B43" s="53" t="s">
         <v>330</v>
       </c>
-      <c r="B43" s="53" t="s">
+      <c r="C43" s="53" t="s">
         <v>331</v>
-      </c>
-      <c r="C43" s="53" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="53" t="s">
+        <v>332</v>
+      </c>
+      <c r="B44" s="53" t="s">
         <v>333</v>
       </c>
-      <c r="B44" s="53" t="s">
+      <c r="C44" s="53" t="s">
         <v>334</v>
-      </c>
-      <c r="C44" s="53" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="30">
       <c r="A45" s="53" t="s">
+        <v>335</v>
+      </c>
+      <c r="B45" s="53" t="s">
         <v>336</v>
       </c>
-      <c r="B45" s="53" t="s">
+      <c r="C45" s="53" t="s">
         <v>337</v>
-      </c>
-      <c r="C45" s="53" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="53" t="s">
+        <v>338</v>
+      </c>
+      <c r="B46" s="53" t="s">
         <v>339</v>
       </c>
-      <c r="B46" s="53" t="s">
+      <c r="C46" s="53" t="s">
         <v>340</v>
-      </c>
-      <c r="C46" s="53" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="30">
       <c r="A47" s="53" t="s">
+        <v>341</v>
+      </c>
+      <c r="B47" s="53" t="s">
         <v>342</v>
       </c>
-      <c r="B47" s="53" t="s">
+      <c r="C47" s="53" t="s">
         <v>343</v>
-      </c>
-      <c r="C47" s="53" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="30">
       <c r="A48" s="53" t="s">
+        <v>344</v>
+      </c>
+      <c r="B48" s="53" t="s">
         <v>345</v>
       </c>
-      <c r="B48" s="53" t="s">
+      <c r="C48" s="53" t="s">
         <v>346</v>
       </c>
-      <c r="C48" s="53" t="s">
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="77" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="49" spans="1:3">
-      <c r="A49" s="75" t="s">
+      <c r="B49" s="53" t="s">
         <v>348</v>
       </c>
-      <c r="B49" s="53" t="s">
+      <c r="C49" s="77" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="77"/>
+      <c r="B50" s="53"/>
+      <c r="C50" s="77"/>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="77"/>
+      <c r="B51" s="53" t="s">
         <v>349</v>
       </c>
-      <c r="C49" s="75" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3">
-      <c r="A50" s="75"/>
-      <c r="B50" s="53"/>
-      <c r="C50" s="75"/>
-    </row>
-    <row r="51" spans="1:3">
-      <c r="A51" s="75"/>
-      <c r="B51" s="53" t="s">
-        <v>350</v>
-      </c>
-      <c r="C51" s="75"/>
+      <c r="C51" s="77"/>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="53" t="s">
+        <v>351</v>
+      </c>
+      <c r="B52" s="53" t="s">
         <v>352</v>
       </c>
-      <c r="B52" s="53" t="s">
+      <c r="C52" s="53" t="s">
         <v>353</v>
-      </c>
-      <c r="C52" s="53" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -10777,38 +10962,38 @@
     </row>
     <row r="54" spans="1:3" ht="31.5">
       <c r="B54" s="22" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="B55" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="B56" s="58"/>
     </row>
     <row r="57" spans="1:3" ht="32.25" customHeight="1">
-      <c r="B57" s="79" t="s">
+      <c r="B57" s="81" t="s">
+        <v>356</v>
+      </c>
+      <c r="C57" s="81"/>
+    </row>
+    <row r="58" spans="1:3" ht="33" customHeight="1">
+      <c r="B58" s="81" t="s">
         <v>357</v>
       </c>
-      <c r="C57" s="79"/>
-    </row>
-    <row r="58" spans="1:3" ht="33" customHeight="1">
-      <c r="B58" s="79" t="s">
+      <c r="C58" s="81"/>
+    </row>
+    <row r="59" spans="1:3" ht="19.5" customHeight="1">
+      <c r="B59" s="81" t="s">
         <v>358</v>
       </c>
-      <c r="C58" s="79"/>
-    </row>
-    <row r="59" spans="1:3" ht="19.5" customHeight="1">
-      <c r="B59" s="79" t="s">
-        <v>359</v>
-      </c>
-      <c r="C59" s="79"/>
+      <c r="C59" s="81"/>
     </row>
     <row r="60" spans="1:3">
       <c r="B60" s="2" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C60" s="2"/>
     </row>
@@ -10818,157 +11003,157 @@
     </row>
     <row r="62" spans="1:3">
       <c r="B62" s="60" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C62" s="2"/>
     </row>
     <row r="63" spans="1:3" ht="30">
       <c r="B63" s="61" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C63" s="2"/>
     </row>
     <row r="64" spans="1:3">
       <c r="B64" s="60" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C64" s="2"/>
     </row>
     <row r="65" spans="2:3" ht="225">
       <c r="B65" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="C65" s="54" t="s">
         <v>364</v>
-      </c>
-      <c r="C65" s="54" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="66" spans="2:3" ht="30">
       <c r="B66" s="37" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C66" s="37"/>
     </row>
     <row r="67" spans="2:3" ht="30.75">
       <c r="B67" s="63" t="s">
+        <v>365</v>
+      </c>
+      <c r="C67" s="54" t="s">
         <v>366</v>
-      </c>
-      <c r="C67" s="54" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="68" spans="2:3" ht="137.25" customHeight="1">
       <c r="B68" s="64" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C68" s="16" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="69" spans="2:3" ht="105.75">
       <c r="B69" s="63" t="s">
+        <v>368</v>
+      </c>
+      <c r="C69" s="54" t="s">
         <v>369</v>
-      </c>
-      <c r="C69" s="54" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="70" spans="2:3" ht="53.25" customHeight="1">
       <c r="B70" s="65" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C70" s="62" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="71" spans="2:3" ht="32.25" customHeight="1">
       <c r="B71" s="63" t="s">
+        <v>372</v>
+      </c>
+      <c r="C71" s="62" t="s">
         <v>373</v>
-      </c>
-      <c r="C71" s="62" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="72" spans="2:3" ht="135">
       <c r="B72" s="63" t="s">
+        <v>375</v>
+      </c>
+      <c r="C72" s="66" t="s">
         <v>376</v>
-      </c>
-      <c r="C72" s="66" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="73" spans="2:3" ht="30.75">
       <c r="B73" s="63" t="s">
+        <v>377</v>
+      </c>
+      <c r="C73" s="54" t="s">
         <v>378</v>
-      </c>
-      <c r="C73" s="54" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="74" spans="2:3">
       <c r="B74" s="67" t="s">
+        <v>379</v>
+      </c>
+      <c r="C74" s="67" t="s">
         <v>380</v>
-      </c>
-      <c r="C74" s="67" t="s">
-        <v>381</v>
       </c>
     </row>
     <row r="75" spans="2:3" ht="30">
       <c r="B75" s="67" t="s">
+        <v>381</v>
+      </c>
+      <c r="C75" s="54" t="s">
         <v>382</v>
-      </c>
-      <c r="C75" s="54" t="s">
-        <v>383</v>
       </c>
     </row>
     <row r="76" spans="2:3" ht="33.75" customHeight="1">
       <c r="B76" s="67" t="s">
+        <v>383</v>
+      </c>
+      <c r="C76" s="54" t="s">
         <v>384</v>
-      </c>
-      <c r="C76" s="54" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="77" spans="2:3" ht="30">
       <c r="B77" s="67" t="s">
+        <v>385</v>
+      </c>
+      <c r="C77" s="54" t="s">
         <v>386</v>
-      </c>
-      <c r="C77" s="54" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="78" spans="2:3" ht="30.75">
       <c r="B78" s="67" t="s">
+        <v>387</v>
+      </c>
+      <c r="C78" s="54" t="s">
         <v>388</v>
-      </c>
-      <c r="C78" s="54" t="s">
-        <v>389</v>
       </c>
     </row>
     <row r="79" spans="2:3" ht="30">
       <c r="B79" s="67" t="s">
+        <v>389</v>
+      </c>
+      <c r="C79" s="54" t="s">
         <v>390</v>
-      </c>
-      <c r="C79" s="54" t="s">
-        <v>391</v>
       </c>
     </row>
     <row r="80" spans="2:3">
       <c r="B80" s="67" t="s">
+        <v>391</v>
+      </c>
+      <c r="C80" s="54" t="s">
         <v>392</v>
-      </c>
-      <c r="C80" s="54" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" s="68" t="s">
+        <v>399</v>
+      </c>
+      <c r="B82" s="15" t="s">
+        <v>216</v>
+      </c>
+      <c r="C82" s="69" t="s">
         <v>400</v>
-      </c>
-      <c r="B82" s="15" t="s">
-        <v>217</v>
-      </c>
-      <c r="C82" s="69" t="s">
-        <v>401</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="270">
@@ -10976,10 +11161,10 @@
         <v>1</v>
       </c>
       <c r="B83" s="70" t="s">
+        <v>393</v>
+      </c>
+      <c r="C83" s="54" t="s">
         <v>394</v>
-      </c>
-      <c r="C83" s="54" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="240">
@@ -10987,10 +11172,10 @@
         <v>2</v>
       </c>
       <c r="B84" s="54" t="s">
+        <v>395</v>
+      </c>
+      <c r="C84" s="54" t="s">
         <v>396</v>
-      </c>
-      <c r="C84" s="54" t="s">
-        <v>397</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="255">
@@ -10998,22 +11183,119 @@
         <v>3</v>
       </c>
       <c r="B85" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="C85" s="13" t="s">
         <v>398</v>
-      </c>
-      <c r="C85" s="13" t="s">
-        <v>399</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="195">
       <c r="B86" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="C86" s="42" t="s">
         <v>292</v>
       </c>
-      <c r="C86" s="42" t="s">
-        <v>293</v>
-      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="B87" s="83"/>
+      <c r="C87" s="84"/>
+    </row>
+    <row r="88" spans="1:3" ht="51" customHeight="1">
+      <c r="B88" s="81" t="s">
+        <v>409</v>
+      </c>
+      <c r="C88" s="81"/>
+    </row>
+    <row r="89" spans="1:3" ht="31.5">
+      <c r="B89" s="22" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" ht="30" customHeight="1">
+      <c r="A90" t="s">
+        <v>411</v>
+      </c>
+      <c r="B90" s="81" t="s">
+        <v>410</v>
+      </c>
+      <c r="C90" s="81"/>
+    </row>
+    <row r="91" spans="1:3" ht="45.75" customHeight="1">
+      <c r="A91" s="85" t="s">
+        <v>414</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="C91" s="73" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" ht="30">
+      <c r="A92" s="85"/>
+      <c r="B92" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="C92" s="73" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93" t="s">
+        <v>415</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="C93" s="73" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3">
+      <c r="A94" t="s">
+        <v>420</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="C94" s="73" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3">
+      <c r="B95" s="2"/>
+      <c r="C95" s="73"/>
+    </row>
+    <row r="96" spans="1:3">
+      <c r="B96" s="2"/>
+      <c r="C96" s="73"/>
+    </row>
+    <row r="97" spans="2:3">
+      <c r="B97" s="2"/>
+      <c r="C97" s="73"/>
+    </row>
+    <row r="98" spans="2:3">
+      <c r="B98" s="2"/>
+      <c r="C98" s="73"/>
+    </row>
+    <row r="99" spans="2:3">
+      <c r="B99" s="2"/>
+      <c r="C99" s="2"/>
+    </row>
+    <row r="100" spans="2:3">
+      <c r="B100" s="2"/>
+      <c r="C100" s="2"/>
+    </row>
+    <row r="101" spans="2:3">
+      <c r="B101" s="2"/>
+      <c r="C101" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="8">
+    <mergeCell ref="B88:C88"/>
+    <mergeCell ref="B90:C90"/>
+    <mergeCell ref="A91:A92"/>
     <mergeCell ref="B57:C57"/>
     <mergeCell ref="B58:C58"/>
     <mergeCell ref="B59:C59"/>
@@ -11030,8 +11312,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:C49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11051,195 +11333,195 @@
     </row>
     <row r="3" spans="2:3" ht="75">
       <c r="B3" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="C3" s="39" t="s">
         <v>265</v>
-      </c>
-      <c r="C3" s="39" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="205.5" customHeight="1">
       <c r="B4" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C4" s="40" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="62.25" customHeight="1">
       <c r="B5" s="35" t="s">
+        <v>402</v>
+      </c>
+      <c r="C5" s="40" t="s">
         <v>403</v>
-      </c>
-      <c r="C5" s="40" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="307.5" customHeight="1">
       <c r="B6" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="C6" s="40" t="s">
         <v>268</v>
-      </c>
-      <c r="C6" s="40" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="180">
       <c r="B7" s="37" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C7" s="56" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="105">
       <c r="B8" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C8" s="37" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="9" spans="2:3">
       <c r="B9" s="15" t="s">
+        <v>274</v>
+      </c>
+      <c r="C9" s="15" t="s">
         <v>275</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="10" spans="2:3">
       <c r="B10" s="37" t="s">
+        <v>276</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>277</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="11" spans="2:3">
       <c r="B11" s="37" t="s">
+        <v>278</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>279</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="12" spans="2:3">
       <c r="B12" s="37" t="s">
+        <v>280</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>281</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="13" spans="2:3">
       <c r="B13" s="37" t="s">
+        <v>282</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>283</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="14" spans="2:3">
       <c r="B14" s="37" t="s">
+        <v>284</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>285</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="15" spans="2:3">
       <c r="B15" s="37" t="s">
+        <v>286</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>287</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="16" spans="2:3">
       <c r="B16" s="37"/>
       <c r="C16" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="17" spans="2:3" ht="60">
       <c r="B17" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="C17" s="37" t="s">
         <v>272</v>
-      </c>
-      <c r="C17" s="37" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="18" spans="2:3" ht="165">
       <c r="B18" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="C18" s="41" t="s">
         <v>290</v>
-      </c>
-      <c r="C18" s="41" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="19" spans="2:3" ht="195">
       <c r="B19" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="C19" s="42" t="s">
         <v>292</v>
-      </c>
-      <c r="C19" s="42" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="20" spans="2:3" ht="165">
       <c r="B20" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="C20" s="37" t="s">
         <v>294</v>
-      </c>
-      <c r="C20" s="37" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="21" spans="2:3" ht="409.5" customHeight="1">
       <c r="B21" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="C21" s="40" t="s">
         <v>296</v>
-      </c>
-      <c r="C21" s="40" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="22" spans="2:3" ht="45">
       <c r="B22" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C22" s="71" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="23" spans="2:3" ht="30">
       <c r="B23" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="C23" s="37" t="s">
         <v>299</v>
-      </c>
-      <c r="C23" s="37" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="24" spans="2:3" ht="225">
       <c r="B24" s="43" t="s">
+        <v>300</v>
+      </c>
+      <c r="C24" s="40" t="s">
         <v>301</v>
-      </c>
-      <c r="C24" s="40" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="25" spans="2:3" ht="26.25">
       <c r="B25" s="44" t="s">
+        <v>302</v>
+      </c>
+      <c r="C25" s="37"/>
+    </row>
+    <row r="26" spans="2:3" ht="33" customHeight="1">
+      <c r="B26" s="82" t="s">
         <v>303</v>
       </c>
-      <c r="C25" s="37"/>
-    </row>
-    <row r="26" spans="2:3" ht="33" customHeight="1">
-      <c r="B26" s="80" t="s">
+      <c r="C26" s="82"/>
+    </row>
+    <row r="27" spans="2:3">
+      <c r="B27" s="82" t="s">
         <v>304</v>
       </c>
-      <c r="C26" s="80"/>
-    </row>
-    <row r="27" spans="2:3">
-      <c r="B27" s="80" t="s">
-        <v>305</v>
-      </c>
-      <c r="C27" s="80"/>
+      <c r="C27" s="82"/>
     </row>
     <row r="28" spans="2:3" ht="15.75" thickBot="1">
       <c r="B28" s="48" t="s">
@@ -11249,19 +11531,19 @@
     </row>
     <row r="29" spans="2:3" ht="15.75" thickBot="1">
       <c r="B29" s="47" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C29" s="2"/>
     </row>
     <row r="30" spans="2:3" ht="15.75" thickBot="1">
       <c r="B30" s="46" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C30" s="2"/>
     </row>
     <row r="31" spans="2:3" ht="15.75" thickBot="1">
       <c r="B31" s="47" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C31" s="2"/>
     </row>
@@ -11271,98 +11553,98 @@
     </row>
     <row r="33" spans="2:3" ht="15.75" thickBot="1">
       <c r="B33" s="47" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C33" s="2"/>
     </row>
     <row r="34" spans="2:3" ht="15.75" thickBot="1">
       <c r="B34" s="46" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C34" s="2"/>
     </row>
     <row r="35" spans="2:3" ht="15.75" thickBot="1">
       <c r="B35" s="46" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C35" s="2"/>
     </row>
     <row r="36" spans="2:3">
       <c r="B36" s="50" t="s">
+        <v>311</v>
+      </c>
+      <c r="C36" s="51"/>
+    </row>
+    <row r="37" spans="2:3" ht="50.25" customHeight="1">
+      <c r="B37" s="82" t="s">
         <v>312</v>
       </c>
-      <c r="C36" s="51"/>
-    </row>
-    <row r="37" spans="2:3" ht="50.25" customHeight="1">
-      <c r="B37" s="80" t="s">
+      <c r="C37" s="82"/>
+    </row>
+    <row r="38" spans="2:3" ht="32.25" customHeight="1">
+      <c r="B38" s="82" t="s">
         <v>313</v>
       </c>
-      <c r="C37" s="80"/>
-    </row>
-    <row r="38" spans="2:3" ht="32.25" customHeight="1">
-      <c r="B38" s="80" t="s">
-        <v>314</v>
-      </c>
-      <c r="C38" s="80"/>
+      <c r="C38" s="82"/>
     </row>
     <row r="39" spans="2:3" ht="15.75" thickBot="1">
       <c r="B39" s="52" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C39" s="49"/>
     </row>
     <row r="40" spans="2:3" ht="15.75" thickBot="1">
       <c r="B40" s="46" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C40" s="2"/>
     </row>
     <row r="41" spans="2:3" ht="15.75" thickBot="1">
       <c r="B41" s="46" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="42" spans="2:3" ht="15.75" thickBot="1">
       <c r="B42" s="46" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="43" spans="2:3" ht="15.75" thickBot="1">
       <c r="B43" s="46" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="44" spans="2:3" ht="15.75" thickBot="1">
       <c r="B44" s="46" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="45" spans="2:3" ht="15.75" thickBot="1">
       <c r="B45" s="46" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="46" spans="2:3" ht="15.75" thickBot="1">
       <c r="B46" s="46" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="47" spans="2:3">
       <c r="B47" s="50" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" ht="36" customHeight="1">
+      <c r="B48" s="82" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="48" spans="2:3" ht="36" customHeight="1">
-      <c r="B48" s="80" t="s">
+      <c r="C48" s="82"/>
+    </row>
+    <row r="49" spans="2:3" ht="49.5" customHeight="1">
+      <c r="B49" s="82" t="s">
         <v>324</v>
       </c>
-      <c r="C48" s="80"/>
-    </row>
-    <row r="49" spans="2:3" ht="49.5" customHeight="1">
-      <c r="B49" s="80" t="s">
-        <v>325</v>
-      </c>
-      <c r="C49" s="80"/>
+      <c r="C49" s="82"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Modify logging and update training plan.
</commit_message>
<xml_diff>
--- a/Training_Plan.xlsx
+++ b/Training_Plan.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="429">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="442">
   <si>
     <t>Java core</t>
   </si>
@@ -509,18 +509,18 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">3) HashMap is a </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>new class introduced in JDK 1.2</t>
+      <t xml:space="preserve">4) HashMap is </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>fast</t>
     </r>
     <r>
       <rPr>
@@ -535,18 +535,18 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Hashtable is a </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>legacy class</t>
+      <t xml:space="preserve">Hashtable is </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>slow</t>
     </r>
     <r>
       <rPr>
@@ -560,19 +560,28 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">4) HashMap is </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>fast</t>
+    <t>5) We can make the HashMap as synchronized by calling this code</t>
+  </si>
+  <si>
+    <t>Map m = Collections.synchronizedMap(hashMap);</t>
+  </si>
+  <si>
+    <t>Hashtable is internally synchronized and can't be unsynchronized.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">6) HashMap is </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>traversed by Iterator</t>
     </r>
     <r>
       <rPr>
@@ -598,6 +607,171 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t>traversed by Enumerator and Iterator</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Enumerator in Hashtable is </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>not fail-fast</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">8) HashMap inherits </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>AbstractMap</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> class.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Hashtable inherits </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Dictionary</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> class.</t>
+    </r>
+  </si>
+  <si>
+    <t>Difference between ArrayList and Vector?</t>
+  </si>
+  <si>
+    <t>ArrayList and Vector both implements List interface and maintains insertion order.</t>
+  </si>
+  <si>
+    <t>Vector</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1) ArrayList is </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>not synchronized</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Vector is </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>synchronized</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Vector is </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>slow</t>
     </r>
     <r>
@@ -608,367 +782,11 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <t>5) We can make the HashMap as synchronized by calling this code</t>
-  </si>
-  <si>
-    <t>Map m = Collections.synchronizedMap(hashMap);</t>
-  </si>
-  <si>
-    <t>Hashtable is internally synchronized and can't be unsynchronized.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">6) HashMap is </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>traversed by Iterator</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Hashtable is </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>traversed by Enumerator and Iterator</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">7) Iterator in HashMap is </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>fail-fast</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Enumerator in Hashtable is </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>not fail-fast</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">8) HashMap inherits </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>AbstractMap</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> class.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Hashtable inherits </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Dictionary</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> class.</t>
-    </r>
-  </si>
-  <si>
-    <t>Difference between ArrayList and Vector?</t>
-  </si>
-  <si>
-    <t>ArrayList and Vector both implements List interface and maintains insertion order.</t>
-  </si>
-  <si>
-    <t>Vector</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">1) ArrayList is </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>not synchronized</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Vector is </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>synchronized</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">3) ArrayList is </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>not a legacy</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> class, it is introduced in JDK 1.2.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Vector is a </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>legacy</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> class.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">4) ArrayList is </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>fast</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> because it is non-synchronized.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Vector is </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>slow</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t xml:space="preserve"> because it is synchronized i.e. in multithreading environment, it will hold the other threads in runnable or non-runnable state until current thread releases the lock of object.</t>
     </r>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">5) ArrayList uses </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Iterator</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> interface to traverse the elements.</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">Vector uses </t>
     </r>
     <r>
@@ -991,52 +809,6 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> interface to traverse the elements. But it can use Iterator also.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>2) ArrayList</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>increments 50%</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> of</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> current array size if number of element exceeds from its capacity.</t>
     </r>
   </si>
   <si>
@@ -2994,76 +2766,6 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> which does same thing but atomically and thus eliminates above race condition.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve"> - Additional feature called "</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>concurrency level</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>", which allows ConcurrentHashMap to</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> partition Map</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">. 
- - This is achieved by partitioning Map into different parts based on concurrency level and </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">locking only a partion of Map during updates
- - </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Iterator of ConcurrentHashMap's keySet area also fail-safe and doesn’t throw ConcurrentModificationExceptoin
- - Default concurrency level is 16 and can be changed, by providing a number which make sense and work for you while creating ConcurrentHashMap</t>
     </r>
   </si>
   <si>
@@ -7740,6 +7442,439 @@
     <t xml:space="preserve"> - This method is used to get unique integer for given object. 
  - This integer is used to find bucket when storing in hashmap or hashset.
  - By default, This method returns integer represention of memory address where object is stored.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2) ArrayList is </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>fast</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> because it is non-synchronized.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>3) ArrayList</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>increments 50%</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> of</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> current array size if number of element exceeds from its capacity.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">4) ArrayList uses </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Iterator</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> interface to traverse the elements.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">7) Iterator in HashMap is </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>fail-fast</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">.
+Fail fast iterator while iterating through the collection , instantly throws </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Concurrent Modification Exception</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> if</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> there is structural modification  of the collection </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> - Additional feature called "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>concurrency level</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>", which allows ConcurrentHashMap to</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> portion Map</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. 
+ - This is achieved by partitioning Map into different parts based on concurrency level and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">locking only a portion of Map during updates
+ - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Iterator of ConcurrentHashMap's keySet are also fail-safe and doesn’t throw ConcurrentModificationException
+ - Default concurrency level is 16 and can be changed, by providing a number which make sense and work for you while creating ConcurrentHashMap</t>
+    </r>
+  </si>
+  <si>
+    <t>How to analyze Deadlock in java?</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>tasklist</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> command from a Command Prompt window. This displays all processes, their </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>PIDs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, and a variety of other details.
+2. “jstack PID &gt;&gt; mydumps.tdump“ to generate the thread dump</t>
+    </r>
+  </si>
+  <si>
+    <t>REST vs SOAP, the difference between soap and rest</t>
+  </si>
+  <si>
+    <t>SOAP (Simple Object Access Protocol)</t>
+  </si>
+  <si>
+    <t>REST (Representational State Transfer)</t>
+  </si>
+  <si>
+    <t>REST permits many different data formats such as:
+- Json, XML, RSS, CSV…</t>
+  </si>
+  <si>
+    <t>SOAP only permits XML</t>
+  </si>
+  <si>
+    <t>SOAP based reads cannot be cached.</t>
+  </si>
+  <si>
+    <t>REST reads can be cached ==&gt; Rest is faster</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SOAP has a standard specification</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+WSDL is a sort of formal contract to define the interface that the Web service offers</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">REST </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">don't </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>hava a standard specification</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+The service producer and service consumer need to have a common understanding of the context as well as the content being passed along as there is no standard set of rules to describe the REST Web services interface.</t>
+    </r>
+  </si>
+  <si>
+    <t>What's Race Condition?</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Race conditions occur only if multiple threads are </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>accessing the same resource</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, and one or more of the threads </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>write</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> to the resource. If multiple threads read the same resource race conditions do not occur.</t>
+    </r>
+  </si>
+  <si>
+    <t>What's thread safety?</t>
+  </si>
+  <si>
+    <t>Thread safety is a process to make our program safe to use in multithread environment. That means we make sure that the shared resources couldn’t be changed while being reading by multiple threads</t>
+  </si>
+  <si>
+    <t>How to make our program thread safe?</t>
+  </si>
+  <si>
+    <t>1. Making shared object immutable in order to make sure that it's never updated by any of threads.
+2. synchronization</t>
   </si>
 </sst>
 </file>
@@ -8135,7 +8270,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -8306,6 +8441,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -8330,18 +8475,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -8363,13 +8501,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>47624</xdr:colOff>
-      <xdr:row>92</xdr:row>
+      <xdr:row>94</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>85724</xdr:colOff>
-      <xdr:row>102</xdr:row>
+      <xdr:row>104</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -8399,6 +8537,53 @@
           <a:headEnd/>
           <a:tailEnd/>
         </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>752475</xdr:colOff>
+      <xdr:row>146</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>3019425</xdr:colOff>
+      <xdr:row>185</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:srcRect l="30547" t="9959" r="6406" b="10366"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1400175" y="75980925"/>
+          <a:ext cx="7686675" cy="7467600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -8969,7 +9154,7 @@
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="10">
@@ -9206,10 +9391,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:E151"/>
+  <dimension ref="B2:E155"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="E71" sqref="E71"/>
+    <sheetView tabSelected="1" topLeftCell="B77" workbookViewId="0">
+      <selection activeCell="E83" sqref="E83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9222,7 +9407,7 @@
   <sheetData>
     <row r="2" spans="2:5" ht="31.5">
       <c r="B2" s="22" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="2:5">
@@ -9301,7 +9486,7 @@
     </row>
     <row r="10" spans="2:5" ht="31.5">
       <c r="B10" s="22" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="C10" s="23"/>
       <c r="D10" s="23"/>
@@ -9323,100 +9508,100 @@
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="10" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="E12" s="29" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
     </row>
     <row r="13" spans="2:5">
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="31" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="E13" s="31" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
     </row>
     <row r="14" spans="2:5">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="E14" s="29" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
     </row>
     <row r="15" spans="2:5" ht="30">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="E15" s="29" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
     </row>
     <row r="16" spans="2:5">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="E16" s="29" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
     </row>
     <row r="17" spans="2:5">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="E17" s="29" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
     </row>
     <row r="18" spans="2:5">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="E18" s="29" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
     </row>
     <row r="19" spans="2:5" ht="74.25" customHeight="1">
       <c r="B19" s="2"/>
       <c r="C19" s="32"/>
       <c r="D19" s="33" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="E19" s="30" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
     </row>
     <row r="20" spans="2:5" ht="78.75">
       <c r="B20" s="2"/>
       <c r="C20" s="32"/>
       <c r="D20" s="33" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="E20" s="30" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
     </row>
     <row r="21" spans="2:5" ht="93.75">
       <c r="B21" s="2"/>
       <c r="C21" s="32"/>
       <c r="D21" s="1" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="E21" s="30" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
     </row>
     <row r="22" spans="2:5">
@@ -9427,7 +9612,7 @@
     </row>
     <row r="23" spans="2:5" ht="31.5">
       <c r="B23" s="22" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="C23" s="23"/>
       <c r="D23" s="23"/>
@@ -9460,10 +9645,10 @@
     <row r="27" spans="2:5">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
-      <c r="D27" s="74" t="s">
+      <c r="D27" s="78" t="s">
         <v>47</v>
       </c>
-      <c r="E27" s="75"/>
+      <c r="E27" s="79"/>
     </row>
     <row r="28" spans="2:5">
       <c r="B28" s="2"/>
@@ -9519,17 +9704,17 @@
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="18" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E33" s="16"/>
     </row>
     <row r="34" spans="2:5">
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
-      <c r="D34" s="78" t="s">
-        <v>81</v>
-      </c>
-      <c r="E34" s="78"/>
+      <c r="D34" s="82" t="s">
+        <v>78</v>
+      </c>
+      <c r="E34" s="82"/>
     </row>
     <row r="35" spans="2:5">
       <c r="B35" s="2"/>
@@ -9538,540 +9723,544 @@
         <v>48</v>
       </c>
       <c r="E35" s="15" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="36" spans="2:5">
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="14" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E36" s="14" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="37" spans="2:5" ht="30">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" ht="45">
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
-      <c r="D37" s="14" t="s">
-        <v>91</v>
+      <c r="D37" s="74" t="s">
+        <v>420</v>
       </c>
       <c r="E37" s="14" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="38" spans="2:5">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" ht="30">
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
-      <c r="D38" s="14" t="s">
-        <v>85</v>
+      <c r="D38" s="74" t="s">
+        <v>421</v>
       </c>
       <c r="E38" s="14" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="39" spans="2:5" ht="45">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" ht="30">
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
-      <c r="D39" s="14" t="s">
-        <v>87</v>
+      <c r="D39" s="74" t="s">
+        <v>422</v>
       </c>
       <c r="E39" s="14" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="40" spans="2:5" ht="30">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" ht="18.75">
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
-      <c r="D40" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="E40" s="14" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="41" spans="2:5" ht="18.75">
+      <c r="D40" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="E40" s="20"/>
+    </row>
+    <row r="41" spans="2:5">
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
-      <c r="D41" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="E41" s="20"/>
+      <c r="D41" s="83" t="s">
+        <v>86</v>
+      </c>
+      <c r="E41" s="84"/>
     </row>
     <row r="42" spans="2:5">
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
-      <c r="D42" s="79" t="s">
-        <v>94</v>
-      </c>
-      <c r="E42" s="80"/>
-    </row>
-    <row r="43" spans="2:5">
+      <c r="D42" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="E42" s="15" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" ht="45">
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
-      <c r="D43" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="E43" s="15" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="44" spans="2:5" ht="45">
+      <c r="D43" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="E43" s="14" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5">
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="14" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="E44" s="14" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="45" spans="2:5">
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="14" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="E45" s="14" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="46" spans="2:5">
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="D46" s="14" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="E46" s="14" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="47" spans="2:5">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" ht="30">
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
       <c r="D47" s="14" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="E47" s="14" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="48" spans="2:5" ht="30">
-      <c r="B48" s="2"/>
-      <c r="C48" s="2"/>
-      <c r="D48" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="E48" s="14" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="49" spans="2:5">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5">
+      <c r="B48" s="2">
+        <v>2</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+    </row>
+    <row r="49" spans="2:5" ht="18.75">
       <c r="B49" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D49" s="2"/>
+        <v>19</v>
+      </c>
+      <c r="D49" s="18" t="s">
+        <v>59</v>
+      </c>
       <c r="E49" s="2"/>
     </row>
-    <row r="50" spans="2:5" ht="18.75">
-      <c r="B50" s="2">
-        <v>3</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D50" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="E50" s="2"/>
+    <row r="50" spans="2:5">
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="80" t="s">
+        <v>60</v>
+      </c>
+      <c r="E50" s="80"/>
     </row>
     <row r="51" spans="2:5">
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
-      <c r="D51" s="76" t="s">
-        <v>60</v>
-      </c>
-      <c r="E51" s="76"/>
-    </row>
-    <row r="52" spans="2:5">
+      <c r="D51" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="E51" s="15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" ht="30">
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
-      <c r="D52" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="E52" s="15" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="53" spans="2:5" ht="30">
+      <c r="D52" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="E52" s="14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5">
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
       <c r="D53" s="14" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E53" s="14" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="54" spans="2:5">
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
       <c r="D54" s="14" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E54" s="14" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="55" spans="2:5">
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
       <c r="D55" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="E55" s="14" t="s">
-        <v>68</v>
+        <v>69</v>
+      </c>
+      <c r="E55" s="81" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="56" spans="2:5">
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
       <c r="D56" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="E56" s="14" t="s">
         <v>70</v>
       </c>
+      <c r="E56" s="81"/>
     </row>
     <row r="57" spans="2:5">
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
       <c r="D57" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="E57" s="77" t="s">
+        <v>72</v>
+      </c>
+      <c r="E57" s="14" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="58" spans="2:5">
+    <row r="58" spans="2:5" ht="60">
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
-      <c r="D58" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="E58" s="77"/>
+      <c r="D58" s="74" t="s">
+        <v>423</v>
+      </c>
+      <c r="E58" s="14" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="59" spans="2:5">
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
       <c r="D59" s="14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E59" s="14" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="60" spans="2:5">
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
-      <c r="D60" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="E60" s="14" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="61" spans="2:5">
+      <c r="D60" s="73"/>
+      <c r="E60" s="73"/>
+    </row>
+    <row r="61" spans="2:5" ht="31.5">
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
-      <c r="D61" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="E61" s="14" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="62" spans="2:5">
+      <c r="D61" s="22" t="s">
+        <v>414</v>
+      </c>
+      <c r="E61" s="73"/>
+    </row>
+    <row r="62" spans="2:5" ht="18" customHeight="1">
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
-      <c r="D62" s="73"/>
-      <c r="E62" s="73"/>
-    </row>
-    <row r="63" spans="2:5" ht="18.75">
+      <c r="D62" s="69" t="s">
+        <v>416</v>
+      </c>
+      <c r="E62" s="69" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="63" spans="2:5" ht="62.25" customHeight="1">
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
-      <c r="D63" s="18" t="s">
-        <v>423</v>
-      </c>
-      <c r="E63" s="73"/>
-    </row>
-    <row r="64" spans="2:5" ht="18" customHeight="1">
+      <c r="D63" s="13" t="s">
+        <v>419</v>
+      </c>
+      <c r="E63" s="77" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="64" spans="2:5">
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
-      <c r="D64" s="69" t="s">
-        <v>425</v>
-      </c>
-      <c r="E64" s="69" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="65" spans="2:5" ht="62.25" customHeight="1">
+      <c r="D64" s="13"/>
+      <c r="E64" s="13"/>
+    </row>
+    <row r="65" spans="2:5" ht="31.5">
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
-      <c r="D65" s="13" t="s">
-        <v>428</v>
-      </c>
-      <c r="E65" s="86" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="66" spans="2:5">
+      <c r="D65" s="22" t="s">
+        <v>418</v>
+      </c>
+      <c r="E65" s="73"/>
+    </row>
+    <row r="66" spans="2:5" ht="150">
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
-      <c r="D66" s="13"/>
-      <c r="E66" s="13"/>
-    </row>
-    <row r="67" spans="2:5" ht="31.5">
-      <c r="B67" s="2"/>
-      <c r="C67" s="2"/>
-      <c r="D67" s="22" t="s">
-        <v>427</v>
-      </c>
-      <c r="E67" s="73"/>
-    </row>
-    <row r="68" spans="2:5" ht="150">
-      <c r="B68" s="2"/>
-      <c r="C68" s="2"/>
-      <c r="D68" s="73" t="s">
-        <v>422</v>
-      </c>
-      <c r="E68" s="2"/>
-    </row>
-    <row r="70" spans="2:5" ht="31.5">
-      <c r="B70" s="22" t="s">
-        <v>108</v>
+      <c r="D66" s="73" t="s">
+        <v>413</v>
+      </c>
+      <c r="E66" s="2"/>
+    </row>
+    <row r="68" spans="2:5" ht="31.5">
+      <c r="B68" s="22" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="69" spans="2:5" ht="60">
+      <c r="B69" s="2"/>
+      <c r="C69" s="2"/>
+      <c r="D69" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E69" s="25" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="70" spans="2:5" ht="45">
+      <c r="B70" s="2"/>
+      <c r="C70" s="2"/>
+      <c r="D70" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E70" s="17" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="71" spans="2:5" ht="60">
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
-      <c r="D71" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="E71" s="25" t="s">
-        <v>112</v>
+      <c r="D71" t="s">
+        <v>106</v>
+      </c>
+      <c r="E71" s="13" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="72" spans="2:5" ht="45">
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
       <c r="D72" s="2" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="E72" s="17" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="73" spans="2:5" ht="60">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="73" spans="2:5" ht="45">
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
-      <c r="D73" t="s">
-        <v>114</v>
-      </c>
-      <c r="E73" s="13" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="74" spans="2:5" ht="45">
+      <c r="D73" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E73" s="17" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="74" spans="2:5" ht="30">
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
       <c r="D74" s="2" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="E74" s="17" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="75" spans="2:5" ht="45">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="75" spans="2:5" ht="30">
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
       <c r="D75" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="E75" s="17" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="76" spans="2:5" ht="30">
+      <c r="E75" s="72" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="76" spans="2:5" ht="120">
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
       <c r="D76" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E76" s="17" t="s">
         <v>117</v>
       </c>
-      <c r="E76" s="17" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="77" spans="2:5" ht="30">
+    </row>
+    <row r="77" spans="2:5" ht="60">
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
       <c r="D77" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="E77" s="72" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="78" spans="2:5" ht="120">
-      <c r="B78" s="2"/>
-      <c r="C78" s="2"/>
-      <c r="D78" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="E78" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="E77" s="17" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="79" spans="2:5" ht="31.5">
+      <c r="B79" s="22" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="79" spans="2:5" ht="60">
-      <c r="B79" s="2"/>
-      <c r="C79" s="2"/>
-      <c r="D79" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="E79" s="17" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="81" spans="2:5" ht="31.5">
-      <c r="B81" s="22" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="82" spans="2:5" ht="225">
-      <c r="B82" s="2"/>
+    <row r="80" spans="2:5" ht="53.25" customHeight="1">
+      <c r="B80" s="32"/>
+      <c r="C80" s="2"/>
+      <c r="D80" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="E80" s="74" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="81" spans="2:5" ht="53.25" customHeight="1">
+      <c r="B81" s="32"/>
+      <c r="C81" s="2"/>
+      <c r="D81" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="E81" s="74" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="82" spans="2:5" ht="53.25" customHeight="1">
+      <c r="B82" s="32"/>
       <c r="C82" s="2"/>
       <c r="D82" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="E82" s="21" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="83" spans="2:5" ht="30">
+        <v>440</v>
+      </c>
+      <c r="E82" s="74" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="83" spans="2:5" ht="225">
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
       <c r="D83" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="E83" s="17" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="84" spans="2:5" ht="90">
+        <v>120</v>
+      </c>
+      <c r="E83" s="21" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="84" spans="2:5">
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
-      <c r="D84" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="E84" s="17" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="85" spans="2:5" ht="45">
+      <c r="D84" s="2"/>
+      <c r="E84" s="74"/>
+    </row>
+    <row r="85" spans="2:5" ht="30">
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
       <c r="D85" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="E85" s="21" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="86" spans="2:5" ht="60">
+        <v>122</v>
+      </c>
+      <c r="E85" s="17" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="86" spans="2:5" ht="90">
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
       <c r="D86" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="E86" s="21" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="87" spans="2:5" ht="90">
+        <v>121</v>
+      </c>
+      <c r="E86" s="17" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="87" spans="2:5" ht="45">
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
       <c r="D87" s="2" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="E87" s="21" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="88" spans="2:5" ht="30">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="88" spans="2:5" ht="60">
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
       <c r="D88" s="2" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="E88" s="21" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="89" spans="2:5" ht="30">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="89" spans="2:5" ht="90">
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
       <c r="D89" s="2" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="E89" s="21" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="90" spans="2:5" ht="60">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="90" spans="2:5" ht="30">
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
       <c r="D90" s="2" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
       <c r="E90" s="21" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="91" spans="2:5" ht="90">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="91" spans="2:5" ht="30">
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
       <c r="D91" s="2" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="E91" s="21" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
     </row>
     <row r="92" spans="2:5" ht="60">
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
       <c r="D92" s="2" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="E92" s="21" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="93" spans="2:5">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="93" spans="2:5" ht="90">
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
-      <c r="D93" s="2"/>
-      <c r="E93" s="21"/>
-    </row>
-    <row r="94" spans="2:5">
+      <c r="D93" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="E93" s="21" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="94" spans="2:5" ht="60">
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
-      <c r="D94" s="2"/>
-      <c r="E94" s="21"/>
+      <c r="D94" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E94" s="21" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="95" spans="2:5">
       <c r="B95" s="2"/>
@@ -10101,19 +10290,19 @@
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
       <c r="D99" s="2"/>
-      <c r="E99" s="26"/>
+      <c r="E99" s="21"/>
     </row>
     <row r="100" spans="2:5">
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
       <c r="D100" s="2"/>
-      <c r="E100" s="2"/>
+      <c r="E100" s="21"/>
     </row>
     <row r="101" spans="2:5">
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
       <c r="D101" s="2"/>
-      <c r="E101" s="2"/>
+      <c r="E101" s="26"/>
     </row>
     <row r="102" spans="2:5">
       <c r="B102" s="2"/>
@@ -10127,267 +10316,263 @@
       <c r="D103" s="2"/>
       <c r="E103" s="2"/>
     </row>
-    <row r="104" spans="2:5" ht="60">
+    <row r="104" spans="2:5">
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
-      <c r="D104" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="E104" s="26" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="105" spans="2:5" ht="75">
+      <c r="D104" s="2"/>
+      <c r="E104" s="2"/>
+    </row>
+    <row r="105" spans="2:5">
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
-      <c r="D105" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="E105" s="26" t="s">
-        <v>161</v>
-      </c>
+      <c r="D105" s="2"/>
+      <c r="E105" s="2"/>
     </row>
     <row r="106" spans="2:5" ht="60">
       <c r="B106" s="2"/>
       <c r="C106" s="2"/>
       <c r="D106" s="2" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
       <c r="E106" s="26" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="107" spans="2:5" ht="45">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="107" spans="2:5" ht="75">
       <c r="B107" s="2"/>
       <c r="C107" s="2"/>
       <c r="D107" s="2" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="E107" s="26" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="108" spans="2:5">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="108" spans="2:5" ht="60">
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
       <c r="D108" s="2" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="E108" s="26" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="109" spans="2:5" ht="75">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="109" spans="2:5" ht="45">
       <c r="B109" s="2"/>
       <c r="C109" s="2"/>
       <c r="D109" s="2" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="E109" s="26" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="110" spans="2:5" ht="135">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="110" spans="2:5">
       <c r="B110" s="2"/>
       <c r="C110" s="2"/>
       <c r="D110" s="2" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="E110" s="26" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="111" spans="2:5" ht="90">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="111" spans="2:5" ht="75">
       <c r="B111" s="2"/>
       <c r="C111" s="2"/>
       <c r="D111" s="2" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="E111" s="26" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
     </row>
     <row r="112" spans="2:5" ht="45">
       <c r="B112" s="2"/>
-      <c r="C112" s="2"/>
-      <c r="D112" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="E112" s="26" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="113" spans="2:5">
+      <c r="C112" s="32" t="s">
+        <v>425</v>
+      </c>
+      <c r="D112" s="2"/>
+      <c r="E112" s="40" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="113" spans="2:5" ht="31.5">
       <c r="B113" s="2"/>
-      <c r="C113" s="2"/>
-      <c r="D113" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="E113" s="26" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="114" spans="2:5" ht="30">
+      <c r="C113" s="22"/>
+      <c r="D113" s="2"/>
+      <c r="E113" s="74"/>
+    </row>
+    <row r="114" spans="2:5" ht="135">
       <c r="B114" s="2"/>
       <c r="C114" s="2"/>
-      <c r="D114" s="26" t="s">
-        <v>180</v>
+      <c r="D114" s="2" t="s">
+        <v>164</v>
       </c>
       <c r="E114" s="26" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="115" spans="2:5">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="115" spans="2:5" ht="90">
       <c r="B115" s="2"/>
       <c r="C115" s="2"/>
       <c r="D115" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="E115" s="26"/>
-    </row>
-    <row r="116" spans="2:5">
+        <v>166</v>
+      </c>
+      <c r="E115" s="26" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="116" spans="2:5" ht="45">
       <c r="B116" s="2"/>
       <c r="C116" s="2"/>
-      <c r="D116" s="15" t="s">
-        <v>183</v>
-      </c>
-      <c r="E116" s="15" t="s">
-        <v>184</v>
+      <c r="D116" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="E116" s="26" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="117" spans="2:5">
       <c r="B117" s="2"/>
       <c r="C117" s="2"/>
-      <c r="D117" s="26" t="s">
-        <v>185</v>
+      <c r="D117" s="2" t="s">
+        <v>170</v>
       </c>
       <c r="E117" s="26" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="118" spans="2:5">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="118" spans="2:5" ht="30">
       <c r="B118" s="2"/>
       <c r="C118" s="2"/>
       <c r="D118" s="26" t="s">
-        <v>187</v>
+        <v>172</v>
       </c>
       <c r="E118" s="26" t="s">
-        <v>188</v>
+        <v>173</v>
       </c>
     </row>
     <row r="119" spans="2:5">
       <c r="B119" s="2"/>
       <c r="C119" s="2"/>
-      <c r="D119" s="26" t="s">
-        <v>189</v>
-      </c>
-      <c r="E119" s="26" t="s">
-        <v>190</v>
-      </c>
+      <c r="D119" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="E119" s="26"/>
     </row>
     <row r="120" spans="2:5">
       <c r="B120" s="2"/>
       <c r="C120" s="2"/>
-      <c r="D120" s="26" t="s">
-        <v>191</v>
-      </c>
-      <c r="E120" s="26" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="121" spans="2:5" ht="31.5">
+      <c r="D120" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="E120" s="15" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="121" spans="2:5">
       <c r="B121" s="2"/>
-      <c r="C121" s="22" t="s">
-        <v>193</v>
-      </c>
-      <c r="D121" s="2"/>
-      <c r="E121" s="26"/>
-    </row>
-    <row r="122" spans="2:5" ht="105">
+      <c r="C121" s="2"/>
+      <c r="D121" s="26" t="s">
+        <v>177</v>
+      </c>
+      <c r="E121" s="26" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="122" spans="2:5">
       <c r="B122" s="2"/>
       <c r="C122" s="2"/>
-      <c r="D122" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="E122" s="28" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="123" spans="2:5" ht="120">
+      <c r="D122" s="26" t="s">
+        <v>179</v>
+      </c>
+      <c r="E122" s="26" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="123" spans="2:5">
       <c r="B123" s="2"/>
       <c r="C123" s="2"/>
-      <c r="D123" s="2" t="s">
-        <v>195</v>
+      <c r="D123" s="26" t="s">
+        <v>181</v>
       </c>
       <c r="E123" s="26" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="124" spans="2:5" ht="255">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="124" spans="2:5">
       <c r="B124" s="2"/>
       <c r="C124" s="2"/>
-      <c r="D124" s="2" t="s">
-        <v>196</v>
+      <c r="D124" s="26" t="s">
+        <v>183</v>
       </c>
       <c r="E124" s="26" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="125" spans="2:5" ht="180">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="125" spans="2:5" ht="31.5">
       <c r="B125" s="2"/>
-      <c r="C125" s="2"/>
-      <c r="D125" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="E125" s="28" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="126" spans="2:5" ht="30">
+      <c r="C125" s="22" t="s">
+        <v>185</v>
+      </c>
+      <c r="D125" s="2"/>
+      <c r="E125" s="26"/>
+    </row>
+    <row r="126" spans="2:5" ht="105">
       <c r="B126" s="2"/>
       <c r="C126" s="2"/>
-      <c r="D126" s="28" t="s">
-        <v>204</v>
-      </c>
-      <c r="E126" s="28"/>
-    </row>
-    <row r="127" spans="2:5" ht="30">
+      <c r="D126" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="E126" s="74" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="127" spans="2:5" ht="120">
       <c r="B127" s="2"/>
       <c r="C127" s="2"/>
-      <c r="D127" s="28" t="s">
-        <v>205</v>
-      </c>
-      <c r="E127" s="28"/>
-    </row>
-    <row r="128" spans="2:5" ht="30">
+      <c r="D127" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="E127" s="74" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="128" spans="2:5" ht="255">
       <c r="B128" s="2"/>
       <c r="C128" s="2"/>
-      <c r="D128" s="28" t="s">
-        <v>207</v>
-      </c>
-      <c r="E128" s="28"/>
-    </row>
-    <row r="129" spans="2:5" ht="45">
+      <c r="D128" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="E128" s="26" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="129" spans="2:5" ht="180">
       <c r="B129" s="2"/>
       <c r="C129" s="2"/>
-      <c r="D129" s="28" t="s">
-        <v>201</v>
-      </c>
-      <c r="E129" s="28"/>
-    </row>
-    <row r="130" spans="2:5">
+      <c r="D129" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="E129" s="28" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="130" spans="2:5" ht="30">
       <c r="B130" s="2"/>
       <c r="C130" s="2"/>
       <c r="D130" s="28" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
       <c r="E130" s="28"/>
     </row>
-    <row r="131" spans="2:5" ht="60">
+    <row r="131" spans="2:5" ht="30">
       <c r="B131" s="2"/>
       <c r="C131" s="2"/>
       <c r="D131" s="28" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
       <c r="E131" s="28"/>
     </row>
@@ -10395,108 +10580,116 @@
       <c r="B132" s="2"/>
       <c r="C132" s="2"/>
       <c r="D132" s="28" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="E132" s="28"/>
     </row>
-    <row r="133" spans="2:5">
+    <row r="133" spans="2:5" ht="45">
       <c r="B133" s="2"/>
       <c r="C133" s="2"/>
       <c r="D133" s="28" t="s">
-        <v>211</v>
+        <v>192</v>
       </c>
       <c r="E133" s="28"/>
     </row>
-    <row r="134" spans="2:5" ht="30">
+    <row r="134" spans="2:5">
       <c r="B134" s="2"/>
       <c r="C134" s="2"/>
       <c r="D134" s="28" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E134" s="28"/>
     </row>
-    <row r="135" spans="2:5" ht="30">
+    <row r="135" spans="2:5" ht="60">
       <c r="B135" s="2"/>
       <c r="C135" s="2"/>
       <c r="D135" s="28" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="E135" s="28"/>
     </row>
-    <row r="136" spans="2:5">
+    <row r="136" spans="2:5" ht="30">
       <c r="B136" s="2"/>
       <c r="C136" s="2"/>
-      <c r="D136" s="28"/>
-      <c r="E136" s="26"/>
-    </row>
-    <row r="138" spans="2:5" ht="31.5">
-      <c r="C138" s="22" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="139" spans="2:5" ht="90">
+      <c r="D136" s="28" t="s">
+        <v>201</v>
+      </c>
+      <c r="E136" s="28"/>
+    </row>
+    <row r="137" spans="2:5">
+      <c r="B137" s="2"/>
+      <c r="C137" s="2"/>
+      <c r="D137" s="28" t="s">
+        <v>202</v>
+      </c>
+      <c r="E137" s="28"/>
+    </row>
+    <row r="138" spans="2:5" ht="30">
+      <c r="B138" s="2"/>
+      <c r="C138" s="2"/>
+      <c r="D138" s="28" t="s">
+        <v>193</v>
+      </c>
+      <c r="E138" s="28"/>
+    </row>
+    <row r="139" spans="2:5" ht="30">
       <c r="B139" s="2"/>
       <c r="C139" s="2"/>
-      <c r="D139" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="E139" s="21" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="140" spans="2:5" ht="90">
+      <c r="D139" s="28" t="s">
+        <v>194</v>
+      </c>
+      <c r="E139" s="28"/>
+    </row>
+    <row r="140" spans="2:5">
       <c r="B140" s="2"/>
       <c r="C140" s="2"/>
-      <c r="D140" s="28" t="s">
-        <v>154</v>
-      </c>
-      <c r="E140" s="21" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="141" spans="2:5" ht="105">
-      <c r="B141" s="2"/>
-      <c r="C141" s="2"/>
-      <c r="D141" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="E141" s="21" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="142" spans="2:5" ht="90">
-      <c r="B142" s="2"/>
-      <c r="C142" s="2"/>
-      <c r="D142" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="E142" s="21" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="143" spans="2:5">
+      <c r="D140" s="28"/>
+      <c r="E140" s="26"/>
+    </row>
+    <row r="142" spans="2:5" ht="31.5">
+      <c r="C142" s="22" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="143" spans="2:5" ht="90">
       <c r="B143" s="2"/>
       <c r="C143" s="2"/>
-      <c r="D143" s="2"/>
-      <c r="E143" s="21"/>
-    </row>
-    <row r="144" spans="2:5">
+      <c r="D143" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E143" s="21" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="144" spans="2:5" ht="90">
       <c r="B144" s="2"/>
       <c r="C144" s="2"/>
-      <c r="D144" s="2"/>
-      <c r="E144" s="21"/>
-    </row>
-    <row r="145" spans="2:5">
+      <c r="D144" s="28" t="s">
+        <v>146</v>
+      </c>
+      <c r="E144" s="21" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="145" spans="2:5" ht="105">
       <c r="B145" s="2"/>
       <c r="C145" s="2"/>
-      <c r="D145" s="2"/>
-      <c r="E145" s="21"/>
-    </row>
-    <row r="146" spans="2:5">
+      <c r="D145" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="E145" s="21" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="146" spans="2:5" ht="90">
       <c r="B146" s="2"/>
       <c r="C146" s="2"/>
-      <c r="D146" s="2"/>
-      <c r="E146" s="21"/>
+      <c r="D146" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E146" s="21" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="147" spans="2:5">
       <c r="B147" s="2"/>
@@ -10523,22 +10716,43 @@
       <c r="E150" s="21"/>
     </row>
     <row r="151" spans="2:5">
-      <c r="E151" s="27"/>
+      <c r="B151" s="2"/>
+      <c r="C151" s="2"/>
+      <c r="D151" s="2"/>
+      <c r="E151" s="21"/>
+    </row>
+    <row r="152" spans="2:5">
+      <c r="B152" s="2"/>
+      <c r="C152" s="2"/>
+      <c r="D152" s="2"/>
+      <c r="E152" s="21"/>
+    </row>
+    <row r="153" spans="2:5">
+      <c r="B153" s="2"/>
+      <c r="C153" s="2"/>
+      <c r="D153" s="2"/>
+      <c r="E153" s="21"/>
+    </row>
+    <row r="154" spans="2:5">
+      <c r="B154" s="2"/>
+      <c r="C154" s="2"/>
+      <c r="D154" s="2"/>
+      <c r="E154" s="21"/>
+    </row>
+    <row r="155" spans="2:5">
+      <c r="E155" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="E57:E58"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="E55:E56"/>
     <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D41:E41"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="D63" r:id="rId1" display="http://www.java2blog.com/2014/02/hashcode-and-equals-method-in-java.html"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
-  <drawing r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -10547,7 +10761,7 @@
   <dimension ref="B3:C13"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10566,62 +10780,62 @@
     </row>
     <row r="4" spans="2:3" ht="45">
       <c r="B4" s="1" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
     </row>
     <row r="5" spans="2:3">
       <c r="B5" s="2" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="30" customHeight="1">
       <c r="B6" s="1" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="C6" s="2"/>
     </row>
     <row r="7" spans="2:3" ht="315">
       <c r="B7" s="30" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="105">
       <c r="B8" s="1" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
     </row>
     <row r="9" spans="2:3" ht="60">
       <c r="B9" s="1" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="C9" s="34" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
     </row>
     <row r="10" spans="2:3" ht="165">
       <c r="B10" s="1" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
     </row>
     <row r="11" spans="2:3" ht="105">
       <c r="B11" s="2"/>
       <c r="C11" s="30" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
     </row>
     <row r="12" spans="2:3">
@@ -10640,10 +10854,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A3:C101"/>
+  <dimension ref="A3:C102"/>
   <sheetViews>
-    <sheetView topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="B102" sqref="B102"/>
+    <sheetView topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="B98" sqref="B98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10655,61 +10869,61 @@
   <sheetData>
     <row r="3" spans="2:3" ht="90.75">
       <c r="B3" s="35" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="23.25">
       <c r="B4" s="36" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="C4" s="2"/>
     </row>
     <row r="5" spans="2:3" ht="45">
       <c r="B5" s="2" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="135">
       <c r="B6" s="2" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="315">
       <c r="B7" s="2" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="60">
       <c r="B8" s="2" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
     </row>
     <row r="9" spans="2:3" ht="31.5">
       <c r="B9" s="36" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
     </row>
     <row r="10" spans="2:3" ht="31.5">
       <c r="B10" s="32" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="C10" s="2"/>
     </row>
@@ -10819,142 +11033,142 @@
     </row>
     <row r="37" spans="1:3" ht="90">
       <c r="B37" s="2" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="C37" s="37" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="B38" s="2" t="s">
-        <v>263</v>
+        <v>254</v>
       </c>
       <c r="C38" s="37"/>
     </row>
     <row r="40" spans="1:3">
       <c r="B40" s="2" t="s">
-        <v>325</v>
+        <v>316</v>
       </c>
       <c r="C40" s="2"/>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="55"/>
       <c r="B41" s="15" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
       <c r="C41" s="15" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="30">
       <c r="A42" s="53" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
       <c r="B42" s="53" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="C42" s="53" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="53" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="B43" s="53" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="C43" s="53" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="53" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
       <c r="B44" s="53" t="s">
-        <v>333</v>
+        <v>324</v>
       </c>
       <c r="C44" s="53" t="s">
-        <v>334</v>
+        <v>325</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="30">
       <c r="A45" s="53" t="s">
-        <v>335</v>
+        <v>326</v>
       </c>
       <c r="B45" s="53" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
       <c r="C45" s="53" t="s">
-        <v>337</v>
+        <v>328</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="53" t="s">
-        <v>338</v>
+        <v>329</v>
       </c>
       <c r="B46" s="53" t="s">
-        <v>339</v>
+        <v>330</v>
       </c>
       <c r="C46" s="53" t="s">
-        <v>340</v>
+        <v>331</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="30">
       <c r="A47" s="53" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
       <c r="B47" s="53" t="s">
-        <v>342</v>
+        <v>333</v>
       </c>
       <c r="C47" s="53" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="30">
       <c r="A48" s="53" t="s">
-        <v>344</v>
+        <v>335</v>
       </c>
       <c r="B48" s="53" t="s">
-        <v>345</v>
+        <v>336</v>
       </c>
       <c r="C48" s="53" t="s">
-        <v>346</v>
+        <v>337</v>
       </c>
     </row>
     <row r="49" spans="1:3">
-      <c r="A49" s="77" t="s">
-        <v>347</v>
+      <c r="A49" s="81" t="s">
+        <v>338</v>
       </c>
       <c r="B49" s="53" t="s">
-        <v>348</v>
-      </c>
-      <c r="C49" s="77" t="s">
-        <v>350</v>
+        <v>339</v>
+      </c>
+      <c r="C49" s="81" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="50" spans="1:3">
-      <c r="A50" s="77"/>
+      <c r="A50" s="81"/>
       <c r="B50" s="53"/>
-      <c r="C50" s="77"/>
+      <c r="C50" s="81"/>
     </row>
     <row r="51" spans="1:3">
-      <c r="A51" s="77"/>
+      <c r="A51" s="81"/>
       <c r="B51" s="53" t="s">
-        <v>349</v>
-      </c>
-      <c r="C51" s="77"/>
+        <v>340</v>
+      </c>
+      <c r="C51" s="81"/>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="53" t="s">
-        <v>351</v>
+        <v>342</v>
       </c>
       <c r="B52" s="53" t="s">
-        <v>352</v>
+        <v>343</v>
       </c>
       <c r="C52" s="53" t="s">
-        <v>353</v>
+        <v>344</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -10962,38 +11176,38 @@
     </row>
     <row r="54" spans="1:3" ht="31.5">
       <c r="B54" s="22" t="s">
-        <v>354</v>
+        <v>345</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="B55" t="s">
-        <v>355</v>
+        <v>346</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="B56" s="58"/>
     </row>
     <row r="57" spans="1:3" ht="32.25" customHeight="1">
-      <c r="B57" s="81" t="s">
-        <v>356</v>
-      </c>
-      <c r="C57" s="81"/>
+      <c r="B57" s="85" t="s">
+        <v>347</v>
+      </c>
+      <c r="C57" s="85"/>
     </row>
     <row r="58" spans="1:3" ht="33" customHeight="1">
-      <c r="B58" s="81" t="s">
-        <v>357</v>
-      </c>
-      <c r="C58" s="81"/>
+      <c r="B58" s="85" t="s">
+        <v>348</v>
+      </c>
+      <c r="C58" s="85"/>
     </row>
     <row r="59" spans="1:3" ht="19.5" customHeight="1">
-      <c r="B59" s="81" t="s">
-        <v>358</v>
-      </c>
-      <c r="C59" s="81"/>
+      <c r="B59" s="85" t="s">
+        <v>349</v>
+      </c>
+      <c r="C59" s="85"/>
     </row>
     <row r="60" spans="1:3">
       <c r="B60" s="2" t="s">
-        <v>359</v>
+        <v>350</v>
       </c>
       <c r="C60" s="2"/>
     </row>
@@ -11003,157 +11217,157 @@
     </row>
     <row r="62" spans="1:3">
       <c r="B62" s="60" t="s">
-        <v>360</v>
+        <v>351</v>
       </c>
       <c r="C62" s="2"/>
     </row>
     <row r="63" spans="1:3" ht="30">
       <c r="B63" s="61" t="s">
-        <v>361</v>
+        <v>352</v>
       </c>
       <c r="C63" s="2"/>
     </row>
     <row r="64" spans="1:3">
       <c r="B64" s="60" t="s">
-        <v>362</v>
+        <v>353</v>
       </c>
       <c r="C64" s="2"/>
     </row>
     <row r="65" spans="2:3" ht="225">
       <c r="B65" s="2" t="s">
-        <v>363</v>
+        <v>354</v>
       </c>
       <c r="C65" s="54" t="s">
-        <v>364</v>
+        <v>355</v>
       </c>
     </row>
     <row r="66" spans="2:3" ht="30">
       <c r="B66" s="37" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="C66" s="37"/>
     </row>
     <row r="67" spans="2:3" ht="30.75">
       <c r="B67" s="63" t="s">
-        <v>365</v>
+        <v>356</v>
       </c>
       <c r="C67" s="54" t="s">
-        <v>366</v>
+        <v>357</v>
       </c>
     </row>
     <row r="68" spans="2:3" ht="137.25" customHeight="1">
       <c r="B68" s="64" t="s">
-        <v>367</v>
+        <v>358</v>
       </c>
       <c r="C68" s="16" t="s">
-        <v>374</v>
+        <v>365</v>
       </c>
     </row>
     <row r="69" spans="2:3" ht="105.75">
       <c r="B69" s="63" t="s">
-        <v>368</v>
+        <v>359</v>
       </c>
       <c r="C69" s="54" t="s">
-        <v>369</v>
+        <v>360</v>
       </c>
     </row>
     <row r="70" spans="2:3" ht="53.25" customHeight="1">
       <c r="B70" s="65" t="s">
-        <v>371</v>
+        <v>362</v>
       </c>
       <c r="C70" s="62" t="s">
-        <v>370</v>
+        <v>361</v>
       </c>
     </row>
     <row r="71" spans="2:3" ht="32.25" customHeight="1">
       <c r="B71" s="63" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
       <c r="C71" s="62" t="s">
-        <v>373</v>
+        <v>364</v>
       </c>
     </row>
     <row r="72" spans="2:3" ht="135">
       <c r="B72" s="63" t="s">
-        <v>375</v>
+        <v>366</v>
       </c>
       <c r="C72" s="66" t="s">
-        <v>376</v>
+        <v>367</v>
       </c>
     </row>
     <row r="73" spans="2:3" ht="30.75">
       <c r="B73" s="63" t="s">
-        <v>377</v>
+        <v>368</v>
       </c>
       <c r="C73" s="54" t="s">
-        <v>378</v>
+        <v>369</v>
       </c>
     </row>
     <row r="74" spans="2:3">
       <c r="B74" s="67" t="s">
-        <v>379</v>
+        <v>370</v>
       </c>
       <c r="C74" s="67" t="s">
-        <v>380</v>
+        <v>371</v>
       </c>
     </row>
     <row r="75" spans="2:3" ht="30">
       <c r="B75" s="67" t="s">
-        <v>381</v>
+        <v>372</v>
       </c>
       <c r="C75" s="54" t="s">
-        <v>382</v>
+        <v>373</v>
       </c>
     </row>
     <row r="76" spans="2:3" ht="33.75" customHeight="1">
       <c r="B76" s="67" t="s">
-        <v>383</v>
+        <v>374</v>
       </c>
       <c r="C76" s="54" t="s">
-        <v>384</v>
+        <v>375</v>
       </c>
     </row>
     <row r="77" spans="2:3" ht="30">
       <c r="B77" s="67" t="s">
-        <v>385</v>
+        <v>376</v>
       </c>
       <c r="C77" s="54" t="s">
-        <v>386</v>
+        <v>377</v>
       </c>
     </row>
     <row r="78" spans="2:3" ht="30.75">
       <c r="B78" s="67" t="s">
-        <v>387</v>
+        <v>378</v>
       </c>
       <c r="C78" s="54" t="s">
-        <v>388</v>
+        <v>379</v>
       </c>
     </row>
     <row r="79" spans="2:3" ht="30">
       <c r="B79" s="67" t="s">
-        <v>389</v>
+        <v>380</v>
       </c>
       <c r="C79" s="54" t="s">
-        <v>390</v>
+        <v>381</v>
       </c>
     </row>
     <row r="80" spans="2:3">
       <c r="B80" s="67" t="s">
-        <v>391</v>
+        <v>382</v>
       </c>
       <c r="C80" s="54" t="s">
-        <v>392</v>
+        <v>383</v>
       </c>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" s="68" t="s">
-        <v>399</v>
+        <v>390</v>
       </c>
       <c r="B82" s="15" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="C82" s="69" t="s">
-        <v>400</v>
+        <v>391</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="270">
@@ -11161,10 +11375,10 @@
         <v>1</v>
       </c>
       <c r="B83" s="70" t="s">
-        <v>393</v>
+        <v>384</v>
       </c>
       <c r="C83" s="54" t="s">
-        <v>394</v>
+        <v>385</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="240">
@@ -11172,10 +11386,10 @@
         <v>2</v>
       </c>
       <c r="B84" s="54" t="s">
-        <v>395</v>
+        <v>386</v>
       </c>
       <c r="C84" s="54" t="s">
-        <v>396</v>
+        <v>387</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="255">
@@ -11183,124 +11397,146 @@
         <v>3</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>397</v>
+        <v>388</v>
       </c>
       <c r="C85" s="13" t="s">
-        <v>398</v>
+        <v>389</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="195">
       <c r="B86" s="4" t="s">
-        <v>291</v>
+        <v>282</v>
       </c>
       <c r="C86" s="42" t="s">
-        <v>292</v>
+        <v>283</v>
       </c>
     </row>
     <row r="87" spans="1:3">
-      <c r="B87" s="83"/>
-      <c r="C87" s="84"/>
+      <c r="B87" s="75"/>
+      <c r="C87" s="76"/>
     </row>
     <row r="88" spans="1:3" ht="51" customHeight="1">
-      <c r="B88" s="81" t="s">
-        <v>409</v>
-      </c>
-      <c r="C88" s="81"/>
+      <c r="B88" s="85" t="s">
+        <v>400</v>
+      </c>
+      <c r="C88" s="85"/>
     </row>
     <row r="89" spans="1:3" ht="31.5">
       <c r="B89" s="22" t="s">
-        <v>407</v>
+        <v>398</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="30" customHeight="1">
       <c r="A90" t="s">
-        <v>411</v>
-      </c>
-      <c r="B90" s="81" t="s">
-        <v>410</v>
-      </c>
-      <c r="C90" s="81"/>
+        <v>402</v>
+      </c>
+      <c r="B90" s="85" t="s">
+        <v>401</v>
+      </c>
+      <c r="C90" s="85"/>
     </row>
     <row r="91" spans="1:3" ht="45.75" customHeight="1">
-      <c r="A91" s="85" t="s">
-        <v>414</v>
+      <c r="A91" s="86" t="s">
+        <v>405</v>
       </c>
       <c r="B91" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="C91" s="73" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" ht="30">
+      <c r="A92" s="86"/>
+      <c r="B92" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="C91" s="73" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" ht="30">
-      <c r="A92" s="85"/>
-      <c r="B92" s="2" t="s">
-        <v>417</v>
-      </c>
       <c r="C92" s="73" t="s">
-        <v>413</v>
+        <v>404</v>
       </c>
     </row>
     <row r="93" spans="1:3">
       <c r="A93" t="s">
-        <v>415</v>
+        <v>406</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>418</v>
+        <v>409</v>
       </c>
       <c r="C93" s="73" t="s">
-        <v>416</v>
+        <v>407</v>
       </c>
     </row>
     <row r="94" spans="1:3">
       <c r="A94" t="s">
-        <v>420</v>
+        <v>411</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>421</v>
+        <v>412</v>
       </c>
       <c r="C94" s="73" t="s">
-        <v>419</v>
+        <v>410</v>
       </c>
     </row>
     <row r="95" spans="1:3">
       <c r="B95" s="2"/>
       <c r="C95" s="73"/>
     </row>
-    <row r="96" spans="1:3">
-      <c r="B96" s="2"/>
+    <row r="96" spans="1:3" ht="31.5">
+      <c r="B96" s="32" t="s">
+        <v>427</v>
+      </c>
       <c r="C96" s="73"/>
     </row>
     <row r="97" spans="2:3">
-      <c r="B97" s="2"/>
-      <c r="C97" s="73"/>
-    </row>
-    <row r="98" spans="2:3">
-      <c r="B98" s="2"/>
-      <c r="C98" s="73"/>
-    </row>
-    <row r="99" spans="2:3">
-      <c r="B99" s="2"/>
-      <c r="C99" s="2"/>
+      <c r="B97" s="38" t="s">
+        <v>428</v>
+      </c>
+      <c r="C97" s="69" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="98" spans="2:3" ht="60">
+      <c r="B98" s="74" t="s">
+        <v>434</v>
+      </c>
+      <c r="C98" s="74" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="99" spans="2:3" ht="30">
+      <c r="B99" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="C99" s="74" t="s">
+        <v>430</v>
+      </c>
     </row>
     <row r="100" spans="2:3">
-      <c r="B100" s="2"/>
-      <c r="C100" s="2"/>
+      <c r="B100" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>433</v>
+      </c>
     </row>
     <row r="101" spans="2:3">
-      <c r="B101" s="2"/>
-      <c r="C101" s="2"/>
+      <c r="B101" s="74"/>
+      <c r="C101" s="74"/>
+    </row>
+    <row r="102" spans="2:3">
+      <c r="B102" s="2"/>
+      <c r="C102" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="C49:C51"/>
     <mergeCell ref="B88:C88"/>
     <mergeCell ref="B90:C90"/>
     <mergeCell ref="A91:A92"/>
     <mergeCell ref="B57:C57"/>
     <mergeCell ref="B58:C58"/>
     <mergeCell ref="B59:C59"/>
-    <mergeCell ref="A49:A51"/>
-    <mergeCell ref="C49:C51"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -11333,195 +11569,195 @@
     </row>
     <row r="3" spans="2:3" ht="75">
       <c r="B3" s="2" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
       <c r="C3" s="39" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="205.5" customHeight="1">
       <c r="B4" s="2" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
       <c r="C4" s="40" t="s">
-        <v>404</v>
+        <v>395</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="62.25" customHeight="1">
       <c r="B5" s="35" t="s">
-        <v>402</v>
+        <v>393</v>
       </c>
       <c r="C5" s="40" t="s">
-        <v>403</v>
+        <v>394</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="307.5" customHeight="1">
       <c r="B6" s="4" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
       <c r="C6" s="40" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="180">
       <c r="B7" s="37" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
       <c r="C7" s="56" t="s">
-        <v>401</v>
+        <v>392</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="105">
       <c r="B8" s="2" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
       <c r="C8" s="37" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
     </row>
     <row r="9" spans="2:3">
       <c r="B9" s="15" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
     </row>
     <row r="10" spans="2:3">
       <c r="B10" s="37" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
     </row>
     <row r="11" spans="2:3">
       <c r="B11" s="37" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>279</v>
+        <v>270</v>
       </c>
     </row>
     <row r="12" spans="2:3">
       <c r="B12" s="37" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>281</v>
+        <v>272</v>
       </c>
     </row>
     <row r="13" spans="2:3">
       <c r="B13" s="37" t="s">
-        <v>282</v>
+        <v>273</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
     </row>
     <row r="14" spans="2:3">
       <c r="B14" s="37" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>285</v>
+        <v>276</v>
       </c>
     </row>
     <row r="15" spans="2:3">
       <c r="B15" s="37" t="s">
-        <v>286</v>
+        <v>277</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
     </row>
     <row r="16" spans="2:3">
       <c r="B16" s="37"/>
       <c r="C16" s="2" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
     </row>
     <row r="17" spans="2:3" ht="60">
       <c r="B17" s="2" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
       <c r="C17" s="37" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
     </row>
     <row r="18" spans="2:3" ht="165">
       <c r="B18" s="2" t="s">
-        <v>289</v>
+        <v>280</v>
       </c>
       <c r="C18" s="41" t="s">
-        <v>290</v>
+        <v>281</v>
       </c>
     </row>
     <row r="19" spans="2:3" ht="195">
       <c r="B19" s="4" t="s">
-        <v>291</v>
+        <v>282</v>
       </c>
       <c r="C19" s="42" t="s">
-        <v>292</v>
+        <v>283</v>
       </c>
     </row>
     <row r="20" spans="2:3" ht="165">
       <c r="B20" s="2" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="C20" s="37" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
     </row>
     <row r="21" spans="2:3" ht="409.5" customHeight="1">
       <c r="B21" s="2" t="s">
-        <v>295</v>
+        <v>286</v>
       </c>
       <c r="C21" s="40" t="s">
-        <v>296</v>
+        <v>287</v>
       </c>
     </row>
     <row r="22" spans="2:3" ht="45">
       <c r="B22" s="2" t="s">
-        <v>297</v>
+        <v>288</v>
       </c>
       <c r="C22" s="71" t="s">
-        <v>405</v>
+        <v>396</v>
       </c>
     </row>
     <row r="23" spans="2:3" ht="30">
       <c r="B23" s="2" t="s">
-        <v>298</v>
+        <v>289</v>
       </c>
       <c r="C23" s="37" t="s">
-        <v>299</v>
+        <v>290</v>
       </c>
     </row>
     <row r="24" spans="2:3" ht="225">
       <c r="B24" s="43" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="C24" s="40" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
     </row>
     <row r="25" spans="2:3" ht="26.25">
       <c r="B25" s="44" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
       <c r="C25" s="37"/>
     </row>
     <row r="26" spans="2:3" ht="33" customHeight="1">
-      <c r="B26" s="82" t="s">
-        <v>303</v>
-      </c>
-      <c r="C26" s="82"/>
+      <c r="B26" s="87" t="s">
+        <v>294</v>
+      </c>
+      <c r="C26" s="87"/>
     </row>
     <row r="27" spans="2:3">
-      <c r="B27" s="82" t="s">
-        <v>304</v>
-      </c>
-      <c r="C27" s="82"/>
+      <c r="B27" s="87" t="s">
+        <v>295</v>
+      </c>
+      <c r="C27" s="87"/>
     </row>
     <row r="28" spans="2:3" ht="15.75" thickBot="1">
       <c r="B28" s="48" t="s">
@@ -11531,19 +11767,19 @@
     </row>
     <row r="29" spans="2:3" ht="15.75" thickBot="1">
       <c r="B29" s="47" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
       <c r="C29" s="2"/>
     </row>
     <row r="30" spans="2:3" ht="15.75" thickBot="1">
       <c r="B30" s="46" t="s">
-        <v>306</v>
+        <v>297</v>
       </c>
       <c r="C30" s="2"/>
     </row>
     <row r="31" spans="2:3" ht="15.75" thickBot="1">
       <c r="B31" s="47" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
       <c r="C31" s="2"/>
     </row>
@@ -11553,98 +11789,98 @@
     </row>
     <row r="33" spans="2:3" ht="15.75" thickBot="1">
       <c r="B33" s="47" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
       <c r="C33" s="2"/>
     </row>
     <row r="34" spans="2:3" ht="15.75" thickBot="1">
       <c r="B34" s="46" t="s">
-        <v>309</v>
+        <v>300</v>
       </c>
       <c r="C34" s="2"/>
     </row>
     <row r="35" spans="2:3" ht="15.75" thickBot="1">
       <c r="B35" s="46" t="s">
-        <v>310</v>
+        <v>301</v>
       </c>
       <c r="C35" s="2"/>
     </row>
     <row r="36" spans="2:3">
       <c r="B36" s="50" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
       <c r="C36" s="51"/>
     </row>
     <row r="37" spans="2:3" ht="50.25" customHeight="1">
-      <c r="B37" s="82" t="s">
-        <v>312</v>
-      </c>
-      <c r="C37" s="82"/>
+      <c r="B37" s="87" t="s">
+        <v>303</v>
+      </c>
+      <c r="C37" s="87"/>
     </row>
     <row r="38" spans="2:3" ht="32.25" customHeight="1">
-      <c r="B38" s="82" t="s">
-        <v>313</v>
-      </c>
-      <c r="C38" s="82"/>
+      <c r="B38" s="87" t="s">
+        <v>304</v>
+      </c>
+      <c r="C38" s="87"/>
     </row>
     <row r="39" spans="2:3" ht="15.75" thickBot="1">
       <c r="B39" s="52" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
       <c r="C39" s="49"/>
     </row>
     <row r="40" spans="2:3" ht="15.75" thickBot="1">
       <c r="B40" s="46" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="C40" s="2"/>
     </row>
     <row r="41" spans="2:3" ht="15.75" thickBot="1">
       <c r="B41" s="46" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
     </row>
     <row r="42" spans="2:3" ht="15.75" thickBot="1">
       <c r="B42" s="46" t="s">
-        <v>317</v>
+        <v>308</v>
       </c>
     </row>
     <row r="43" spans="2:3" ht="15.75" thickBot="1">
       <c r="B43" s="46" t="s">
-        <v>318</v>
+        <v>309</v>
       </c>
     </row>
     <row r="44" spans="2:3" ht="15.75" thickBot="1">
       <c r="B44" s="46" t="s">
-        <v>319</v>
+        <v>310</v>
       </c>
     </row>
     <row r="45" spans="2:3" ht="15.75" thickBot="1">
       <c r="B45" s="46" t="s">
-        <v>320</v>
+        <v>311</v>
       </c>
     </row>
     <row r="46" spans="2:3" ht="15.75" thickBot="1">
       <c r="B46" s="46" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
     </row>
     <row r="47" spans="2:3">
       <c r="B47" s="50" t="s">
-        <v>322</v>
+        <v>313</v>
       </c>
     </row>
     <row r="48" spans="2:3" ht="36" customHeight="1">
-      <c r="B48" s="82" t="s">
-        <v>323</v>
-      </c>
-      <c r="C48" s="82"/>
+      <c r="B48" s="87" t="s">
+        <v>314</v>
+      </c>
+      <c r="C48" s="87"/>
     </row>
     <row r="49" spans="2:3" ht="49.5" customHeight="1">
-      <c r="B49" s="82" t="s">
-        <v>324</v>
-      </c>
-      <c r="C49" s="82"/>
+      <c r="B49" s="87" t="s">
+        <v>315</v>
+      </c>
+      <c r="C49" s="87"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Commit the immutability object.
</commit_message>
<xml_diff>
--- a/Training_Plan.xlsx
+++ b/Training_Plan.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="45" windowWidth="19155" windowHeight="11760" activeTab="1"/>
@@ -16,12 +16,12 @@
   <definedNames>
     <definedName name="jaxrs_intro" localSheetId="3">'RESTful WS'!$B$6</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="442">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="454">
   <si>
     <t>Java core</t>
   </si>
@@ -7876,12 +7876,308 @@
     <t>1. Making shared object immutable in order to make sure that it's never updated by any of threads.
 2. synchronization</t>
   </si>
+  <si>
+    <t xml:space="preserve">Benefits of making a class immutable?
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - are simple to construct, test, and use
+  - are automatically thread-safe and have no synchronization issues
+  - do not need a copy constructor
+  - do not need an implementation of clone
+  - allow hashCode to use lazy initialization, and to cache its return value
+  - do not need to be copied defensively when used as a field
+  - make good Map keys and Set elements (these objects must not change state while in the collection)
+  - have their class invariant established once upon construction, and it never needs to be checked again
+  - always have “failure atomicity” (a term used by Joshua Bloch) : if an  immutable object throws an exception, it’s never left in an undesirable or indeterminate state</t>
+  </si>
+  <si>
+    <t>This principle says that for all mutable properties in your class, do not provide setter methods. Setter methods are meant to change the state of object and this is what we want to prevent here.</t>
+  </si>
+  <si>
+    <t>Guidelines to make a class immutable</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Don’t</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> provide </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>“setter”</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> methods — methods that modify fields or objects referred to by fields.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>2) Make</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> all fields</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>final</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>private</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>This is another way to increase immutability. Fields declared private will not be accessible outside the class and</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> making them final will ensure the even accidentally you can not change them.</t>
+    </r>
+  </si>
+  <si>
+    <t>The simplest way to do this is to declare the class as final. Final classes in java can not be overridden.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">3) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Don’t</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>allow</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> subclasses to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>override methods</t>
+    </r>
+  </si>
+  <si>
+    <t>4) Special attention when having mutable instance variables</t>
+  </si>
+  <si>
+    <r>
+      <t>A more sophisticated approach is to make the constructor </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF222222"/>
+        <rFont val="Inherit"/>
+      </rPr>
+      <t>private</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> and construct instances in </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>factory methods</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Always remember that your instance variables will be either </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>mutable or immutable</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. Identify them and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>return new objects with copied content for all mutable objects.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Immutable variables can be returned safely without extra effort.</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="29">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="32">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -8090,6 +8386,26 @@
       <name val="Arial Unicode MS"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF222222"/>
+      <name val="Inherit"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -8270,7 +8586,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -8451,6 +8767,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -8481,6 +8800,7 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -8501,13 +8821,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>47624</xdr:colOff>
-      <xdr:row>94</xdr:row>
+      <xdr:row>101</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>85724</xdr:colOff>
-      <xdr:row>104</xdr:row>
+      <xdr:row>111</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -8545,13 +8865,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>752475</xdr:colOff>
-      <xdr:row>146</xdr:row>
+      <xdr:row>153</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>3019425</xdr:colOff>
-      <xdr:row>185</xdr:row>
+      <xdr:row>192</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -8715,6 +9035,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -8749,6 +9070,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -8924,7 +9246,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J30"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
@@ -9390,11 +9712,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:E155"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:E162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B77" workbookViewId="0">
-      <selection activeCell="E83" sqref="E83"/>
+    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
+      <selection activeCell="D89" sqref="D89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9645,10 +9967,10 @@
     <row r="27" spans="2:5">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
-      <c r="D27" s="78" t="s">
+      <c r="D27" s="79" t="s">
         <v>47</v>
       </c>
-      <c r="E27" s="79"/>
+      <c r="E27" s="80"/>
     </row>
     <row r="28" spans="2:5">
       <c r="B28" s="2"/>
@@ -9711,10 +10033,10 @@
     <row r="34" spans="2:5">
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
-      <c r="D34" s="82" t="s">
+      <c r="D34" s="83" t="s">
         <v>78</v>
       </c>
-      <c r="E34" s="82"/>
+      <c r="E34" s="83"/>
     </row>
     <row r="35" spans="2:5">
       <c r="B35" s="2"/>
@@ -9777,10 +10099,10 @@
     <row r="41" spans="2:5">
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
-      <c r="D41" s="83" t="s">
+      <c r="D41" s="84" t="s">
         <v>86</v>
       </c>
-      <c r="E41" s="84"/>
+      <c r="E41" s="85"/>
     </row>
     <row r="42" spans="2:5">
       <c r="B42" s="2"/>
@@ -9867,10 +10189,10 @@
     <row r="50" spans="2:5">
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
-      <c r="D50" s="80" t="s">
+      <c r="D50" s="81" t="s">
         <v>60</v>
       </c>
-      <c r="E50" s="80"/>
+      <c r="E50" s="81"/>
     </row>
     <row r="51" spans="2:5">
       <c r="B51" s="2"/>
@@ -9918,7 +10240,7 @@
       <c r="D55" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="E55" s="81" t="s">
+      <c r="E55" s="82" t="s">
         <v>71</v>
       </c>
     </row>
@@ -9928,7 +10250,7 @@
       <c r="D56" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="E56" s="81"/>
+      <c r="E56" s="82"/>
     </row>
     <row r="57" spans="2:5">
       <c r="B57" s="2"/>
@@ -10146,481 +10468,491 @@
         <v>441</v>
       </c>
     </row>
-    <row r="83" spans="2:5" ht="225">
-      <c r="B83" s="2"/>
+    <row r="83" spans="2:5" ht="205.5" customHeight="1">
+      <c r="B83" s="32"/>
       <c r="C83" s="2"/>
-      <c r="D83" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="E83" s="21" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="84" spans="2:5">
-      <c r="B84" s="2"/>
-      <c r="C84" s="2"/>
-      <c r="D84" s="2"/>
-      <c r="E84" s="74"/>
-    </row>
-    <row r="85" spans="2:5" ht="30">
-      <c r="B85" s="2"/>
+      <c r="D83" s="78" t="s">
+        <v>442</v>
+      </c>
+      <c r="E83" s="13" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="84" spans="2:5" ht="35.25" customHeight="1">
+      <c r="B84" s="32"/>
+      <c r="C84" s="22" t="s">
+        <v>445</v>
+      </c>
+      <c r="D84" s="78"/>
+      <c r="E84" s="13"/>
+    </row>
+    <row r="85" spans="2:5" ht="52.5" customHeight="1">
+      <c r="B85" s="32"/>
       <c r="C85" s="2"/>
-      <c r="D85" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="E85" s="17" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="86" spans="2:5" ht="90">
-      <c r="B86" s="2"/>
+      <c r="D85" s="78" t="s">
+        <v>446</v>
+      </c>
+      <c r="E85" s="13" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="86" spans="2:5" ht="52.5" customHeight="1">
+      <c r="B86" s="32"/>
       <c r="C86" s="2"/>
-      <c r="D86" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="E86" s="17" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="87" spans="2:5" ht="45">
-      <c r="B87" s="2"/>
+      <c r="D86" s="78" t="s">
+        <v>447</v>
+      </c>
+      <c r="E86" s="13" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="87" spans="2:5" ht="36" customHeight="1">
+      <c r="B87" s="32"/>
       <c r="C87" s="2"/>
-      <c r="D87" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="E87" s="21" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="88" spans="2:5" ht="60">
-      <c r="B88" s="2"/>
+      <c r="D87" s="78" t="s">
+        <v>450</v>
+      </c>
+      <c r="E87" s="13" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="88" spans="2:5" ht="67.5" customHeight="1">
+      <c r="B88" s="32"/>
       <c r="C88" s="2"/>
-      <c r="D88" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="E88" s="21" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="89" spans="2:5" ht="90">
-      <c r="B89" s="2"/>
+      <c r="D88" s="78" t="s">
+        <v>451</v>
+      </c>
+      <c r="E88" s="13" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="89" spans="2:5" ht="31.5">
+      <c r="B89" s="32"/>
       <c r="C89" s="2"/>
-      <c r="D89" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="E89" s="21" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="90" spans="2:5" ht="30">
+      <c r="D89" s="89" t="s">
+        <v>452</v>
+      </c>
+      <c r="E89" s="13"/>
+    </row>
+    <row r="90" spans="2:5" ht="225">
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
       <c r="D90" s="2" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="E90" s="21" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="91" spans="2:5" ht="30">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="91" spans="2:5">
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
-      <c r="D91" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="E91" s="21" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="92" spans="2:5" ht="60">
+      <c r="D91" s="2"/>
+      <c r="E91" s="74"/>
+    </row>
+    <row r="92" spans="2:5" ht="30">
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
       <c r="D92" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="E92" s="21" t="s">
-        <v>136</v>
+        <v>122</v>
+      </c>
+      <c r="E92" s="17" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="93" spans="2:5" ht="90">
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
       <c r="D93" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="E93" s="21" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="94" spans="2:5" ht="60">
+        <v>121</v>
+      </c>
+      <c r="E93" s="17" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="94" spans="2:5" ht="45">
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
       <c r="D94" s="2" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="E94" s="21" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="95" spans="2:5">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="95" spans="2:5" ht="60">
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
-      <c r="D95" s="2"/>
-      <c r="E95" s="21"/>
-    </row>
-    <row r="96" spans="2:5">
+      <c r="D95" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="E95" s="21" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="96" spans="2:5" ht="90">
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
-      <c r="D96" s="2"/>
-      <c r="E96" s="21"/>
-    </row>
-    <row r="97" spans="2:5">
+      <c r="D96" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E96" s="21" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="97" spans="2:5" ht="30">
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
-      <c r="D97" s="2"/>
-      <c r="E97" s="21"/>
-    </row>
-    <row r="98" spans="2:5">
+      <c r="D97" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E97" s="21" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="98" spans="2:5" ht="30">
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
-      <c r="D98" s="2"/>
-      <c r="E98" s="21"/>
-    </row>
-    <row r="99" spans="2:5">
+      <c r="D98" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E98" s="21" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="99" spans="2:5" ht="60">
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
-      <c r="D99" s="2"/>
-      <c r="E99" s="21"/>
-    </row>
-    <row r="100" spans="2:5">
+      <c r="D99" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E99" s="21" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="100" spans="2:5" ht="90">
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
-      <c r="D100" s="2"/>
-      <c r="E100" s="21"/>
-    </row>
-    <row r="101" spans="2:5">
+      <c r="D100" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="E100" s="21" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="101" spans="2:5" ht="60">
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
-      <c r="D101" s="2"/>
-      <c r="E101" s="26"/>
+      <c r="D101" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E101" s="21" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="102" spans="2:5">
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
       <c r="D102" s="2"/>
-      <c r="E102" s="2"/>
+      <c r="E102" s="21"/>
     </row>
     <row r="103" spans="2:5">
       <c r="B103" s="2"/>
       <c r="C103" s="2"/>
       <c r="D103" s="2"/>
-      <c r="E103" s="2"/>
+      <c r="E103" s="21"/>
     </row>
     <row r="104" spans="2:5">
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
       <c r="D104" s="2"/>
-      <c r="E104" s="2"/>
+      <c r="E104" s="21"/>
     </row>
     <row r="105" spans="2:5">
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
       <c r="D105" s="2"/>
-      <c r="E105" s="2"/>
-    </row>
-    <row r="106" spans="2:5" ht="60">
+      <c r="E105" s="21"/>
+    </row>
+    <row r="106" spans="2:5">
       <c r="B106" s="2"/>
       <c r="C106" s="2"/>
-      <c r="D106" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="E106" s="26" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="107" spans="2:5" ht="75">
+      <c r="D106" s="2"/>
+      <c r="E106" s="21"/>
+    </row>
+    <row r="107" spans="2:5">
       <c r="B107" s="2"/>
       <c r="C107" s="2"/>
-      <c r="D107" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="E107" s="26" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="108" spans="2:5" ht="60">
+      <c r="D107" s="2"/>
+      <c r="E107" s="21"/>
+    </row>
+    <row r="108" spans="2:5">
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
-      <c r="D108" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="E108" s="26" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="109" spans="2:5" ht="45">
+      <c r="D108" s="2"/>
+      <c r="E108" s="26"/>
+    </row>
+    <row r="109" spans="2:5">
       <c r="B109" s="2"/>
       <c r="C109" s="2"/>
-      <c r="D109" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="E109" s="26" t="s">
-        <v>159</v>
-      </c>
+      <c r="D109" s="2"/>
+      <c r="E109" s="2"/>
     </row>
     <row r="110" spans="2:5">
       <c r="B110" s="2"/>
       <c r="C110" s="2"/>
-      <c r="D110" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="E110" s="26" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="111" spans="2:5" ht="75">
+      <c r="D110" s="2"/>
+      <c r="E110" s="2"/>
+    </row>
+    <row r="111" spans="2:5">
       <c r="B111" s="2"/>
       <c r="C111" s="2"/>
-      <c r="D111" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="E111" s="26" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="112" spans="2:5" ht="45">
+      <c r="D111" s="2"/>
+      <c r="E111" s="2"/>
+    </row>
+    <row r="112" spans="2:5">
       <c r="B112" s="2"/>
-      <c r="C112" s="32" t="s">
-        <v>425</v>
-      </c>
+      <c r="C112" s="2"/>
       <c r="D112" s="2"/>
-      <c r="E112" s="40" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="113" spans="2:5" ht="31.5">
+      <c r="E112" s="2"/>
+    </row>
+    <row r="113" spans="2:5" ht="60">
       <c r="B113" s="2"/>
-      <c r="C113" s="22"/>
-      <c r="D113" s="2"/>
-      <c r="E113" s="74"/>
-    </row>
-    <row r="114" spans="2:5" ht="135">
+      <c r="C113" s="2"/>
+      <c r="D113" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E113" s="26" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="114" spans="2:5" ht="75">
       <c r="B114" s="2"/>
       <c r="C114" s="2"/>
       <c r="D114" s="2" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="E114" s="26" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="115" spans="2:5" ht="90">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="115" spans="2:5" ht="60">
       <c r="B115" s="2"/>
       <c r="C115" s="2"/>
       <c r="D115" s="2" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="E115" s="26" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
     </row>
     <row r="116" spans="2:5" ht="45">
       <c r="B116" s="2"/>
       <c r="C116" s="2"/>
       <c r="D116" s="2" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="E116" s="26" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
     </row>
     <row r="117" spans="2:5">
       <c r="B117" s="2"/>
       <c r="C117" s="2"/>
       <c r="D117" s="2" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="E117" s="26" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="118" spans="2:5" ht="30">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="118" spans="2:5" ht="75">
       <c r="B118" s="2"/>
       <c r="C118" s="2"/>
-      <c r="D118" s="26" t="s">
-        <v>172</v>
+      <c r="D118" s="2" t="s">
+        <v>162</v>
       </c>
       <c r="E118" s="26" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="119" spans="2:5">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="119" spans="2:5" ht="45">
       <c r="B119" s="2"/>
-      <c r="C119" s="2"/>
-      <c r="D119" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="E119" s="26"/>
-    </row>
-    <row r="120" spans="2:5">
+      <c r="C119" s="32" t="s">
+        <v>425</v>
+      </c>
+      <c r="D119" s="2"/>
+      <c r="E119" s="40" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="120" spans="2:5" ht="31.5">
       <c r="B120" s="2"/>
-      <c r="C120" s="2"/>
-      <c r="D120" s="15" t="s">
-        <v>175</v>
-      </c>
-      <c r="E120" s="15" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="121" spans="2:5">
+      <c r="C120" s="22"/>
+      <c r="D120" s="2"/>
+      <c r="E120" s="74"/>
+    </row>
+    <row r="121" spans="2:5" ht="135">
       <c r="B121" s="2"/>
       <c r="C121" s="2"/>
-      <c r="D121" s="26" t="s">
-        <v>177</v>
+      <c r="D121" s="2" t="s">
+        <v>164</v>
       </c>
       <c r="E121" s="26" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="122" spans="2:5">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="122" spans="2:5" ht="90">
       <c r="B122" s="2"/>
       <c r="C122" s="2"/>
-      <c r="D122" s="26" t="s">
-        <v>179</v>
+      <c r="D122" s="2" t="s">
+        <v>166</v>
       </c>
       <c r="E122" s="26" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="123" spans="2:5">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="123" spans="2:5" ht="45">
       <c r="B123" s="2"/>
       <c r="C123" s="2"/>
-      <c r="D123" s="26" t="s">
-        <v>181</v>
+      <c r="D123" s="2" t="s">
+        <v>168</v>
       </c>
       <c r="E123" s="26" t="s">
-        <v>182</v>
+        <v>169</v>
       </c>
     </row>
     <row r="124" spans="2:5">
       <c r="B124" s="2"/>
       <c r="C124" s="2"/>
-      <c r="D124" s="26" t="s">
-        <v>183</v>
+      <c r="D124" s="2" t="s">
+        <v>170</v>
       </c>
       <c r="E124" s="26" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="125" spans="2:5" ht="31.5">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="125" spans="2:5" ht="30">
       <c r="B125" s="2"/>
-      <c r="C125" s="22" t="s">
-        <v>185</v>
-      </c>
-      <c r="D125" s="2"/>
-      <c r="E125" s="26"/>
-    </row>
-    <row r="126" spans="2:5" ht="105">
+      <c r="C125" s="2"/>
+      <c r="D125" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="E125" s="26" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="126" spans="2:5">
       <c r="B126" s="2"/>
       <c r="C126" s="2"/>
       <c r="D126" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="E126" s="74" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="127" spans="2:5" ht="120">
+        <v>174</v>
+      </c>
+      <c r="E126" s="26"/>
+    </row>
+    <row r="127" spans="2:5">
       <c r="B127" s="2"/>
       <c r="C127" s="2"/>
-      <c r="D127" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="E127" s="74" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="128" spans="2:5" ht="255">
+      <c r="D127" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="E127" s="15" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="128" spans="2:5">
       <c r="B128" s="2"/>
       <c r="C128" s="2"/>
-      <c r="D128" s="2" t="s">
-        <v>188</v>
+      <c r="D128" s="26" t="s">
+        <v>177</v>
       </c>
       <c r="E128" s="26" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="129" spans="2:5" ht="180">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="129" spans="2:5">
       <c r="B129" s="2"/>
       <c r="C129" s="2"/>
-      <c r="D129" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="E129" s="28" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="130" spans="2:5" ht="30">
+      <c r="D129" s="26" t="s">
+        <v>179</v>
+      </c>
+      <c r="E129" s="26" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="130" spans="2:5">
       <c r="B130" s="2"/>
       <c r="C130" s="2"/>
-      <c r="D130" s="28" t="s">
-        <v>195</v>
-      </c>
-      <c r="E130" s="28"/>
-    </row>
-    <row r="131" spans="2:5" ht="30">
+      <c r="D130" s="26" t="s">
+        <v>181</v>
+      </c>
+      <c r="E130" s="26" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="131" spans="2:5">
       <c r="B131" s="2"/>
       <c r="C131" s="2"/>
-      <c r="D131" s="28" t="s">
-        <v>196</v>
-      </c>
-      <c r="E131" s="28"/>
-    </row>
-    <row r="132" spans="2:5" ht="30">
+      <c r="D131" s="26" t="s">
+        <v>183</v>
+      </c>
+      <c r="E131" s="26" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="132" spans="2:5" ht="31.5">
       <c r="B132" s="2"/>
-      <c r="C132" s="2"/>
-      <c r="D132" s="28" t="s">
-        <v>198</v>
-      </c>
-      <c r="E132" s="28"/>
-    </row>
-    <row r="133" spans="2:5" ht="45">
+      <c r="C132" s="22" t="s">
+        <v>185</v>
+      </c>
+      <c r="D132" s="2"/>
+      <c r="E132" s="26"/>
+    </row>
+    <row r="133" spans="2:5" ht="105">
       <c r="B133" s="2"/>
       <c r="C133" s="2"/>
-      <c r="D133" s="28" t="s">
-        <v>192</v>
-      </c>
-      <c r="E133" s="28"/>
-    </row>
-    <row r="134" spans="2:5">
+      <c r="D133" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="E133" s="74" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="134" spans="2:5" ht="120">
       <c r="B134" s="2"/>
       <c r="C134" s="2"/>
-      <c r="D134" s="28" t="s">
-        <v>199</v>
-      </c>
-      <c r="E134" s="28"/>
-    </row>
-    <row r="135" spans="2:5" ht="60">
+      <c r="D134" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="E134" s="74" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="135" spans="2:5" ht="255">
       <c r="B135" s="2"/>
       <c r="C135" s="2"/>
-      <c r="D135" s="28" t="s">
-        <v>200</v>
-      </c>
-      <c r="E135" s="28"/>
-    </row>
-    <row r="136" spans="2:5" ht="30">
+      <c r="D135" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="E135" s="26" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="136" spans="2:5" ht="180">
       <c r="B136" s="2"/>
       <c r="C136" s="2"/>
-      <c r="D136" s="28" t="s">
-        <v>201</v>
-      </c>
-      <c r="E136" s="28"/>
-    </row>
-    <row r="137" spans="2:5">
+      <c r="D136" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="E136" s="28" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="137" spans="2:5" ht="30">
       <c r="B137" s="2"/>
       <c r="C137" s="2"/>
       <c r="D137" s="28" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="E137" s="28"/>
     </row>
@@ -10628,7 +10960,7 @@
       <c r="B138" s="2"/>
       <c r="C138" s="2"/>
       <c r="D138" s="28" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="E138" s="28"/>
     </row>
@@ -10636,102 +10968,116 @@
       <c r="B139" s="2"/>
       <c r="C139" s="2"/>
       <c r="D139" s="28" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="E139" s="28"/>
     </row>
-    <row r="140" spans="2:5">
+    <row r="140" spans="2:5" ht="45">
       <c r="B140" s="2"/>
       <c r="C140" s="2"/>
-      <c r="D140" s="28"/>
-      <c r="E140" s="26"/>
-    </row>
-    <row r="142" spans="2:5" ht="31.5">
-      <c r="C142" s="22" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="143" spans="2:5" ht="90">
+      <c r="D140" s="28" t="s">
+        <v>192</v>
+      </c>
+      <c r="E140" s="28"/>
+    </row>
+    <row r="141" spans="2:5">
+      <c r="B141" s="2"/>
+      <c r="C141" s="2"/>
+      <c r="D141" s="28" t="s">
+        <v>199</v>
+      </c>
+      <c r="E141" s="28"/>
+    </row>
+    <row r="142" spans="2:5" ht="60">
+      <c r="B142" s="2"/>
+      <c r="C142" s="2"/>
+      <c r="D142" s="28" t="s">
+        <v>200</v>
+      </c>
+      <c r="E142" s="28"/>
+    </row>
+    <row r="143" spans="2:5" ht="30">
       <c r="B143" s="2"/>
       <c r="C143" s="2"/>
-      <c r="D143" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="E143" s="21" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="144" spans="2:5" ht="90">
+      <c r="D143" s="28" t="s">
+        <v>201</v>
+      </c>
+      <c r="E143" s="28"/>
+    </row>
+    <row r="144" spans="2:5">
       <c r="B144" s="2"/>
       <c r="C144" s="2"/>
       <c r="D144" s="28" t="s">
-        <v>146</v>
-      </c>
-      <c r="E144" s="21" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="145" spans="2:5" ht="105">
+        <v>202</v>
+      </c>
+      <c r="E144" s="28"/>
+    </row>
+    <row r="145" spans="2:5" ht="30">
       <c r="B145" s="2"/>
       <c r="C145" s="2"/>
-      <c r="D145" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="E145" s="21" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="146" spans="2:5" ht="90">
+      <c r="D145" s="28" t="s">
+        <v>193</v>
+      </c>
+      <c r="E145" s="28"/>
+    </row>
+    <row r="146" spans="2:5" ht="30">
       <c r="B146" s="2"/>
       <c r="C146" s="2"/>
-      <c r="D146" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="E146" s="21" t="s">
-        <v>149</v>
-      </c>
+      <c r="D146" s="28" t="s">
+        <v>194</v>
+      </c>
+      <c r="E146" s="28"/>
     </row>
     <row r="147" spans="2:5">
       <c r="B147" s="2"/>
       <c r="C147" s="2"/>
-      <c r="D147" s="2"/>
-      <c r="E147" s="21"/>
-    </row>
-    <row r="148" spans="2:5">
-      <c r="B148" s="2"/>
-      <c r="C148" s="2"/>
-      <c r="D148" s="2"/>
-      <c r="E148" s="21"/>
-    </row>
-    <row r="149" spans="2:5">
-      <c r="B149" s="2"/>
-      <c r="C149" s="2"/>
-      <c r="D149" s="2"/>
-      <c r="E149" s="21"/>
-    </row>
-    <row r="150" spans="2:5">
+      <c r="D147" s="28"/>
+      <c r="E147" s="26"/>
+    </row>
+    <row r="149" spans="2:5" ht="31.5">
+      <c r="C149" s="22" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="150" spans="2:5" ht="90">
       <c r="B150" s="2"/>
       <c r="C150" s="2"/>
-      <c r="D150" s="2"/>
-      <c r="E150" s="21"/>
-    </row>
-    <row r="151" spans="2:5">
+      <c r="D150" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E150" s="21" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="151" spans="2:5" ht="90">
       <c r="B151" s="2"/>
       <c r="C151" s="2"/>
-      <c r="D151" s="2"/>
-      <c r="E151" s="21"/>
-    </row>
-    <row r="152" spans="2:5">
+      <c r="D151" s="28" t="s">
+        <v>146</v>
+      </c>
+      <c r="E151" s="21" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="152" spans="2:5" ht="105">
       <c r="B152" s="2"/>
       <c r="C152" s="2"/>
-      <c r="D152" s="2"/>
-      <c r="E152" s="21"/>
-    </row>
-    <row r="153" spans="2:5">
+      <c r="D152" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="E152" s="21" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="153" spans="2:5" ht="90">
       <c r="B153" s="2"/>
       <c r="C153" s="2"/>
-      <c r="D153" s="2"/>
-      <c r="E153" s="21"/>
+      <c r="D153" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E153" s="21" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="154" spans="2:5">
       <c r="B154" s="2"/>
@@ -10740,7 +11086,49 @@
       <c r="E154" s="21"/>
     </row>
     <row r="155" spans="2:5">
-      <c r="E155" s="27"/>
+      <c r="B155" s="2"/>
+      <c r="C155" s="2"/>
+      <c r="D155" s="2"/>
+      <c r="E155" s="21"/>
+    </row>
+    <row r="156" spans="2:5">
+      <c r="B156" s="2"/>
+      <c r="C156" s="2"/>
+      <c r="D156" s="2"/>
+      <c r="E156" s="21"/>
+    </row>
+    <row r="157" spans="2:5">
+      <c r="B157" s="2"/>
+      <c r="C157" s="2"/>
+      <c r="D157" s="2"/>
+      <c r="E157" s="21"/>
+    </row>
+    <row r="158" spans="2:5">
+      <c r="B158" s="2"/>
+      <c r="C158" s="2"/>
+      <c r="D158" s="2"/>
+      <c r="E158" s="21"/>
+    </row>
+    <row r="159" spans="2:5">
+      <c r="B159" s="2"/>
+      <c r="C159" s="2"/>
+      <c r="D159" s="2"/>
+      <c r="E159" s="21"/>
+    </row>
+    <row r="160" spans="2:5">
+      <c r="B160" s="2"/>
+      <c r="C160" s="2"/>
+      <c r="D160" s="2"/>
+      <c r="E160" s="21"/>
+    </row>
+    <row r="161" spans="2:5">
+      <c r="B161" s="2"/>
+      <c r="C161" s="2"/>
+      <c r="D161" s="2"/>
+      <c r="E161" s="21"/>
+    </row>
+    <row r="162" spans="2:5">
+      <c r="E162" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -10757,7 +11145,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:C13"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
@@ -10853,7 +11241,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:C102"/>
   <sheetViews>
     <sheetView topLeftCell="A79" workbookViewId="0">
@@ -11138,27 +11526,27 @@
       </c>
     </row>
     <row r="49" spans="1:3">
-      <c r="A49" s="81" t="s">
+      <c r="A49" s="82" t="s">
         <v>338</v>
       </c>
       <c r="B49" s="53" t="s">
         <v>339</v>
       </c>
-      <c r="C49" s="81" t="s">
+      <c r="C49" s="82" t="s">
         <v>341</v>
       </c>
     </row>
     <row r="50" spans="1:3">
-      <c r="A50" s="81"/>
+      <c r="A50" s="82"/>
       <c r="B50" s="53"/>
-      <c r="C50" s="81"/>
+      <c r="C50" s="82"/>
     </row>
     <row r="51" spans="1:3">
-      <c r="A51" s="81"/>
+      <c r="A51" s="82"/>
       <c r="B51" s="53" t="s">
         <v>340</v>
       </c>
-      <c r="C51" s="81"/>
+      <c r="C51" s="82"/>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="53" t="s">
@@ -11188,22 +11576,22 @@
       <c r="B56" s="58"/>
     </row>
     <row r="57" spans="1:3" ht="32.25" customHeight="1">
-      <c r="B57" s="85" t="s">
+      <c r="B57" s="86" t="s">
         <v>347</v>
       </c>
-      <c r="C57" s="85"/>
+      <c r="C57" s="86"/>
     </row>
     <row r="58" spans="1:3" ht="33" customHeight="1">
-      <c r="B58" s="85" t="s">
+      <c r="B58" s="86" t="s">
         <v>348</v>
       </c>
-      <c r="C58" s="85"/>
+      <c r="C58" s="86"/>
     </row>
     <row r="59" spans="1:3" ht="19.5" customHeight="1">
-      <c r="B59" s="85" t="s">
+      <c r="B59" s="86" t="s">
         <v>349</v>
       </c>
-      <c r="C59" s="85"/>
+      <c r="C59" s="86"/>
     </row>
     <row r="60" spans="1:3">
       <c r="B60" s="2" t="s">
@@ -11247,7 +11635,7 @@
       </c>
       <c r="C66" s="37"/>
     </row>
-    <row r="67" spans="2:3" ht="30.75">
+    <row r="67" spans="2:3" ht="30">
       <c r="B67" s="63" t="s">
         <v>356</v>
       </c>
@@ -11263,7 +11651,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="69" spans="2:3" ht="105.75">
+    <row r="69" spans="2:3" ht="105">
       <c r="B69" s="63" t="s">
         <v>359</v>
       </c>
@@ -11295,7 +11683,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="73" spans="2:3" ht="30.75">
+    <row r="73" spans="2:3" ht="30">
       <c r="B73" s="63" t="s">
         <v>368</v>
       </c>
@@ -11335,7 +11723,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="78" spans="2:3" ht="30.75">
+    <row r="78" spans="2:3" ht="30">
       <c r="B78" s="67" t="s">
         <v>378</v>
       </c>
@@ -11416,10 +11804,10 @@
       <c r="C87" s="76"/>
     </row>
     <row r="88" spans="1:3" ht="51" customHeight="1">
-      <c r="B88" s="85" t="s">
+      <c r="B88" s="86" t="s">
         <v>400</v>
       </c>
-      <c r="C88" s="85"/>
+      <c r="C88" s="86"/>
     </row>
     <row r="89" spans="1:3" ht="31.5">
       <c r="B89" s="22" t="s">
@@ -11430,13 +11818,13 @@
       <c r="A90" t="s">
         <v>402</v>
       </c>
-      <c r="B90" s="85" t="s">
+      <c r="B90" s="86" t="s">
         <v>401</v>
       </c>
-      <c r="C90" s="85"/>
+      <c r="C90" s="86"/>
     </row>
     <row r="91" spans="1:3" ht="45.75" customHeight="1">
-      <c r="A91" s="86" t="s">
+      <c r="A91" s="87" t="s">
         <v>405</v>
       </c>
       <c r="B91" s="2" t="s">
@@ -11447,7 +11835,7 @@
       </c>
     </row>
     <row r="92" spans="1:3" ht="30">
-      <c r="A92" s="86"/>
+      <c r="A92" s="87"/>
       <c r="B92" s="2" t="s">
         <v>408</v>
       </c>
@@ -11545,7 +11933,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C49"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
@@ -11748,16 +12136,16 @@
       <c r="C25" s="37"/>
     </row>
     <row r="26" spans="2:3" ht="33" customHeight="1">
-      <c r="B26" s="87" t="s">
+      <c r="B26" s="88" t="s">
         <v>294</v>
       </c>
-      <c r="C26" s="87"/>
+      <c r="C26" s="88"/>
     </row>
     <row r="27" spans="2:3">
-      <c r="B27" s="87" t="s">
+      <c r="B27" s="88" t="s">
         <v>295</v>
       </c>
-      <c r="C27" s="87"/>
+      <c r="C27" s="88"/>
     </row>
     <row r="28" spans="2:3" ht="15.75" thickBot="1">
       <c r="B28" s="48" t="s">
@@ -11812,16 +12200,16 @@
       <c r="C36" s="51"/>
     </row>
     <row r="37" spans="2:3" ht="50.25" customHeight="1">
-      <c r="B37" s="87" t="s">
+      <c r="B37" s="88" t="s">
         <v>303</v>
       </c>
-      <c r="C37" s="87"/>
+      <c r="C37" s="88"/>
     </row>
     <row r="38" spans="2:3" ht="32.25" customHeight="1">
-      <c r="B38" s="87" t="s">
+      <c r="B38" s="88" t="s">
         <v>304</v>
       </c>
-      <c r="C38" s="87"/>
+      <c r="C38" s="88"/>
     </row>
     <row r="39" spans="2:3" ht="15.75" thickBot="1">
       <c r="B39" s="52" t="s">
@@ -11871,16 +12259,16 @@
       </c>
     </row>
     <row r="48" spans="2:3" ht="36" customHeight="1">
-      <c r="B48" s="87" t="s">
+      <c r="B48" s="88" t="s">
         <v>314</v>
       </c>
-      <c r="C48" s="87"/>
+      <c r="C48" s="88"/>
     </row>
     <row r="49" spans="2:3" ht="49.5" customHeight="1">
-      <c r="B49" s="87" t="s">
+      <c r="B49" s="88" t="s">
         <v>315</v>
       </c>
-      <c r="C49" s="87"/>
+      <c r="C49" s="88"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Understand final, private constructor and deep-copy the mutable variable when creating immutable object.
</commit_message>
<xml_diff>
--- a/Training_Plan.xlsx
+++ b/Training_Plan.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="45" windowWidth="19155" windowHeight="11760" activeTab="1"/>
@@ -16,12 +16,12 @@
   <definedNames>
     <definedName name="jaxrs_intro" localSheetId="3">'RESTful WS'!$B$6</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="454">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="455">
   <si>
     <t>Java core</t>
   </si>
@@ -8003,22 +8003,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>This is another way to increase immutability. Fields declared private will not be accessible outside the class and</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> making them final will ensure the even accidentally you can not change them.</t>
-    </r>
-  </si>
-  <si>
     <t>The simplest way to do this is to declare the class as final. Final classes in java can not be overridden.</t>
   </si>
   <si>
@@ -8126,8 +8110,39 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Always remember that your instance variables will be either </t>
+    <t>making the constructor private and providing createInstance() (factory method) does not help by itself: it is one of few things you should do in order to allow users to actually use the class and its instances while you still have the control of the way instances are created</t>
+  </si>
+  <si>
+    <r>
+      <t>This is another way to increase immutability. Fields declared private will not be accessible outside the class and</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> making them final will ensure the even accidentally you can not change them. 
+Make them final to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>avoid changing state by using reflection</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">- Always remember that your instance variables will be either </t>
     </r>
     <r>
       <rPr>
@@ -8148,7 +8163,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">. Identify them and </t>
+      <t xml:space="preserve">. 
+ - Identify them and </t>
     </r>
     <r>
       <rPr>
@@ -8159,24 +8175,26 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>return new objects with copied content for all mutable objects.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Immutable variables can be returned safely without extra effort.</t>
+      <t xml:space="preserve">return new objects with copied content for all mutable objects (deep-copy) 
+ - A defensive copy of the mutable object must be made any time it's passed into (constructors and set methods) or out of (get methods) the class.
+ - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Immutable variables can be returned safely without extra effort.</t>
     </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="32">
     <font>
       <sz val="11"/>
@@ -8586,7 +8604,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -8770,6 +8788,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -8800,7 +8822,6 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -8821,13 +8842,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>47624</xdr:colOff>
-      <xdr:row>101</xdr:row>
+      <xdr:row>102</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>85724</xdr:colOff>
-      <xdr:row>111</xdr:row>
+      <xdr:row>112</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -8865,13 +8886,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>752475</xdr:colOff>
-      <xdr:row>153</xdr:row>
+      <xdr:row>154</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>3019425</xdr:colOff>
-      <xdr:row>192</xdr:row>
+      <xdr:row>193</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -9035,7 +9056,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -9070,7 +9090,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -9246,7 +9265,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:J30"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
@@ -9712,11 +9731,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E162"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B2:E163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
-      <selection activeCell="D89" sqref="D89"/>
+    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
+      <selection activeCell="D90" sqref="D90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9967,10 +9986,10 @@
     <row r="27" spans="2:5">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
-      <c r="D27" s="79" t="s">
+      <c r="D27" s="81" t="s">
         <v>47</v>
       </c>
-      <c r="E27" s="80"/>
+      <c r="E27" s="82"/>
     </row>
     <row r="28" spans="2:5">
       <c r="B28" s="2"/>
@@ -10033,10 +10052,10 @@
     <row r="34" spans="2:5">
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
-      <c r="D34" s="83" t="s">
+      <c r="D34" s="85" t="s">
         <v>78</v>
       </c>
-      <c r="E34" s="83"/>
+      <c r="E34" s="85"/>
     </row>
     <row r="35" spans="2:5">
       <c r="B35" s="2"/>
@@ -10099,10 +10118,10 @@
     <row r="41" spans="2:5">
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
-      <c r="D41" s="84" t="s">
+      <c r="D41" s="86" t="s">
         <v>86</v>
       </c>
-      <c r="E41" s="85"/>
+      <c r="E41" s="87"/>
     </row>
     <row r="42" spans="2:5">
       <c r="B42" s="2"/>
@@ -10189,10 +10208,10 @@
     <row r="50" spans="2:5">
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
-      <c r="D50" s="81" t="s">
+      <c r="D50" s="83" t="s">
         <v>60</v>
       </c>
-      <c r="E50" s="81"/>
+      <c r="E50" s="83"/>
     </row>
     <row r="51" spans="2:5">
       <c r="B51" s="2"/>
@@ -10240,7 +10259,7 @@
       <c r="D55" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="E55" s="82" t="s">
+      <c r="E55" s="84" t="s">
         <v>71</v>
       </c>
     </row>
@@ -10250,7 +10269,7 @@
       <c r="D56" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="E56" s="82"/>
+      <c r="E56" s="84"/>
     </row>
     <row r="57" spans="2:5">
       <c r="B57" s="2"/>
@@ -10503,158 +10522,160 @@
         <v>447</v>
       </c>
       <c r="E86" s="13" t="s">
-        <v>448</v>
+        <v>453</v>
       </c>
     </row>
     <row r="87" spans="2:5" ht="36" customHeight="1">
       <c r="B87" s="32"/>
       <c r="C87" s="2"/>
       <c r="D87" s="78" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="E87" s="13" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="88" spans="2:5" ht="67.5" customHeight="1">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="88" spans="2:5" ht="120.75" customHeight="1">
       <c r="B88" s="32"/>
       <c r="C88" s="2"/>
       <c r="D88" s="78" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="E88" s="13" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
     </row>
     <row r="89" spans="2:5" ht="31.5">
       <c r="B89" s="32"/>
       <c r="C89" s="2"/>
-      <c r="D89" s="89" t="s">
+      <c r="D89" s="80" t="s">
+        <v>451</v>
+      </c>
+      <c r="E89" s="13"/>
+    </row>
+    <row r="90" spans="2:5" ht="66" customHeight="1">
+      <c r="B90" s="32"/>
+      <c r="C90" s="2"/>
+      <c r="D90" s="79" t="s">
         <v>452</v>
       </c>
-      <c r="E89" s="13"/>
-    </row>
-    <row r="90" spans="2:5" ht="225">
-      <c r="B90" s="2"/>
-      <c r="C90" s="2"/>
-      <c r="D90" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="E90" s="21" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="91" spans="2:5">
+      <c r="E90" s="13"/>
+    </row>
+    <row r="91" spans="2:5" ht="225">
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
-      <c r="D91" s="2"/>
-      <c r="E91" s="74"/>
-    </row>
-    <row r="92" spans="2:5" ht="30">
+      <c r="D91" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E91" s="21" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="92" spans="2:5">
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
-      <c r="D92" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="E92" s="17" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="93" spans="2:5" ht="90">
+      <c r="D92" s="2"/>
+      <c r="E92" s="74"/>
+    </row>
+    <row r="93" spans="2:5" ht="30">
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
       <c r="D93" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E93" s="17" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="94" spans="2:5" ht="45">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="94" spans="2:5" ht="90">
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
       <c r="D94" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="E94" s="21" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="95" spans="2:5" ht="60">
+        <v>121</v>
+      </c>
+      <c r="E94" s="17" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="95" spans="2:5" ht="45">
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
       <c r="D95" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E95" s="21" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="96" spans="2:5" ht="90">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="96" spans="2:5" ht="60">
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
       <c r="D96" s="2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E96" s="21" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="97" spans="2:5" ht="30">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="97" spans="2:5" ht="90">
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
       <c r="D97" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E97" s="21" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="98" spans="2:5" ht="30">
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
       <c r="D98" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E98" s="21" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="99" spans="2:5" ht="60">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="99" spans="2:5" ht="30">
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
       <c r="D99" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E99" s="21" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="100" spans="2:5" ht="90">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="100" spans="2:5" ht="60">
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
       <c r="D100" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E100" s="21" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="101" spans="2:5" ht="60">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="101" spans="2:5" ht="90">
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
       <c r="D101" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E101" s="21" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="102" spans="2:5">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="102" spans="2:5" ht="60">
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
-      <c r="D102" s="2"/>
-      <c r="E102" s="21"/>
+      <c r="D102" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E102" s="21" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="103" spans="2:5">
       <c r="B103" s="2"/>
@@ -10690,13 +10711,13 @@
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
       <c r="D108" s="2"/>
-      <c r="E108" s="26"/>
+      <c r="E108" s="21"/>
     </row>
     <row r="109" spans="2:5">
       <c r="B109" s="2"/>
       <c r="C109" s="2"/>
       <c r="D109" s="2"/>
-      <c r="E109" s="2"/>
+      <c r="E109" s="26"/>
     </row>
     <row r="110" spans="2:5">
       <c r="B110" s="2"/>
@@ -10716,251 +10737,249 @@
       <c r="D112" s="2"/>
       <c r="E112" s="2"/>
     </row>
-    <row r="113" spans="2:5" ht="60">
+    <row r="113" spans="2:5">
       <c r="B113" s="2"/>
       <c r="C113" s="2"/>
-      <c r="D113" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="E113" s="26" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="114" spans="2:5" ht="75">
+      <c r="D113" s="2"/>
+      <c r="E113" s="2"/>
+    </row>
+    <row r="114" spans="2:5" ht="60">
       <c r="B114" s="2"/>
       <c r="C114" s="2"/>
       <c r="D114" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E114" s="26" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="115" spans="2:5" ht="60">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="115" spans="2:5" ht="75">
       <c r="B115" s="2"/>
       <c r="C115" s="2"/>
       <c r="D115" s="2" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E115" s="26" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="116" spans="2:5" ht="45">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="116" spans="2:5" ht="60">
       <c r="B116" s="2"/>
       <c r="C116" s="2"/>
       <c r="D116" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E116" s="26" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="117" spans="2:5">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="117" spans="2:5" ht="45">
       <c r="B117" s="2"/>
       <c r="C117" s="2"/>
       <c r="D117" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E117" s="26" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="118" spans="2:5" ht="75">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="118" spans="2:5">
       <c r="B118" s="2"/>
       <c r="C118" s="2"/>
       <c r="D118" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="E118" s="26" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="119" spans="2:5" ht="75">
+      <c r="B119" s="2"/>
+      <c r="C119" s="2"/>
+      <c r="D119" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="E118" s="26" t="s">
+      <c r="E119" s="26" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="119" spans="2:5" ht="45">
-      <c r="B119" s="2"/>
-      <c r="C119" s="32" t="s">
+    <row r="120" spans="2:5" ht="45">
+      <c r="B120" s="2"/>
+      <c r="C120" s="32" t="s">
         <v>425</v>
       </c>
-      <c r="D119" s="2"/>
-      <c r="E119" s="40" t="s">
+      <c r="D120" s="2"/>
+      <c r="E120" s="40" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="120" spans="2:5" ht="31.5">
-      <c r="B120" s="2"/>
-      <c r="C120" s="22"/>
-      <c r="D120" s="2"/>
-      <c r="E120" s="74"/>
-    </row>
-    <row r="121" spans="2:5" ht="135">
+    <row r="121" spans="2:5" ht="31.5">
       <c r="B121" s="2"/>
-      <c r="C121" s="2"/>
-      <c r="D121" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="E121" s="26" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="122" spans="2:5" ht="90">
+      <c r="C121" s="22"/>
+      <c r="D121" s="2"/>
+      <c r="E121" s="74"/>
+    </row>
+    <row r="122" spans="2:5" ht="135">
       <c r="B122" s="2"/>
       <c r="C122" s="2"/>
       <c r="D122" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E122" s="26" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="123" spans="2:5" ht="45">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="123" spans="2:5" ht="90">
       <c r="B123" s="2"/>
       <c r="C123" s="2"/>
       <c r="D123" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E123" s="26" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="124" spans="2:5">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="124" spans="2:5" ht="45">
       <c r="B124" s="2"/>
       <c r="C124" s="2"/>
       <c r="D124" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E124" s="26" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="125" spans="2:5" ht="30">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="125" spans="2:5">
       <c r="B125" s="2"/>
       <c r="C125" s="2"/>
-      <c r="D125" s="26" t="s">
-        <v>172</v>
+      <c r="D125" s="2" t="s">
+        <v>170</v>
       </c>
       <c r="E125" s="26" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="126" spans="2:5">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="126" spans="2:5" ht="30">
       <c r="B126" s="2"/>
       <c r="C126" s="2"/>
-      <c r="D126" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="E126" s="26"/>
+      <c r="D126" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="E126" s="26" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="127" spans="2:5">
       <c r="B127" s="2"/>
       <c r="C127" s="2"/>
-      <c r="D127" s="15" t="s">
-        <v>175</v>
-      </c>
-      <c r="E127" s="15" t="s">
-        <v>176</v>
-      </c>
+      <c r="D127" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="E127" s="26"/>
     </row>
     <row r="128" spans="2:5">
       <c r="B128" s="2"/>
       <c r="C128" s="2"/>
-      <c r="D128" s="26" t="s">
-        <v>177</v>
-      </c>
-      <c r="E128" s="26" t="s">
-        <v>178</v>
+      <c r="D128" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="E128" s="15" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="129" spans="2:5">
       <c r="B129" s="2"/>
       <c r="C129" s="2"/>
       <c r="D129" s="26" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E129" s="26" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="130" spans="2:5">
       <c r="B130" s="2"/>
       <c r="C130" s="2"/>
       <c r="D130" s="26" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E130" s="26" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="131" spans="2:5">
       <c r="B131" s="2"/>
       <c r="C131" s="2"/>
       <c r="D131" s="26" t="s">
+        <v>181</v>
+      </c>
+      <c r="E131" s="26" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="132" spans="2:5">
+      <c r="B132" s="2"/>
+      <c r="C132" s="2"/>
+      <c r="D132" s="26" t="s">
         <v>183</v>
       </c>
-      <c r="E131" s="26" t="s">
+      <c r="E132" s="26" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="132" spans="2:5" ht="31.5">
-      <c r="B132" s="2"/>
-      <c r="C132" s="22" t="s">
+    <row r="133" spans="2:5" ht="31.5">
+      <c r="B133" s="2"/>
+      <c r="C133" s="22" t="s">
         <v>185</v>
       </c>
-      <c r="D132" s="2"/>
-      <c r="E132" s="26"/>
-    </row>
-    <row r="133" spans="2:5" ht="105">
-      <c r="B133" s="2"/>
-      <c r="C133" s="2"/>
-      <c r="D133" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="E133" s="74" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="134" spans="2:5" ht="120">
+      <c r="D133" s="2"/>
+      <c r="E133" s="26"/>
+    </row>
+    <row r="134" spans="2:5" ht="105">
       <c r="B134" s="2"/>
       <c r="C134" s="2"/>
       <c r="D134" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E134" s="74" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="135" spans="2:5" ht="255">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="135" spans="2:5" ht="120">
       <c r="B135" s="2"/>
       <c r="C135" s="2"/>
       <c r="D135" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="E135" s="26" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="136" spans="2:5" ht="180">
+        <v>187</v>
+      </c>
+      <c r="E135" s="74" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="136" spans="2:5" ht="255">
       <c r="B136" s="2"/>
       <c r="C136" s="2"/>
       <c r="D136" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="E136" s="28" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="137" spans="2:5" ht="30">
+        <v>188</v>
+      </c>
+      <c r="E136" s="26" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="137" spans="2:5" ht="180">
       <c r="B137" s="2"/>
       <c r="C137" s="2"/>
-      <c r="D137" s="28" t="s">
-        <v>195</v>
-      </c>
-      <c r="E137" s="28"/>
+      <c r="D137" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="E137" s="28" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="138" spans="2:5" ht="30">
       <c r="B138" s="2"/>
       <c r="C138" s="2"/>
       <c r="D138" s="28" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E138" s="28"/>
     </row>
@@ -10968,55 +10987,55 @@
       <c r="B139" s="2"/>
       <c r="C139" s="2"/>
       <c r="D139" s="28" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E139" s="28"/>
     </row>
-    <row r="140" spans="2:5" ht="45">
+    <row r="140" spans="2:5" ht="30">
       <c r="B140" s="2"/>
       <c r="C140" s="2"/>
       <c r="D140" s="28" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="E140" s="28"/>
     </row>
-    <row r="141" spans="2:5">
+    <row r="141" spans="2:5" ht="45">
       <c r="B141" s="2"/>
       <c r="C141" s="2"/>
       <c r="D141" s="28" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="E141" s="28"/>
     </row>
-    <row r="142" spans="2:5" ht="60">
+    <row r="142" spans="2:5">
       <c r="B142" s="2"/>
       <c r="C142" s="2"/>
       <c r="D142" s="28" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E142" s="28"/>
     </row>
-    <row r="143" spans="2:5" ht="30">
+    <row r="143" spans="2:5" ht="60">
       <c r="B143" s="2"/>
       <c r="C143" s="2"/>
       <c r="D143" s="28" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E143" s="28"/>
     </row>
-    <row r="144" spans="2:5">
+    <row r="144" spans="2:5" ht="30">
       <c r="B144" s="2"/>
       <c r="C144" s="2"/>
       <c r="D144" s="28" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E144" s="28"/>
     </row>
-    <row r="145" spans="2:5" ht="30">
+    <row r="145" spans="2:5">
       <c r="B145" s="2"/>
       <c r="C145" s="2"/>
       <c r="D145" s="28" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="E145" s="28"/>
     </row>
@@ -11024,66 +11043,68 @@
       <c r="B146" s="2"/>
       <c r="C146" s="2"/>
       <c r="D146" s="28" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E146" s="28"/>
     </row>
-    <row r="147" spans="2:5">
+    <row r="147" spans="2:5" ht="30">
       <c r="B147" s="2"/>
       <c r="C147" s="2"/>
-      <c r="D147" s="28"/>
-      <c r="E147" s="26"/>
-    </row>
-    <row r="149" spans="2:5" ht="31.5">
-      <c r="C149" s="22" t="s">
+      <c r="D147" s="28" t="s">
+        <v>194</v>
+      </c>
+      <c r="E147" s="28"/>
+    </row>
+    <row r="148" spans="2:5">
+      <c r="B148" s="2"/>
+      <c r="C148" s="2"/>
+      <c r="D148" s="28"/>
+      <c r="E148" s="26"/>
+    </row>
+    <row r="150" spans="2:5" ht="31.5">
+      <c r="C150" s="22" t="s">
         <v>143</v>
-      </c>
-    </row>
-    <row r="150" spans="2:5" ht="90">
-      <c r="B150" s="2"/>
-      <c r="C150" s="2"/>
-      <c r="D150" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="E150" s="21" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="151" spans="2:5" ht="90">
       <c r="B151" s="2"/>
       <c r="C151" s="2"/>
-      <c r="D151" s="28" t="s">
-        <v>146</v>
+      <c r="D151" s="2" t="s">
+        <v>144</v>
       </c>
       <c r="E151" s="21" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="152" spans="2:5" ht="105">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="152" spans="2:5" ht="90">
       <c r="B152" s="2"/>
       <c r="C152" s="2"/>
-      <c r="D152" s="2" t="s">
-        <v>155</v>
+      <c r="D152" s="28" t="s">
+        <v>146</v>
       </c>
       <c r="E152" s="21" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="153" spans="2:5" ht="90">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="153" spans="2:5" ht="105">
       <c r="B153" s="2"/>
       <c r="C153" s="2"/>
       <c r="D153" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E153" s="21" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="154" spans="2:5">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="154" spans="2:5" ht="90">
       <c r="B154" s="2"/>
       <c r="C154" s="2"/>
-      <c r="D154" s="2"/>
-      <c r="E154" s="21"/>
+      <c r="D154" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E154" s="21" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="155" spans="2:5">
       <c r="B155" s="2"/>
@@ -11128,7 +11149,13 @@
       <c r="E161" s="21"/>
     </row>
     <row r="162" spans="2:5">
-      <c r="E162" s="27"/>
+      <c r="B162" s="2"/>
+      <c r="C162" s="2"/>
+      <c r="D162" s="2"/>
+      <c r="E162" s="21"/>
+    </row>
+    <row r="163" spans="2:5">
+      <c r="E163" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -11145,7 +11172,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B3:C13"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
@@ -11241,7 +11268,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A3:C102"/>
   <sheetViews>
     <sheetView topLeftCell="A79" workbookViewId="0">
@@ -11526,27 +11553,27 @@
       </c>
     </row>
     <row r="49" spans="1:3">
-      <c r="A49" s="82" t="s">
+      <c r="A49" s="84" t="s">
         <v>338</v>
       </c>
       <c r="B49" s="53" t="s">
         <v>339</v>
       </c>
-      <c r="C49" s="82" t="s">
+      <c r="C49" s="84" t="s">
         <v>341</v>
       </c>
     </row>
     <row r="50" spans="1:3">
-      <c r="A50" s="82"/>
+      <c r="A50" s="84"/>
       <c r="B50" s="53"/>
-      <c r="C50" s="82"/>
+      <c r="C50" s="84"/>
     </row>
     <row r="51" spans="1:3">
-      <c r="A51" s="82"/>
+      <c r="A51" s="84"/>
       <c r="B51" s="53" t="s">
         <v>340</v>
       </c>
-      <c r="C51" s="82"/>
+      <c r="C51" s="84"/>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="53" t="s">
@@ -11576,22 +11603,22 @@
       <c r="B56" s="58"/>
     </row>
     <row r="57" spans="1:3" ht="32.25" customHeight="1">
-      <c r="B57" s="86" t="s">
+      <c r="B57" s="88" t="s">
         <v>347</v>
       </c>
-      <c r="C57" s="86"/>
+      <c r="C57" s="88"/>
     </row>
     <row r="58" spans="1:3" ht="33" customHeight="1">
-      <c r="B58" s="86" t="s">
+      <c r="B58" s="88" t="s">
         <v>348</v>
       </c>
-      <c r="C58" s="86"/>
+      <c r="C58" s="88"/>
     </row>
     <row r="59" spans="1:3" ht="19.5" customHeight="1">
-      <c r="B59" s="86" t="s">
+      <c r="B59" s="88" t="s">
         <v>349</v>
       </c>
-      <c r="C59" s="86"/>
+      <c r="C59" s="88"/>
     </row>
     <row r="60" spans="1:3">
       <c r="B60" s="2" t="s">
@@ -11635,7 +11662,7 @@
       </c>
       <c r="C66" s="37"/>
     </row>
-    <row r="67" spans="2:3" ht="30">
+    <row r="67" spans="2:3" ht="30.75">
       <c r="B67" s="63" t="s">
         <v>356</v>
       </c>
@@ -11651,7 +11678,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="69" spans="2:3" ht="105">
+    <row r="69" spans="2:3" ht="105.75">
       <c r="B69" s="63" t="s">
         <v>359</v>
       </c>
@@ -11683,7 +11710,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="73" spans="2:3" ht="30">
+    <row r="73" spans="2:3" ht="30.75">
       <c r="B73" s="63" t="s">
         <v>368</v>
       </c>
@@ -11723,7 +11750,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="78" spans="2:3" ht="30">
+    <row r="78" spans="2:3" ht="30.75">
       <c r="B78" s="67" t="s">
         <v>378</v>
       </c>
@@ -11804,10 +11831,10 @@
       <c r="C87" s="76"/>
     </row>
     <row r="88" spans="1:3" ht="51" customHeight="1">
-      <c r="B88" s="86" t="s">
+      <c r="B88" s="88" t="s">
         <v>400</v>
       </c>
-      <c r="C88" s="86"/>
+      <c r="C88" s="88"/>
     </row>
     <row r="89" spans="1:3" ht="31.5">
       <c r="B89" s="22" t="s">
@@ -11818,13 +11845,13 @@
       <c r="A90" t="s">
         <v>402</v>
       </c>
-      <c r="B90" s="86" t="s">
+      <c r="B90" s="88" t="s">
         <v>401</v>
       </c>
-      <c r="C90" s="86"/>
+      <c r="C90" s="88"/>
     </row>
     <row r="91" spans="1:3" ht="45.75" customHeight="1">
-      <c r="A91" s="87" t="s">
+      <c r="A91" s="89" t="s">
         <v>405</v>
       </c>
       <c r="B91" s="2" t="s">
@@ -11835,7 +11862,7 @@
       </c>
     </row>
     <row r="92" spans="1:3" ht="30">
-      <c r="A92" s="87"/>
+      <c r="A92" s="89"/>
       <c r="B92" s="2" t="s">
         <v>408</v>
       </c>
@@ -11933,7 +11960,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:C49"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
@@ -12136,16 +12163,16 @@
       <c r="C25" s="37"/>
     </row>
     <row r="26" spans="2:3" ht="33" customHeight="1">
-      <c r="B26" s="88" t="s">
+      <c r="B26" s="90" t="s">
         <v>294</v>
       </c>
-      <c r="C26" s="88"/>
+      <c r="C26" s="90"/>
     </row>
     <row r="27" spans="2:3">
-      <c r="B27" s="88" t="s">
+      <c r="B27" s="90" t="s">
         <v>295</v>
       </c>
-      <c r="C27" s="88"/>
+      <c r="C27" s="90"/>
     </row>
     <row r="28" spans="2:3" ht="15.75" thickBot="1">
       <c r="B28" s="48" t="s">
@@ -12200,16 +12227,16 @@
       <c r="C36" s="51"/>
     </row>
     <row r="37" spans="2:3" ht="50.25" customHeight="1">
-      <c r="B37" s="88" t="s">
+      <c r="B37" s="90" t="s">
         <v>303</v>
       </c>
-      <c r="C37" s="88"/>
+      <c r="C37" s="90"/>
     </row>
     <row r="38" spans="2:3" ht="32.25" customHeight="1">
-      <c r="B38" s="88" t="s">
+      <c r="B38" s="90" t="s">
         <v>304</v>
       </c>
-      <c r="C38" s="88"/>
+      <c r="C38" s="90"/>
     </row>
     <row r="39" spans="2:3" ht="15.75" thickBot="1">
       <c r="B39" s="52" t="s">
@@ -12259,16 +12286,16 @@
       </c>
     </row>
     <row r="48" spans="2:3" ht="36" customHeight="1">
-      <c r="B48" s="88" t="s">
+      <c r="B48" s="90" t="s">
         <v>314</v>
       </c>
-      <c r="C48" s="88"/>
+      <c r="C48" s="90"/>
     </row>
     <row r="49" spans="2:3" ht="49.5" customHeight="1">
-      <c r="B49" s="88" t="s">
+      <c r="B49" s="90" t="s">
         <v>315</v>
       </c>
-      <c r="C49" s="88"/>
+      <c r="C49" s="90"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
update some fixing bugs
</commit_message>
<xml_diff>
--- a/Training_Plan.xlsx
+++ b/Training_Plan.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="19155" windowHeight="11760" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="19155" windowHeight="11760" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Plan" sheetId="1" r:id="rId1"/>
@@ -12,16 +12,17 @@
     <sheet name="SOAP WS" sheetId="3" r:id="rId3"/>
     <sheet name="RESTful WS" sheetId="4" r:id="rId4"/>
     <sheet name="Spring framework" sheetId="5" r:id="rId5"/>
+    <sheet name="MongoDBJasper" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="jaxrs_intro" localSheetId="3">'RESTful WS'!$B$6</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="455">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="463">
   <si>
     <t>Java core</t>
   </si>
@@ -8190,12 +8191,154 @@
       <t>Immutable variables can be returned safely without extra effort.</t>
     </r>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">To do this first we need to place the jasperPrint object in the http session using the following code.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>request.getSession().setAttribute(ImageServlet.DEFAULT_JASPER_PRINT_SESSION_ATTRIBUTE, jasperPrint);</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+After placing the jasperPrint object in the session, we need to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>set the image handler for images</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> in the report using the code,
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>exporterOutput.setImageHandler(new WebHtmlResourceHandler("image?image={0}"));</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+The images are served by ImageServlet which should be mapped to ‘/image’ in the web.xml. Here is the configuration that should be added to web.xml file.
+ &lt;servlet&gt;
+    &lt;servlet-name&gt;ImageServlet&lt;/servlet-name&gt;
+    &lt;servlet-class&gt;net.sf.jasperreports.j2ee.servlets.ImageServlet&lt;/servlet-class&gt; &lt;/servlet&gt;
+ &lt;servlet-mapping&gt;
+     &lt;servlet-name&gt;ImageServlet&lt;/servlet-name&gt;
+     &lt;url-pattern&gt;/image&lt;/url-pattern&gt;
+ &lt;/servlet-mapping&gt;
+The JasperCompileManager.compileReport(jrxmlSource) method compiles and generates a jasperReport object which is used to generate jasperPrint object using the JasperFillManager.fillReport(jasperReport, parameters, dataSource) method. In the following example the dataSource is populated using a string which is in json format. I am exporting the generated documents to the response. So, accordingly I have set content-type, content-disposition headers appropriately, which I have not shown in the code. The headers are set for all formats except for the type html as htmls are to be displayed in the browser along with images.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">        private static final Logger logger = LoggerFactory.getLogger(YOURCLASS.class);
+ JRDataSource dataSource = getDataSource(jsonData);//pass jsonData to populate the dataSource
+ JasperReport jasperReport = null;
+ JasperPrint jasperPrint = null;
+ //String type = Any of the types mentioned above
+ //jrxmlSource is the the jrxml generated using the iReport
+ Map&lt;String, Object&gt; parameters = new HashMap&lt;String, Object&gt;();
+ //Add any parameters that are referenced in the jrxml to this map
+ try {
+  jasperReport = JasperCompileManager.compileReport(jRXMLSource);
+  jasperPrint = JasperFillManager.fillReport(jasperReport, parameters, dataSource);
+ } catch (JRException ex) {
+  ex.printStackTrace();
+ }
+</t>
+  </si>
+  <si>
+    <t>request.getSession().setAttribute(ImageServlet.DEFAULT_JASPER_PRINT_SESSION_ATTRIBUTE,jasperPrint);
+  HtmlExporter exporterHTML = new HtmlExporter();
+  SimpleExporterInput exporterInput = new SimpleExporterInput(jasperPrint);
+  exporterHTML.setExporterInput(exporterInput);
+  SimpleHtmlExporterOutput exporterOutput;
+  try {
+   exporterOutput = new SimpleHtmlExporterOutput(response.getOutputStream());
+   exporterOutput.setImageHandler(new WebHtmlResourceHandler("image?image={0}"));
+   exporterHTML.setExporterOutput(exporterOutput);
+          SimpleHtmlReportConfiguration reportExportConfiguration = new SimpleHtmlReportConfiguration();
+   reportExportConfiguration.setWhitePageBackground(false);
+   reportExportConfiguration.setRemoveEmptySpaceBetweenRows(true);
+   exporterHTML.setConfiguration(reportExportConfiguration);
+   exporterHTML.exportReport();
+  } catch (IOException e) {
+   logger.error("IOException occured", e);
+   e.printStackTrace();
+  } catch (JRException e) {
+   logger.error("JRException while exporting for html format", e);
+   e.printStackTrace();}
+ }</t>
+  </si>
+  <si>
+    <t>Problems</t>
+  </si>
+  <si>
+    <t>Resolves</t>
+  </si>
+  <si>
+    <t>Exporting the jasperPrint object which consists of images into html format</t>
+  </si>
+  <si>
+    <t>[#5794] - "No MongoDB connection" when trying to use mongodb connection with subreports/subdatasets on Jasper Server</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   conn = new MongoDbConnection(mongoURI, null, null);
+   Map&lt;String, Object&gt; parameters = new HashMap&lt;String, Object&gt;();
+   //parameters.put(MongoDbDataSource.CONNECTION, conn);
+   JasperReport jasperReport = JasperCompileManager.compileReport("D:\\TrainingCodes\\reportsTemplate\\Table_Report.jrxml");
+   JasperPrint fillReport = JasperFillManager.fillReport(jasperReport, parameters, conn);
+   //JasperExportManager.exportReportToHtmlFile("D:\\TrainingCodes\\reportsTemplate\\MongoDbReport.html");
+   JasperExportManager.exportReportToPdfFile(fillReport,"D:\\TrainingCodes\\reportsTemplate\\Table_Report.pdf");
+   </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="32">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="33">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -8424,6 +8567,12 @@
       <color rgb="FF222222"/>
       <name val="Inherit"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Courier"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -8451,7 +8600,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -8600,11 +8749,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -8792,6 +8952,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -8821,6 +8987,18 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -9056,7 +9234,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -9091,7 +9268,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -9267,7 +9443,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:J30"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
@@ -9733,10 +9909,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:E163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A114" workbookViewId="0">
+    <sheetView topLeftCell="A114" workbookViewId="0">
       <selection activeCell="D117" sqref="D117"/>
     </sheetView>
   </sheetViews>
@@ -9988,10 +10164,10 @@
     <row r="27" spans="2:5">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
-      <c r="D27" s="81" t="s">
+      <c r="D27" s="83" t="s">
         <v>47</v>
       </c>
-      <c r="E27" s="82"/>
+      <c r="E27" s="84"/>
     </row>
     <row r="28" spans="2:5">
       <c r="B28" s="2"/>
@@ -10054,10 +10230,10 @@
     <row r="34" spans="2:5">
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
-      <c r="D34" s="85" t="s">
+      <c r="D34" s="87" t="s">
         <v>78</v>
       </c>
-      <c r="E34" s="85"/>
+      <c r="E34" s="87"/>
     </row>
     <row r="35" spans="2:5">
       <c r="B35" s="2"/>
@@ -10120,10 +10296,10 @@
     <row r="41" spans="2:5">
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
-      <c r="D41" s="86" t="s">
+      <c r="D41" s="88" t="s">
         <v>86</v>
       </c>
-      <c r="E41" s="87"/>
+      <c r="E41" s="89"/>
     </row>
     <row r="42" spans="2:5">
       <c r="B42" s="2"/>
@@ -10210,10 +10386,10 @@
     <row r="50" spans="2:5">
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
-      <c r="D50" s="83" t="s">
+      <c r="D50" s="85" t="s">
         <v>60</v>
       </c>
-      <c r="E50" s="83"/>
+      <c r="E50" s="85"/>
     </row>
     <row r="51" spans="2:5">
       <c r="B51" s="2"/>
@@ -10261,7 +10437,7 @@
       <c r="D55" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="E55" s="84" t="s">
+      <c r="E55" s="86" t="s">
         <v>71</v>
       </c>
     </row>
@@ -10271,7 +10447,7 @@
       <c r="D56" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="E56" s="84"/>
+      <c r="E56" s="86"/>
     </row>
     <row r="57" spans="2:5">
       <c r="B57" s="2"/>
@@ -11174,7 +11350,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B3:C13"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
@@ -11270,7 +11446,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A3:C102"/>
   <sheetViews>
     <sheetView topLeftCell="A89" workbookViewId="0">
@@ -11555,27 +11731,27 @@
       </c>
     </row>
     <row r="49" spans="1:3">
-      <c r="A49" s="84" t="s">
+      <c r="A49" s="86" t="s">
         <v>338</v>
       </c>
       <c r="B49" s="53" t="s">
         <v>339</v>
       </c>
-      <c r="C49" s="84" t="s">
+      <c r="C49" s="86" t="s">
         <v>341</v>
       </c>
     </row>
     <row r="50" spans="1:3">
-      <c r="A50" s="84"/>
+      <c r="A50" s="86"/>
       <c r="B50" s="53"/>
-      <c r="C50" s="84"/>
+      <c r="C50" s="86"/>
     </row>
     <row r="51" spans="1:3">
-      <c r="A51" s="84"/>
+      <c r="A51" s="86"/>
       <c r="B51" s="53" t="s">
         <v>340</v>
       </c>
-      <c r="C51" s="84"/>
+      <c r="C51" s="86"/>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="53" t="s">
@@ -11605,22 +11781,22 @@
       <c r="B56" s="58"/>
     </row>
     <row r="57" spans="1:3" ht="32.25" customHeight="1">
-      <c r="B57" s="88" t="s">
+      <c r="B57" s="90" t="s">
         <v>347</v>
       </c>
-      <c r="C57" s="88"/>
+      <c r="C57" s="90"/>
     </row>
     <row r="58" spans="1:3" ht="33" customHeight="1">
-      <c r="B58" s="88" t="s">
+      <c r="B58" s="90" t="s">
         <v>348</v>
       </c>
-      <c r="C58" s="88"/>
+      <c r="C58" s="90"/>
     </row>
     <row r="59" spans="1:3" ht="19.5" customHeight="1">
-      <c r="B59" s="88" t="s">
+      <c r="B59" s="90" t="s">
         <v>349</v>
       </c>
-      <c r="C59" s="88"/>
+      <c r="C59" s="90"/>
     </row>
     <row r="60" spans="1:3">
       <c r="B60" s="2" t="s">
@@ -11664,7 +11840,7 @@
       </c>
       <c r="C66" s="37"/>
     </row>
-    <row r="67" spans="2:3" ht="30">
+    <row r="67" spans="2:3" ht="30.75">
       <c r="B67" s="63" t="s">
         <v>356</v>
       </c>
@@ -11680,7 +11856,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="69" spans="2:3" ht="105">
+    <row r="69" spans="2:3" ht="105.75">
       <c r="B69" s="63" t="s">
         <v>359</v>
       </c>
@@ -11712,7 +11888,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="73" spans="2:3" ht="30">
+    <row r="73" spans="2:3" ht="30.75">
       <c r="B73" s="63" t="s">
         <v>368</v>
       </c>
@@ -11752,7 +11928,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="78" spans="2:3" ht="30">
+    <row r="78" spans="2:3" ht="30.75">
       <c r="B78" s="67" t="s">
         <v>378</v>
       </c>
@@ -11833,10 +12009,10 @@
       <c r="C87" s="76"/>
     </row>
     <row r="88" spans="1:3" ht="51" customHeight="1">
-      <c r="B88" s="88" t="s">
+      <c r="B88" s="90" t="s">
         <v>400</v>
       </c>
-      <c r="C88" s="88"/>
+      <c r="C88" s="90"/>
     </row>
     <row r="89" spans="1:3" ht="31.5">
       <c r="B89" s="22" t="s">
@@ -11847,13 +12023,13 @@
       <c r="A90" t="s">
         <v>402</v>
       </c>
-      <c r="B90" s="88" t="s">
+      <c r="B90" s="90" t="s">
         <v>401</v>
       </c>
-      <c r="C90" s="88"/>
+      <c r="C90" s="90"/>
     </row>
     <row r="91" spans="1:3" ht="45.75" customHeight="1">
-      <c r="A91" s="89" t="s">
+      <c r="A91" s="91" t="s">
         <v>405</v>
       </c>
       <c r="B91" s="2" t="s">
@@ -11864,7 +12040,7 @@
       </c>
     </row>
     <row r="92" spans="1:3" ht="30">
-      <c r="A92" s="89"/>
+      <c r="A92" s="91"/>
       <c r="B92" s="2" t="s">
         <v>408</v>
       </c>
@@ -11962,7 +12138,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:C49"/>
   <sheetViews>
     <sheetView topLeftCell="A34" workbookViewId="0">
@@ -12165,16 +12341,16 @@
       <c r="C25" s="37"/>
     </row>
     <row r="26" spans="2:3" ht="33" customHeight="1">
-      <c r="B26" s="90" t="s">
+      <c r="B26" s="92" t="s">
         <v>294</v>
       </c>
-      <c r="C26" s="90"/>
+      <c r="C26" s="92"/>
     </row>
     <row r="27" spans="2:3">
-      <c r="B27" s="90" t="s">
+      <c r="B27" s="92" t="s">
         <v>295</v>
       </c>
-      <c r="C27" s="90"/>
+      <c r="C27" s="92"/>
     </row>
     <row r="28" spans="2:3" ht="15.75" thickBot="1">
       <c r="B28" s="48" t="s">
@@ -12229,16 +12405,16 @@
       <c r="C36" s="51"/>
     </row>
     <row r="37" spans="2:3" ht="50.25" customHeight="1">
-      <c r="B37" s="90" t="s">
+      <c r="B37" s="92" t="s">
         <v>303</v>
       </c>
-      <c r="C37" s="90"/>
+      <c r="C37" s="92"/>
     </row>
     <row r="38" spans="2:3" ht="32.25" customHeight="1">
-      <c r="B38" s="90" t="s">
+      <c r="B38" s="92" t="s">
         <v>304</v>
       </c>
-      <c r="C38" s="90"/>
+      <c r="C38" s="92"/>
     </row>
     <row r="39" spans="2:3" ht="15.75" thickBot="1">
       <c r="B39" s="52" t="s">
@@ -12288,16 +12464,16 @@
       </c>
     </row>
     <row r="48" spans="2:3" ht="36" customHeight="1">
-      <c r="B48" s="90" t="s">
+      <c r="B48" s="92" t="s">
         <v>314</v>
       </c>
-      <c r="C48" s="90"/>
+      <c r="C48" s="92"/>
     </row>
     <row r="49" spans="2:3" ht="49.5" customHeight="1">
-      <c r="B49" s="90" t="s">
+      <c r="B49" s="92" t="s">
         <v>315</v>
       </c>
-      <c r="C49" s="90"/>
+      <c r="C49" s="92"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -12311,4 +12487,93 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B2:C14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="3.42578125" customWidth="1"/>
+    <col min="2" max="2" width="64.140625" customWidth="1"/>
+    <col min="3" max="3" width="138.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3">
+      <c r="B2" s="19" t="s">
+        <v>458</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" ht="285">
+      <c r="B3" s="94" t="s">
+        <v>460</v>
+      </c>
+      <c r="C3" s="81" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" ht="255">
+      <c r="B4" s="95"/>
+      <c r="C4" s="81" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" ht="360">
+      <c r="B5" s="96"/>
+      <c r="C5" s="81" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" ht="168">
+      <c r="B6" s="82" t="s">
+        <v>461</v>
+      </c>
+      <c r="C6" s="93" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3">
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+    </row>
+    <row r="8" spans="2:3">
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+    </row>
+    <row r="9" spans="2:3">
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+    </row>
+    <row r="10" spans="2:3">
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+    </row>
+    <row r="11" spans="2:3">
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+    </row>
+    <row r="12" spans="2:3">
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+    </row>
+    <row r="13" spans="2:3">
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14" spans="2:3">
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>